<commit_message>
more performance data for 8 replica scenario
git-svn-id: file://localhost/tmp/svn2git/svn@1798 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-26280" yWindow="-520" windowWidth="35980" windowHeight="22440" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="35980" windowHeight="22440" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NAMD Runtimes" sheetId="1" r:id="rId1"/>
@@ -14,10 +14,10 @@
   </sheets>
   <calcPr calcId="130404" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId5"/>
-    <pivotCache cacheId="2" r:id="rId6"/>
-    <pivotCache cacheId="1" r:id="rId7"/>
-    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="3" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -28,12 +28,127 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="103">
+  <si>
+    <t>Job Size Cloud (in Cores)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Job Size TG (in Cores)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>n/a</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>SAGA Pilot Sub-Job Runtime</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overhead (in s)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overhead (in %)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 cores</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nimbus</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon </t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 cores</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>EUCA (Indiana)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Number Steps: </t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAMD Run</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Nodes</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Cores (Total)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC2 (m1.large)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machine</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nimbus (Chicago)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC2 (c1.xlarge)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC2 (m2.4xlarge)</t>
+  </si>
+  <si>
+    <t>EC2 (m2.4xlarge)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC2 (m2.4xlarge)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Walltime (in sec)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Startup Times</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Startup Time (in s)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
   <si>
     <t>Instance</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
+    <t>m1.large</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Instances</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 cores</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Instance</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
     <t>Date</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -294,121 +409,6 @@
   </si>
   <si>
     <t># EC2</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Job Size Cloud (in Cores)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Job Size TG (in Cores)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>n/a</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>SAGA Pilot Sub-Job Runtime</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overhead (in s)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overhead (in %)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 cores</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nimbus</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Amazon </t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 cores</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>EUCA (Indiana)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Number Steps: </t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>NAMD Run</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Nodes</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Cores (Total)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>EC2 (m1.large)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machine</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nimbus (Chicago)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>EC2 (c1.xlarge)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>EC2 (m2.4xlarge)</t>
-  </si>
-  <si>
-    <t>EC2 (m2.4xlarge)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>EC2 (m2.4xlarge)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Walltime (in sec)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Startup Times</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Startup Time (in s)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Instance</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>m1.large</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Instances</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 cores</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -723,6 +723,109 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.81826388889" refreshedVersion="3" recordCount="18">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A5:D24" sheet="Setup Times"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Instance" numFmtId="0">
+      <sharedItems count="1">
+        <s v="m1.large"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Number Instances" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="8" count="4">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="4"/>
+        <n v="8"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Number Cores" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="16" count="4">
+        <n v="2"/>
+        <n v="4"/>
+        <n v="8"/>
+        <n v="16"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Startup Time (in s)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="184.43929" maxValue="926.75036907200001" count="18">
+        <n v="198.38312601999999"/>
+        <n v="231.39408302300001"/>
+        <n v="184.43929"/>
+        <n v="224.84699320799999"/>
+        <n v="224.94300818400001"/>
+        <n v="264.62740898099997"/>
+        <n v="245.31360506999999"/>
+        <n v="214.989045143"/>
+        <n v="926.75036907200001"/>
+        <n v="526.78812885299999"/>
+        <n v="476.52785396600001"/>
+        <n v="217.40953397800001"/>
+        <n v="341.61289095900003"/>
+        <n v="849.35805797600005"/>
+        <n v="329.82627201100001"/>
+        <n v="527.52867007299994"/>
+        <n v="304.99875497800002"/>
+        <n v="371.16215205200001"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.816388888888" refreshedVersion="3" recordCount="16">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A30:D46" sheet="Setup Times"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Instance" numFmtId="0">
+      <sharedItems count="2">
+        <s v="2 cores"/>
+        <s v="2 core"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Number Instances" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="3">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="4"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Number Cores" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="8" count="3">
+        <n v="2"/>
+        <n v="4"/>
+        <n v="8"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Startup Time (in s)" numFmtId="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="276.08450388900002" maxValue="472.14579200700001" count="16">
+        <n v="313.49457287799999"/>
+        <n v="295.03079795000002"/>
+        <n v="276.08450388900002"/>
+        <n v="314.97212505300001"/>
+        <n v="315.11944603900002"/>
+        <n v="305.19036102299998"/>
+        <n v="365.65275192299998"/>
+        <n v="472.14579200700001"/>
+        <n v="397.81742381999999"/>
+        <n v="376.035724878"/>
+        <n v="372.41291689899998"/>
+        <n v="373.65681600599999"/>
+        <n v="362.95128488500001"/>
+        <n v="376.37267208100002"/>
+        <n v="361.68812417999999"/>
+        <n v="381.790049076"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.819236111114" refreshedVersion="3" recordCount="20">
   <cacheSource type="worksheet">
     <worksheetSource ref="A53:E73" sheet="Setup Times"/>
@@ -800,109 +903,6 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.816388888888" refreshedVersion="3" recordCount="16">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A30:D46" sheet="Setup Times"/>
-  </cacheSource>
-  <cacheFields count="4">
-    <cacheField name="Instance" numFmtId="0">
-      <sharedItems count="2">
-        <s v="2 cores"/>
-        <s v="2 core"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Number Instances" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="3">
-        <n v="1"/>
-        <n v="2"/>
-        <n v="4"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Number Cores" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="8" count="3">
-        <n v="2"/>
-        <n v="4"/>
-        <n v="8"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Startup Time (in s)" numFmtId="3">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="276.08450388900002" maxValue="472.14579200700001" count="16">
-        <n v="313.49457287799999"/>
-        <n v="295.03079795000002"/>
-        <n v="276.08450388900002"/>
-        <n v="314.97212505300001"/>
-        <n v="315.11944603900002"/>
-        <n v="305.19036102299998"/>
-        <n v="365.65275192299998"/>
-        <n v="472.14579200700001"/>
-        <n v="397.81742381999999"/>
-        <n v="376.035724878"/>
-        <n v="372.41291689899998"/>
-        <n v="373.65681600599999"/>
-        <n v="362.95128488500001"/>
-        <n v="376.37267208100002"/>
-        <n v="361.68812417999999"/>
-        <n v="381.790049076"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.81826388889" refreshedVersion="3" recordCount="18">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A5:D24" sheet="Setup Times"/>
-  </cacheSource>
-  <cacheFields count="4">
-    <cacheField name="Instance" numFmtId="0">
-      <sharedItems count="1">
-        <s v="m1.large"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Number Instances" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="8" count="4">
-        <n v="1"/>
-        <n v="2"/>
-        <n v="4"/>
-        <n v="8"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Number Cores" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="16" count="4">
-        <n v="2"/>
-        <n v="4"/>
-        <n v="8"/>
-        <n v="16"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Startup Time (in s)" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="184.43929" maxValue="926.75036907200001" count="18">
-        <n v="198.38312601999999"/>
-        <n v="231.39408302300001"/>
-        <n v="184.43929"/>
-        <n v="224.84699320799999"/>
-        <n v="224.94300818400001"/>
-        <n v="264.62740898099997"/>
-        <n v="245.31360506999999"/>
-        <n v="214.989045143"/>
-        <n v="926.75036907200001"/>
-        <n v="526.78812885299999"/>
-        <n v="476.52785396600001"/>
-        <n v="217.40953397800001"/>
-        <n v="341.61289095900003"/>
-        <n v="849.35805797600005"/>
-        <n v="329.82627201100001"/>
-        <n v="527.52867007299994"/>
-        <n v="304.99875497800002"/>
-        <n v="371.16215205200001"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-</pivotCacheDefinition>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38662.629386574074" refreshedVersion="3" recordCount="39">
   <cacheSource type="worksheet">
@@ -954,146 +954,114 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="20">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="18">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="15"/>
+  </r>
+  <r>
     <x v="0"/>
     <x v="3"/>
     <x v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="4"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="5"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="6"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="7"/>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="8"/>
-    <x v="8"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="9"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="0"/>
     <x v="3"/>
-    <x v="10"/>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="11"/>
-    <x v="11"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="12"/>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="13"/>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="14"/>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="15"/>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="16"/>
-    <x v="16"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
     <x v="3"/>
     <x v="17"/>
-    <x v="17"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="18"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="19"/>
-    <x v="19"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -1200,114 +1168,146 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="18">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="5"/>
-  </r>
-  <r>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="20">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="6"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="8"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="11"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="15"/>
-  </r>
-  <r>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
     <x v="0"/>
     <x v="3"/>
     <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="7"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="8"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="9"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="10"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="11"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="12"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="13"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="14"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="15"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="16"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="3"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
     <x v="3"/>
     <x v="17"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="18"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="19"/>
+    <x v="19"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -1630,36 +1630,34 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="G5:I20" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
-  <pivotFields count="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="G53:I63" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="5">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
     <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
       <items count="5">
+        <item x="1"/>
         <item x="0"/>
-        <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField dataField="1" compact="0" numFmtId="3" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
   </pivotFields>
   <rowFields count="2">
     <field x="2"/>
     <field x="-2"/>
   </rowFields>
-  <rowItems count="15">
+  <rowItems count="10">
     <i>
       <x/>
       <x/>
     </i>
     <i r="1" i="1">
       <x v="1"/>
-    </i>
-    <i r="1" i="2">
-      <x v="2"/>
     </i>
     <i>
       <x v="1"/>
@@ -1668,18 +1666,12 @@
     <i r="1" i="1">
       <x v="1"/>
     </i>
-    <i r="1" i="2">
-      <x v="2"/>
-    </i>
     <i>
       <x v="2"/>
       <x/>
     </i>
     <i r="1" i="1">
       <x v="1"/>
-    </i>
-    <i r="1" i="2">
-      <x v="2"/>
     </i>
     <i>
       <x v="3"/>
@@ -1688,32 +1680,25 @@
     <i r="1" i="1">
       <x v="1"/>
     </i>
-    <i r="1" i="2">
-      <x v="2"/>
-    </i>
     <i t="grand">
       <x/>
     </i>
     <i t="grand" i="1">
       <x/>
     </i>
-    <i t="grand" i="2">
-      <x/>
-    </i>
   </rowItems>
   <colItems count="1">
     <i/>
   </colItems>
-  <dataFields count="3">
+  <dataFields count="2">
     <dataField name="Mittelwert - Startup Time (in s)" fld="3" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="STABW - Startup Time (in s)" fld="3" subtotal="stdDev" baseField="0" baseItem="0"/>
-    <dataField name="Summe - Number Instances" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="G30:J44" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="4">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
@@ -1801,34 +1786,36 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="3" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="G53:I63" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
-  <pivotFields count="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="G5:I20" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="4">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
     <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
       <items count="5">
+        <item x="0"/>
         <item x="1"/>
-        <item x="0"/>
         <item x="2"/>
         <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField dataField="1" compact="0" numFmtId="3" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
   </pivotFields>
   <rowFields count="2">
     <field x="2"/>
     <field x="-2"/>
   </rowFields>
-  <rowItems count="10">
+  <rowItems count="15">
     <i>
       <x/>
       <x/>
     </i>
     <i r="1" i="1">
       <x v="1"/>
+    </i>
+    <i r="1" i="2">
+      <x v="2"/>
     </i>
     <i>
       <x v="1"/>
@@ -1837,12 +1824,18 @@
     <i r="1" i="1">
       <x v="1"/>
     </i>
+    <i r="1" i="2">
+      <x v="2"/>
+    </i>
     <i>
       <x v="2"/>
       <x/>
     </i>
     <i r="1" i="1">
       <x v="1"/>
+    </i>
+    <i r="1" i="2">
+      <x v="2"/>
     </i>
     <i>
       <x v="3"/>
@@ -1851,25 +1844,32 @@
     <i r="1" i="1">
       <x v="1"/>
     </i>
+    <i r="1" i="2">
+      <x v="2"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
     <i t="grand" i="1">
       <x/>
     </i>
+    <i t="grand" i="2">
+      <x/>
+    </i>
   </rowItems>
   <colItems count="1">
     <i/>
   </colItems>
-  <dataFields count="2">
+  <dataFields count="3">
     <dataField name="Mittelwert - Startup Time (in s)" fld="3" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="STABW - Startup Time (in s)" fld="3" subtotal="stdDev" baseField="0" baseItem="0"/>
+    <dataField name="Summe - Number Instances" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:I12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
@@ -2304,12 +2304,12 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -2317,36 +2317,36 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="39">
       <c r="A4" s="3" t="s">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>87</v>
+        <v>13</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>88</v>
+        <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2366,7 +2366,7 @@
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -2406,7 +2406,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2426,7 +2426,7 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -2446,7 +2446,7 @@
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -2466,7 +2466,7 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2486,7 +2486,7 @@
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -2506,7 +2506,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2546,7 +2546,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -2566,7 +2566,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -2586,7 +2586,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2606,7 +2606,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -2626,7 +2626,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -2646,7 +2646,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -2666,7 +2666,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2697,7 +2697,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2728,7 +2728,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2759,7 +2759,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -2782,7 +2782,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -2805,7 +2805,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -2847,7 +2847,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -2868,7 +2868,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -2889,7 +2889,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -2952,7 +2952,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -2973,7 +2973,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B34">
         <v>8</v>
@@ -2994,7 +2994,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B35">
         <v>8</v>
@@ -3015,7 +3015,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -3057,7 +3057,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="44" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="B38" s="44">
         <v>2</v>
@@ -3078,7 +3078,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -3099,7 +3099,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -3120,7 +3120,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -3162,7 +3162,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -3204,7 +3204,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -3225,7 +3225,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -3256,7 +3256,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -3287,7 +3287,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -3308,7 +3308,7 @@
     </row>
     <row r="49" spans="1:8" s="41" customFormat="1">
       <c r="A49" s="41" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B49" s="41">
         <v>2</v>
@@ -3329,7 +3329,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="39" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B50" s="39">
         <v>4</v>
@@ -3350,7 +3350,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -3371,7 +3371,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -3392,7 +3392,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -3413,7 +3413,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -3434,7 +3434,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -3455,7 +3455,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -3476,7 +3476,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -3497,7 +3497,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -3518,7 +3518,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B59">
         <v>15</v>
@@ -3539,7 +3539,7 @@
     </row>
     <row r="60" spans="1:8" hidden="1">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -3560,7 +3560,7 @@
     </row>
     <row r="61" spans="1:8" hidden="1">
       <c r="A61" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -3572,7 +3572,7 @@
     </row>
     <row r="62" spans="1:8" hidden="1">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -3584,7 +3584,7 @@
     </row>
     <row r="63" spans="1:8" hidden="1">
       <c r="A63" t="s">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -3596,7 +3596,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -3617,7 +3617,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -3638,7 +3638,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -3669,7 +3669,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -3700,7 +3700,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -3731,7 +3731,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -3754,7 +3754,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -3777,7 +3777,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -3800,7 +3800,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -3823,7 +3823,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -3846,7 +3846,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -3869,7 +3869,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B75">
         <v>8</v>
@@ -3892,7 +3892,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B76">
         <v>8</v>
@@ -3915,7 +3915,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B77">
         <v>16</v>
@@ -3938,7 +3938,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B78">
         <v>16</v>
@@ -3961,7 +3961,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B79">
         <v>16</v>
@@ -3984,7 +3984,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B80">
         <v>16</v>
@@ -4007,7 +4007,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B81">
         <v>16</v>
@@ -4030,7 +4030,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B82">
         <v>16</v>
@@ -4053,7 +4053,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="B83">
         <v>16</v>
@@ -4076,7 +4076,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -4096,7 +4096,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -4116,7 +4116,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -4136,7 +4136,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -4156,7 +4156,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -4176,7 +4176,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -4196,7 +4196,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -4216,7 +4216,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>95</v>
+        <v>21</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -4236,7 +4236,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>95</v>
+        <v>21</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>21</v>
       </c>
       <c r="B93">
         <v>4</v>
@@ -4276,7 +4276,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>95</v>
+        <v>21</v>
       </c>
       <c r="B94">
         <v>4</v>
@@ -4296,7 +4296,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -4320,7 +4320,6 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4350,45 +4349,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="26" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4403,7 +4402,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="I6" s="17">
         <v>221.43898490266665</v>
@@ -4411,7 +4410,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4427,7 +4426,7 @@
       </c>
       <c r="G7" s="32"/>
       <c r="H7" s="18" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="I7" s="21">
         <v>27.888301147358074</v>
@@ -4435,7 +4434,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -4451,7 +4450,7 @@
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="18" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="I8" s="21">
         <v>6</v>
@@ -4459,7 +4458,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4477,7 +4476,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="I9" s="17">
         <v>230.1513251065</v>
@@ -4485,7 +4484,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -4501,7 +4500,7 @@
       </c>
       <c r="G10" s="32"/>
       <c r="H10" s="18" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="I10" s="21">
         <v>21.442701960879447</v>
@@ -4509,7 +4508,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -4525,7 +4524,7 @@
       </c>
       <c r="G11" s="32"/>
       <c r="H11" s="18" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="I11" s="21">
         <v>4</v>
@@ -4533,7 +4532,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -4551,7 +4550,7 @@
         <v>8</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="I12" s="17">
         <v>524.47522211100011</v>
@@ -4559,7 +4558,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -4575,7 +4574,7 @@
       </c>
       <c r="G13" s="32"/>
       <c r="H13" s="18" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="I13" s="21">
         <v>249.37176975472715</v>
@@ -4583,7 +4582,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -4599,7 +4598,7 @@
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="18" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="I14" s="21">
         <v>32</v>
@@ -4607,7 +4606,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>26</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -4625,7 +4624,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="I15" s="17">
         <v>338.08045351500004</v>
@@ -4633,7 +4632,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -4649,7 +4648,7 @@
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="18" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="I16" s="21">
         <v>46.784586737362908</v>
@@ -4657,7 +4656,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -4673,7 +4672,7 @@
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="18" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="I17" s="21">
         <v>16</v>
@@ -4681,7 +4680,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -4696,7 +4695,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="H18" s="33"/>
       <c r="I18" s="17">
@@ -4705,7 +4704,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -4720,7 +4719,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="H19" s="33"/>
       <c r="I19" s="17">
@@ -4729,7 +4728,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -4744,7 +4743,7 @@
         <v>0.75</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="H20" s="34"/>
       <c r="I20" s="25">
@@ -4753,7 +4752,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -4770,7 +4769,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -4787,7 +4786,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -4804,7 +4803,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -4821,7 +4820,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="B25">
         <v>16</v>
@@ -4838,7 +4837,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="C26" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="D26" s="2">
         <f>AVERAGE(D6:D25)</f>
@@ -4848,7 +4847,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="C27" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="D27" s="2">
         <f>STDEV(D6:D21)</f>
@@ -4858,42 +4857,42 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="26" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="B29" s="26"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>101</v>
+        <v>27</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -4911,7 +4910,7 @@
         <v>2</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="J31" s="17">
         <v>302.94028916180002</v>
@@ -4919,7 +4918,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -4936,7 +4935,7 @@
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
       <c r="I32" s="18" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="J32" s="21">
         <v>17.23574117758357</v>
@@ -4944,7 +4943,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -4959,7 +4958,7 @@
         <v>0.5625</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="H33" s="33"/>
       <c r="I33" s="33"/>
@@ -4969,7 +4968,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -4984,7 +4983,7 @@
         <v>0.89513888888888893</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -4994,7 +4993,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5015,7 +5014,7 @@
         <v>4</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="J35" s="17">
         <v>305.19036102299998</v>
@@ -5023,7 +5022,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -5041,7 +5040,7 @@
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
       <c r="I36" s="18" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="J36" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5049,7 +5048,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -5065,7 +5064,7 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="H37" s="33"/>
       <c r="I37" s="33"/>
@@ -5075,7 +5074,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -5091,7 +5090,7 @@
         <v>0.57916666666666672</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="H38" s="33"/>
       <c r="I38" s="33"/>
@@ -5101,7 +5100,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -5123,7 +5122,7 @@
         <v>8</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="J39" s="17">
         <v>384.05235557549997</v>
@@ -5131,7 +5130,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -5149,7 +5148,7 @@
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
       <c r="I40" s="18" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="J40" s="21">
         <v>32.66972061151673</v>
@@ -5157,7 +5156,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -5173,7 +5172,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="33"/>
@@ -5183,7 +5182,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -5198,7 +5197,7 @@
         <v>0.70972222222222225</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="H42" s="33"/>
       <c r="I42" s="33"/>
@@ -5208,7 +5207,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -5223,7 +5222,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
@@ -5233,7 +5232,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -5248,7 +5247,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -5258,7 +5257,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -5275,7 +5274,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -5292,7 +5291,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -5307,7 +5306,7 @@
     </row>
     <row r="48" spans="1:10">
       <c r="C48" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="D48" s="2">
         <f>AVERAGE(D30:D47)</f>
@@ -5317,7 +5316,7 @@
     </row>
     <row r="49" spans="1:9">
       <c r="C49" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="D49" s="2">
         <f>STDEV(D31:D47)</f>
@@ -5335,39 +5334,39 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="26" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B52" s="26"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="26" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -5385,7 +5384,7 @@
         <v>4</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="I54" s="17">
         <v>14.1872649193</v>
@@ -5393,7 +5392,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -5409,7 +5408,7 @@
       </c>
       <c r="G55" s="32"/>
       <c r="H55" s="18" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="I55" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5417,7 +5416,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -5435,7 +5434,7 @@
         <v>8</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="I56" s="17">
         <v>44.782275199920001</v>
@@ -5443,7 +5442,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -5459,7 +5458,7 @@
       </c>
       <c r="G57" s="32"/>
       <c r="H57" s="18" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="I57" s="21">
         <v>15.843792242505828</v>
@@ -5467,7 +5466,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -5485,7 +5484,7 @@
         <v>16</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="I58" s="17">
         <v>56.964924156674996</v>
@@ -5493,7 +5492,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -5509,7 +5508,7 @@
       </c>
       <c r="G59" s="32"/>
       <c r="H59" s="18" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="I59" s="21">
         <v>9.4994883808250847</v>
@@ -5517,7 +5516,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -5535,7 +5534,7 @@
         <v>32</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="I60" s="17">
         <v>187.55037531850999</v>
@@ -5543,7 +5542,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -5559,7 +5558,7 @@
       </c>
       <c r="G61" s="32"/>
       <c r="H61" s="18" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="I61" s="21">
         <v>179.97433590633514</v>
@@ -5567,7 +5566,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -5582,7 +5581,7 @@
         <v>0.59236111111111112</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="H62" s="33"/>
       <c r="I62" s="17">
@@ -5591,7 +5590,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -5606,7 +5605,7 @@
         <v>0.61875000000000002</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="H63" s="34"/>
       <c r="I63" s="25">
@@ -5615,7 +5614,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B64">
         <v>8</v>
@@ -5632,7 +5631,7 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -5649,7 +5648,7 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -5666,7 +5665,7 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B67">
         <v>8</v>
@@ -5683,7 +5682,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B68">
         <v>8</v>
@@ -5700,7 +5699,7 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -5717,7 +5716,7 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B70">
         <v>8</v>
@@ -5734,7 +5733,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -5751,7 +5750,7 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -5768,7 +5767,7 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -5783,7 +5782,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B74">
         <v>2</v>
@@ -5798,7 +5797,7 @@
     </row>
     <row r="75" spans="1:5">
       <c r="C75" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="D75" s="2">
         <f>AVERAGE(D54:D73)</f>
@@ -5807,7 +5806,7 @@
     </row>
     <row r="76" spans="1:5">
       <c r="C76" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="D76" s="2">
         <f>STDEV(D54:D73)</f>
@@ -5818,10 +5817,8 @@
       <c r="H88" s="2"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5836,7 +5833,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="A19" sqref="A19:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -5852,69 +5849,69 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="28" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="30" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="28" customFormat="1" ht="39" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="K5" s="28" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="M5" s="28" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -5949,13 +5946,13 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -5990,13 +5987,13 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="B8" s="31">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -6031,7 +6028,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -6069,7 +6066,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -6104,7 +6101,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B11">
         <v>32</v>
@@ -6145,7 +6142,7 @@
     </row>
     <row r="12" spans="1:13" s="49" customFormat="1" ht="14" thickBot="1">
       <c r="A12" s="49" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B12" s="49">
         <v>32</v>
@@ -6186,7 +6183,7 @@
     </row>
     <row r="13" spans="1:13" ht="14" thickTop="1">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -6219,7 +6216,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -6252,7 +6249,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="B15" s="41">
         <v>16</v>
@@ -6285,7 +6282,7 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -6318,7 +6315,7 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B17">
         <v>32</v>
@@ -6339,10 +6336,19 @@
       <c r="I17">
         <v>8</v>
       </c>
+      <c r="J17" s="35">
+        <v>336.34934997599998</v>
+      </c>
+      <c r="K17">
+        <v>8</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B18">
         <v>32</v>
@@ -6363,6 +6369,48 @@
       <c r="I18">
         <v>8</v>
       </c>
+      <c r="J18" s="35">
+        <v>2566.0503461399999</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19">
+        <v>32</v>
+      </c>
+      <c r="E19" s="48">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ref="F19" si="1">E19*2</f>
+        <v>16</v>
+      </c>
+      <c r="G19" s="48">
+        <v>8</v>
+      </c>
+      <c r="H19">
+        <v>8</v>
+      </c>
+      <c r="I19">
+        <v>8</v>
+      </c>
+      <c r="J19" s="35">
+        <v>2559.66540098</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="1:13">
       <c r="M20" s="47"/>
@@ -6371,7 +6419,6 @@
       <c r="I21" s="47"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6413,10 +6460,10 @@
   <sheetData>
     <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -6428,7 +6475,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="11" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
@@ -6452,12 +6499,12 @@
         <v>32</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
@@ -6474,7 +6521,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="18" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="20">
@@ -6491,7 +6538,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="18" t="s">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
@@ -6512,7 +6559,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="18" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B8" s="19">
         <v>2070.8984270000001</v>
@@ -6529,7 +6576,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B9" s="19">
         <v>1095.4940549999999</v>
@@ -6556,7 +6603,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="18" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
@@ -6577,7 +6624,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="18" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -6598,7 +6645,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="22" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="B12" s="23">
         <v>1583.1962410000001</v>

</xml_diff>

<commit_message>
some more performance data and descriptions
git-svn-id: file://localhost/tmp/svn2git/svn@1803 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="35980" windowHeight="22440" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="35980" windowHeight="22440" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NAMD Runtimes" sheetId="1" r:id="rId1"/>
     <sheet name="Setup Times" sheetId="3" r:id="rId2"/>
     <sheet name="Adaptive" sheetId="7" r:id="rId3"/>
-    <sheet name="Pivot" sheetId="4" r:id="rId4"/>
+    <sheet name="Deadline" sheetId="8" r:id="rId4"/>
+    <sheet name="Pivot" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="130404" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId5"/>
-    <pivotCache cacheId="1" r:id="rId6"/>
-    <pivotCache cacheId="0" r:id="rId7"/>
-    <pivotCache cacheId="3" r:id="rId8"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="3" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -28,147 +29,239 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="125">
+  <si>
+    <t>Average</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC2 m1.large</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nimbus</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI 16 core
+Nimbus 16 core</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Run ID</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Replicas</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAX_RUNTIME (in min)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Check Period (in min)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max Cloud Pilots</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cloud Pilot Size</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Runtime (in min)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Runtime (in sec)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t># Nimbus</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t># Poseidon</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t># Cloud Pilots</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start Pilot if not sufficient progress is made</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deadline Scenario</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
   <si>
     <t>Job Size Cloud (in Cores)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Job Size TG (in Cores)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>n/a</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>SAGA Pilot Sub-Job Runtime</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Overhead (in s)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Overhead (in %)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>2 cores</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Nimbus</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Amazon </t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>2 cores</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>EUCA (Indiana)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Number Steps: </t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>NAMD Run</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Number Nodes</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Number Cores (Total)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>EC2 (m1.large)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Machine</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Nimbus (Chicago)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>EC2 (c1.xlarge)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>EC2 (m2.4xlarge)</t>
   </si>
   <si>
     <t>EC2 (m2.4xlarge)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>EC2 (m2.4xlarge)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Walltime (in sec)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Startup Times</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Startup Time (in s)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Instance</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>m1.large</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Number Instances</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>2 cores</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI 8 core
+Nimbus 8 core</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI 8 core 
+Nimbus 16 core</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI 16 core
+Nimbus 8 core</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Startup Time (in s)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Instance</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Date</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>m1.large</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>QB (MPI)</t>
   </si>
   <si>
     <t>QB (MPI)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>QB (CHARM)</t>
   </si>
   <si>
     <t>QB (CHARM)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Mittelwert - Walltime (in sec)</t>
@@ -196,103 +289,103 @@
   </si>
   <si>
     <t>CPU Time (in sec)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>LONI</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Date</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Resource</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Cores</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Poseidon </t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>TG</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Nimbus Number Cores</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Number Cores</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>EC2</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>EC2 Number Cores</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Number Jobs</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>n/a</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Average</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Stddev</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Time-to-Completion (in s)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>m1.large</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>2 cores</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Average</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Startup Time (in s)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Memory (in MB)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Number Instances</t>
@@ -323,34 +416,34 @@
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon (CHARM)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>2 core</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Number Cores</t>
   </si>
   <si>
     <t>Number Cores</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Nodes</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Number Cores</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>m1.large</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>1 STABW - Startup Time (in s)</t>
@@ -381,35 +474,35 @@
   </si>
   <si>
     <t>m1.large</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Adaptive Scenario</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Time for completion for n jobs</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>Jobs run as soon as a resource becomes available</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t># TG</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t># Nimbus</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t># EC2</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -420,8 +513,13 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -648,23 +746,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -683,20 +781,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -713,6 +811,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -720,6 +825,399 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="de-DE"/>
+  <c:style val="1"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>('Setup Times'!$D$27,'Setup Times'!$D$49,'Setup Times'!$D$76)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>206.4680035082333</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>48.59380013431259</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>143.9351872602122</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>('Setup Times'!$D$27,'Setup Times'!$D$49,'Setup Times'!$D$76)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>206.4680035082333</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>48.59380013431259</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>143.9351872602122</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>('Setup Times'!$E$26,'Setup Times'!$E$48,'Setup Times'!$E$75)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>EC2 m1.large</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nimbus</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Poseidon</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Setup Times'!$D$26,'Setup Times'!$D$48,'Setup Times'!$D$75)</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>373.44653231865</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>356.831301927</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>117.073104536535</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="543987816"/>
+        <c:axId val="543749608"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="543987816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="543749608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="543749608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400">
+                    <a:latin typeface="+mn-lt"/>
+                    <a:cs typeface="Times"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1400">
+                    <a:latin typeface="+mn-lt"/>
+                    <a:cs typeface="Times"/>
+                  </a:rPr>
+                  <a:t>Waiting Time (in sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400">
+                <a:latin typeface="+mn-lt"/>
+                <a:cs typeface="Times"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="543987816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="de-DE"/>
+  <c:style val="1"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Adaptive!$N$13:$N$16</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>LONI 8 core_x000d_Nimbus 8 core</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LONI 8 core _x000d_Nimbus 16 core</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>LONI 16 core_x000d_Nimbus 8 core</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>LONI 16 core_x000d_Nimbus 16 core</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Adaptive!$J$13:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1051.73987007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1040.68170691</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>671.081423998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>593.293745995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls/>
+        <c:axId val="499577032"/>
+        <c:axId val="561706376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="499577032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="561706376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="561706376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1400"/>
+                  <a:t>Runtime (in sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="499577032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Diagramm 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2304,12 +2802,12 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -2317,36 +2815,36 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="39">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="I4" s="4" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2366,7 +2864,7 @@
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -2386,7 +2884,7 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -2406,7 +2904,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2426,7 +2924,7 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -2446,7 +2944,7 @@
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -2466,7 +2964,7 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2486,7 +2984,7 @@
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -2506,7 +3004,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -2526,7 +3024,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2546,7 +3044,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -2566,7 +3064,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -2586,7 +3084,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2606,7 +3104,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -2626,7 +3124,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -2646,7 +3144,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -2666,7 +3164,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2697,7 +3195,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2728,7 +3226,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -2759,7 +3257,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -2782,7 +3280,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -2805,7 +3303,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -2826,7 +3324,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -2847,7 +3345,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -2868,7 +3366,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -2889,7 +3387,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -2910,7 +3408,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -2931,7 +3429,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -2952,7 +3450,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -2973,7 +3471,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B34">
         <v>8</v>
@@ -2994,7 +3492,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B35">
         <v>8</v>
@@ -3015,7 +3513,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -3036,7 +3534,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -3057,7 +3555,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="44" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B38" s="44">
         <v>2</v>
@@ -3078,7 +3576,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -3099,7 +3597,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -3120,7 +3618,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -3141,7 +3639,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -3162,7 +3660,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -3183,7 +3681,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -3204,7 +3702,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -3225,7 +3723,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -3256,7 +3754,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -3287,7 +3785,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -3308,7 +3806,7 @@
     </row>
     <row r="49" spans="1:8" s="41" customFormat="1">
       <c r="A49" s="41" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B49" s="41">
         <v>2</v>
@@ -3329,7 +3827,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="39" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B50" s="39">
         <v>4</v>
@@ -3350,7 +3848,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -3371,7 +3869,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -3392,7 +3890,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -3413,7 +3911,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -3434,7 +3932,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -3455,7 +3953,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -3476,7 +3974,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -3497,7 +3995,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -3518,7 +4016,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B59">
         <v>15</v>
@@ -3539,7 +4037,7 @@
     </row>
     <row r="60" spans="1:8" hidden="1">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -3560,7 +4058,7 @@
     </row>
     <row r="61" spans="1:8" hidden="1">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -3572,7 +4070,7 @@
     </row>
     <row r="62" spans="1:8" hidden="1">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -3584,7 +4082,7 @@
     </row>
     <row r="63" spans="1:8" hidden="1">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -3596,7 +4094,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -3617,7 +4115,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -3638,7 +4136,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -3669,7 +4167,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -3700,7 +4198,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -3731,7 +4229,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -3754,7 +4252,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -3777,7 +4275,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -3800,7 +4298,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -3823,7 +4321,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -3846,7 +4344,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -3869,7 +4367,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B75">
         <v>8</v>
@@ -3892,7 +4390,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B76">
         <v>8</v>
@@ -3915,7 +4413,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B77">
         <v>16</v>
@@ -3938,7 +4436,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B78">
         <v>16</v>
@@ -3961,7 +4459,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B79">
         <v>16</v>
@@ -3984,7 +4482,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B80">
         <v>16</v>
@@ -4007,7 +4505,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B81">
         <v>16</v>
@@ -4030,7 +4528,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B82">
         <v>16</v>
@@ -4053,7 +4551,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B83">
         <v>16</v>
@@ -4076,7 +4574,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -4096,7 +4594,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -4116,7 +4614,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -4136,7 +4634,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -4156,7 +4654,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -4176,7 +4674,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -4196,7 +4694,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -4216,7 +4714,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -4236,7 +4734,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -4256,7 +4754,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B93">
         <v>4</v>
@@ -4276,7 +4774,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B94">
         <v>4</v>
@@ -4296,7 +4794,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -4318,7 +4816,7 @@
       <c r="A98" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -4333,8 +4831,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4349,45 +4847,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="26" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4402,7 +4900,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="I6" s="17">
         <v>221.43898490266665</v>
@@ -4410,7 +4908,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4426,7 +4924,7 @@
       </c>
       <c r="G7" s="32"/>
       <c r="H7" s="18" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="I7" s="21">
         <v>27.888301147358074</v>
@@ -4434,7 +4932,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -4450,7 +4948,7 @@
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="18" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="I8" s="21">
         <v>6</v>
@@ -4458,7 +4956,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4476,7 +4974,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="I9" s="17">
         <v>230.1513251065</v>
@@ -4484,7 +4982,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -4500,7 +4998,7 @@
       </c>
       <c r="G10" s="32"/>
       <c r="H10" s="18" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="I10" s="21">
         <v>21.442701960879447</v>
@@ -4508,7 +5006,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -4524,7 +5022,7 @@
       </c>
       <c r="G11" s="32"/>
       <c r="H11" s="18" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="I11" s="21">
         <v>4</v>
@@ -4532,7 +5030,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -4550,7 +5048,7 @@
         <v>8</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="I12" s="17">
         <v>524.47522211100011</v>
@@ -4558,7 +5056,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -4574,7 +5072,7 @@
       </c>
       <c r="G13" s="32"/>
       <c r="H13" s="18" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="I13" s="21">
         <v>249.37176975472715</v>
@@ -4582,7 +5080,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -4598,7 +5096,7 @@
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="18" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="I14" s="21">
         <v>32</v>
@@ -4606,7 +5104,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -4624,7 +5122,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="I15" s="17">
         <v>338.08045351500004</v>
@@ -4632,7 +5130,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -4648,7 +5146,7 @@
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="18" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="I16" s="21">
         <v>46.784586737362908</v>
@@ -4656,7 +5154,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -4672,7 +5170,7 @@
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="18" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="I17" s="21">
         <v>16</v>
@@ -4680,7 +5178,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -4695,7 +5193,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="H18" s="33"/>
       <c r="I18" s="17">
@@ -4704,7 +5202,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -4719,7 +5217,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="H19" s="33"/>
       <c r="I19" s="17">
@@ -4728,7 +5226,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -4743,7 +5241,7 @@
         <v>0.75</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="H20" s="34"/>
       <c r="I20" s="25">
@@ -4752,7 +5250,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -4769,7 +5267,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -4786,7 +5284,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -4803,7 +5301,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -4820,7 +5318,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="B25">
         <v>16</v>
@@ -4837,62 +5335,64 @@
     </row>
     <row r="26" spans="1:10">
       <c r="C26" t="s">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="D26" s="2">
         <f>AVERAGE(D6:D25)</f>
         <v>373.44653231864999</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="7" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:10">
       <c r="C27" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="D27" s="2">
-        <f>STDEV(D6:D21)</f>
-        <v>231.20393612739198</v>
+        <f>STDEV(D6:D25)</f>
+        <v>206.46800350823335</v>
       </c>
       <c r="E27" s="7"/>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="26" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B29" s="26"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -4910,7 +5410,7 @@
         <v>2</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="J31" s="17">
         <v>302.94028916180002</v>
@@ -4918,7 +5418,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -4935,7 +5435,7 @@
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
       <c r="I32" s="18" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="J32" s="21">
         <v>17.23574117758357</v>
@@ -4943,7 +5443,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -4958,7 +5458,7 @@
         <v>0.5625</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="H33" s="33"/>
       <c r="I33" s="33"/>
@@ -4968,7 +5468,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -4983,7 +5483,7 @@
         <v>0.89513888888888893</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -4993,7 +5493,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5014,7 +5514,7 @@
         <v>4</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="J35" s="17">
         <v>305.19036102299998</v>
@@ -5022,7 +5522,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -5040,7 +5540,7 @@
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
       <c r="I36" s="18" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="J36" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5048,7 +5548,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -5064,7 +5564,7 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="H37" s="33"/>
       <c r="I37" s="33"/>
@@ -5074,7 +5574,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -5090,7 +5590,7 @@
         <v>0.57916666666666672</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="H38" s="33"/>
       <c r="I38" s="33"/>
@@ -5100,7 +5600,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -5122,7 +5622,7 @@
         <v>8</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="J39" s="17">
         <v>384.05235557549997</v>
@@ -5130,7 +5630,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -5148,7 +5648,7 @@
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
       <c r="I40" s="18" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="J40" s="21">
         <v>32.66972061151673</v>
@@ -5156,7 +5656,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -5172,7 +5672,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="33"/>
@@ -5182,7 +5682,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -5197,7 +5697,7 @@
         <v>0.70972222222222225</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="H42" s="33"/>
       <c r="I42" s="33"/>
@@ -5207,7 +5707,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -5222,7 +5722,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
@@ -5232,7 +5732,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -5247,7 +5747,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -5257,7 +5757,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -5274,7 +5774,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -5291,7 +5791,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -5306,17 +5806,19 @@
     </row>
     <row r="48" spans="1:10">
       <c r="C48" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="D48" s="2">
         <f>AVERAGE(D30:D47)</f>
         <v>356.83130192700003</v>
       </c>
-      <c r="E48" s="7"/>
+      <c r="E48" s="7" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="49" spans="1:9">
       <c r="C49" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="D49" s="2">
         <f>STDEV(D31:D47)</f>
@@ -5325,7 +5827,6 @@
       <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="D50" s="2"/>
       <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:9">
@@ -5334,39 +5835,37 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="26" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B52" s="26"/>
+      <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="26" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -5374,8 +5873,8 @@
       <c r="C54">
         <v>8</v>
       </c>
-      <c r="D54" s="2">
-        <v>24.626098156000001</v>
+      <c r="D54" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="E54" s="7">
         <v>0.89513888888888893</v>
@@ -5384,7 +5883,7 @@
         <v>4</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="I54" s="17">
         <v>14.1872649193</v>
@@ -5392,7 +5891,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -5401,14 +5900,14 @@
         <v>8</v>
       </c>
       <c r="D55" s="2">
-        <v>44.588248014500003</v>
+        <v>24.626098156000001</v>
       </c>
       <c r="E55" s="7">
         <v>0.90208333333333324</v>
       </c>
       <c r="G55" s="32"/>
       <c r="H55" s="18" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="I55" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5416,7 +5915,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -5425,7 +5924,7 @@
         <v>4</v>
       </c>
       <c r="D56" s="2">
-        <v>14.1872649193</v>
+        <v>44.588248014500003</v>
       </c>
       <c r="E56" s="7">
         <v>0.90972222222222221</v>
@@ -5434,7 +5933,7 @@
         <v>8</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="I56" s="17">
         <v>44.782275199920001</v>
@@ -5442,7 +5941,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -5451,14 +5950,14 @@
         <v>8</v>
       </c>
       <c r="D57" s="2">
-        <v>35.098526954699999</v>
+        <v>14.1872649193</v>
       </c>
       <c r="E57" s="7">
         <v>0.93125000000000002</v>
       </c>
       <c r="G57" s="32"/>
       <c r="H57" s="18" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="I57" s="21">
         <v>15.843792242505828</v>
@@ -5466,7 +5965,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -5475,7 +5974,7 @@
         <v>8</v>
       </c>
       <c r="D58" s="2">
-        <v>64.947054863000005</v>
+        <v>35.098526954699999</v>
       </c>
       <c r="E58" s="7">
         <v>0.93888888888888899</v>
@@ -5484,7 +5983,7 @@
         <v>16</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="I58" s="17">
         <v>56.964924156674996</v>
@@ -5492,7 +5991,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -5501,14 +6000,14 @@
         <v>8</v>
       </c>
       <c r="D59" s="2">
-        <v>54.651448011399999</v>
+        <v>64.947054863000005</v>
       </c>
       <c r="E59" s="7">
         <v>0.95000000000000007</v>
       </c>
       <c r="G59" s="32"/>
       <c r="H59" s="18" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="I59" s="21">
         <v>9.4994883808250847</v>
@@ -5516,7 +6015,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -5525,7 +6024,7 @@
         <v>16</v>
       </c>
       <c r="D60" s="2">
-        <v>55.051728963899997</v>
+        <v>54.651448011399999</v>
       </c>
       <c r="E60" s="7">
         <v>0.96527777777777779</v>
@@ -5534,7 +6033,7 @@
         <v>32</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="I60" s="17">
         <v>187.55037531850999</v>
@@ -5542,7 +6041,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -5551,14 +6050,14 @@
         <v>16</v>
       </c>
       <c r="D61" s="2">
-        <v>50.9480149746</v>
+        <v>55.051728963899997</v>
       </c>
       <c r="E61" s="7">
         <v>0.58402777777777781</v>
       </c>
       <c r="G61" s="32"/>
       <c r="H61" s="18" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="I61" s="21">
         <v>179.97433590633514</v>
@@ -5566,7 +6065,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -5575,13 +6074,13 @@
         <v>16</v>
       </c>
       <c r="D62" s="2">
-        <v>70.915316820100003</v>
+        <v>50.9480149746</v>
       </c>
       <c r="E62" s="7">
         <v>0.59236111111111112</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="H62" s="33"/>
       <c r="I62" s="17">
@@ -5590,7 +6089,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -5599,13 +6098,13 @@
         <v>16</v>
       </c>
       <c r="D63" s="2">
-        <v>50.944635868100001</v>
+        <v>70.915316820100003</v>
       </c>
       <c r="E63" s="7">
         <v>0.61875000000000002</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="H63" s="34"/>
       <c r="I63" s="25">
@@ -5614,7 +6113,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B64">
         <v>8</v>
@@ -5623,7 +6122,7 @@
         <v>32</v>
       </c>
       <c r="D64" s="2">
-        <v>266.05073404299998</v>
+        <v>50.944635868100001</v>
       </c>
       <c r="E64" s="7">
         <v>0.625</v>
@@ -5631,7 +6130,7 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -5640,7 +6139,7 @@
         <v>32</v>
       </c>
       <c r="D65" s="2">
-        <v>35.081162929500003</v>
+        <v>266.05073404299998</v>
       </c>
       <c r="E65" s="7">
         <v>0.67013888888888884</v>
@@ -5648,7 +6147,7 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -5657,7 +6156,7 @@
         <v>32</v>
       </c>
       <c r="D66" s="2">
-        <v>24.897548914000001</v>
+        <v>35.081162929500003</v>
       </c>
       <c r="E66" s="7">
         <v>0.71388888888888891</v>
@@ -5665,7 +6164,7 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B67">
         <v>8</v>
@@ -5674,7 +6173,7 @@
         <v>32</v>
       </c>
       <c r="D67" s="2">
-        <v>325.77829599400002</v>
+        <v>24.897548914000001</v>
       </c>
       <c r="E67" s="7">
         <v>0.73749999999999993</v>
@@ -5682,7 +6181,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B68">
         <v>8</v>
@@ -5691,7 +6190,7 @@
         <v>32</v>
       </c>
       <c r="D68" s="2">
-        <v>75.1672639847</v>
+        <v>325.77829599400002</v>
       </c>
       <c r="E68" s="7">
         <v>0.75</v>
@@ -5699,7 +6198,7 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -5708,7 +6207,7 @@
         <v>32</v>
       </c>
       <c r="D69" s="2">
-        <v>65.186727047000005</v>
+        <v>75.1672639847</v>
       </c>
       <c r="E69" s="7">
         <v>0.76388888888888884</v>
@@ -5716,7 +6215,7 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B70">
         <v>8</v>
@@ -5725,7 +6224,7 @@
         <v>32</v>
       </c>
       <c r="D70" s="2">
-        <v>86.636376142499998</v>
+        <v>65.186727047000005</v>
       </c>
       <c r="E70" s="7">
         <v>0.7715277777777777</v>
@@ -5733,7 +6232,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -5742,7 +6241,7 @@
         <v>32</v>
       </c>
       <c r="D71" s="2">
-        <v>576.54629802700003</v>
+        <v>86.636376142499998</v>
       </c>
       <c r="E71" s="7">
         <v>0.78819444444444453</v>
@@ -5750,7 +6249,7 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -5759,7 +6258,7 @@
         <v>32</v>
       </c>
       <c r="D72" s="2">
-        <v>325.02609419800001</v>
+        <v>576.54629802700003</v>
       </c>
       <c r="E72" s="7">
         <v>0.8125</v>
@@ -5767,7 +6266,7 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -5776,13 +6275,13 @@
         <v>32</v>
       </c>
       <c r="D73" s="2">
-        <v>95.133251905400002</v>
+        <v>325.02609419800001</v>
       </c>
       <c r="E73" s="7"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B74">
         <v>2</v>
@@ -5790,26 +6289,29 @@
       <c r="C74">
         <v>4</v>
       </c>
-      <c r="D74" s="35">
-        <v>50.927874088300001</v>
+      <c r="D74" s="2">
+        <v>95.133251905400002</v>
       </c>
       <c r="E74" s="7"/>
     </row>
     <row r="75" spans="1:5">
       <c r="C75" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="D75" s="2">
-        <f>AVERAGE(D54:D73)</f>
+        <f>AVERAGE(D55:D74)</f>
         <v>117.073104536535</v>
+      </c>
+      <c r="E75" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="C76" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="D76" s="2">
-        <f>STDEV(D54:D73)</f>
+        <f>STDEV(D55:D74)</f>
         <v>143.93518726021225</v>
       </c>
     </row>
@@ -5817,8 +6319,10 @@
       <c r="H88" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5830,10 +6334,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:I19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -5847,71 +6351,71 @@
     <col min="10" max="10" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="30" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="28" customFormat="1" ht="39" customHeight="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="28" customFormat="1" ht="39" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="K5" s="28" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="M5" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -5944,15 +6448,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -5985,15 +6489,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="B8" s="31">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -6026,9 +6530,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -6064,9 +6568,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -6099,9 +6603,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B11">
         <v>32</v>
@@ -6140,9 +6644,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="49" customFormat="1" ht="14" thickBot="1">
+    <row r="12" spans="1:14" s="49" customFormat="1" ht="14" thickBot="1">
       <c r="A12" s="49" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B12" s="49">
         <v>32</v>
@@ -6181,9 +6685,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="14" thickTop="1">
+    <row r="13" spans="1:14" ht="40" thickTop="1">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -6213,10 +6717,13 @@
       <c r="L13" s="48">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13" s="52" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="39">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -6246,10 +6753,13 @@
       <c r="L14" s="48">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14" s="52" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="39">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="B15" s="41">
         <v>16</v>
@@ -6279,10 +6789,13 @@
       <c r="L15" s="48">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15" s="52" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="39">
       <c r="A16" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -6312,10 +6825,13 @@
       <c r="L16">
         <v>0</v>
       </c>
+      <c r="N16" s="52" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B17">
         <v>32</v>
@@ -6348,7 +6864,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B18">
         <v>32</v>
@@ -6381,7 +6897,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B19">
         <v>32</v>
@@ -6419,7 +6935,114 @@
       <c r="I21" s="47"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="54" customFormat="1" ht="39">
+      <c r="A5" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="54" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>45</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="35">
+        <v>2836.47443509</v>
+      </c>
+      <c r="H6">
+        <f>G6/60</f>
+        <v>47.274573918166666</v>
+      </c>
+      <c r="I6">
+        <v>8</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -6430,7 +7053,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A3:I12"/>
@@ -6460,10 +7083,10 @@
   <sheetData>
     <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -6475,7 +7098,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="11" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
@@ -6499,12 +7122,12 @@
         <v>32</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
@@ -6521,7 +7144,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="18" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="20">
@@ -6538,7 +7161,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="18" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
@@ -6559,7 +7182,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="18" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B8" s="19">
         <v>2070.8984270000001</v>
@@ -6576,7 +7199,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B9" s="19">
         <v>1095.4940549999999</v>
@@ -6603,7 +7226,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="18" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
@@ -6624,7 +7247,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="18" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -6645,7 +7268,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="22" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B12" s="23">
         <v>1583.1962410000001</v>
@@ -6673,7 +7296,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
data for deadline driven scenario
git-svn-id: file://localhost/tmp/svn2git/svn@1808 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="35980" windowHeight="22440" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="220" yWindow="220" windowWidth="35740" windowHeight="22200" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NAMD Runtimes" sheetId="1" r:id="rId1"/>
@@ -15,10 +15,10 @@
   </sheets>
   <calcPr calcId="130404" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId6"/>
-    <pivotCache cacheId="1" r:id="rId7"/>
-    <pivotCache cacheId="0" r:id="rId8"/>
-    <pivotCache cacheId="3" r:id="rId9"/>
+    <pivotCache cacheId="4" r:id="rId6"/>
+    <pivotCache cacheId="6" r:id="rId7"/>
+    <pivotCache cacheId="5" r:id="rId8"/>
+    <pivotCache cacheId="7" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -31,6 +31,195 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="125">
   <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Poseidon </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>TG</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nimbus Number Cores</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Cores</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC2 Number Cores</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Jobs</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>n/a</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stddev</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time-to-Completion (in s)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>m1.large</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 cores</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Startup Time (in s)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memory (in MB)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Instances</t>
+  </si>
+  <si>
+    <t>Daten</t>
+  </si>
+  <si>
+    <t>Ergebnis</t>
+  </si>
+  <si>
+    <t>Mittelwert - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>STABW - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>Gesamt: Mittelwert - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>Gesamt: STABW - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>Mittelwert - Startup Time (in s)2</t>
+  </si>
+  <si>
+    <t>Gesamt: Mittelwert - Startup Time (in s)2</t>
+  </si>
+  <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon (CHARM)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 core</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Cores</t>
+  </si>
+  <si>
+    <t>Number Cores</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nodes</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Cores</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>m1.large</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 STABW - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>2 STABW - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>4 STABW - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>1 Mittelwert - Startup Time (in s)2</t>
+  </si>
+  <si>
+    <t>2 Mittelwert - Startup Time (in s)2</t>
+  </si>
+  <si>
+    <t>4 Mittelwert - Startup Time (in s)2</t>
+  </si>
+  <si>
+    <t>Summe - Number Instances</t>
+  </si>
+  <si>
+    <t>Gesamt: Summe - Number Instances</t>
+  </si>
+  <si>
+    <t>Cores</t>
+  </si>
+  <si>
+    <t>m1.large</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adaptive Scenario</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time for completion for n jobs</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jobs run as soon as a resource becomes available</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t># TG</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t># Nimbus</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t># EC2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
     <t>Average</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -313,195 +502,6 @@
   </si>
   <si>
     <t>Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Poseidon </t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>TG</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nimbus Number Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>EC2</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>EC2 Number Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Jobs</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>n/a</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Average</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stddev</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time-to-Completion (in s)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>m1.large</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Average</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Startup Time (in s)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Memory (in MB)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Instances</t>
-  </si>
-  <si>
-    <t>Daten</t>
-  </si>
-  <si>
-    <t>Ergebnis</t>
-  </si>
-  <si>
-    <t>Mittelwert - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>STABW - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>Gesamt: Mittelwert - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>Gesamt: STABW - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>Mittelwert - Startup Time (in s)2</t>
-  </si>
-  <si>
-    <t>Gesamt: Mittelwert - Startup Time (in s)2</t>
-  </si>
-  <si>
-    <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poseidon (CHARM)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 core</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Cores</t>
-  </si>
-  <si>
-    <t>Number Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nodes</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>m1.large</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 STABW - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>2 STABW - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>4 STABW - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>1 Mittelwert - Startup Time (in s)2</t>
-  </si>
-  <si>
-    <t>2 Mittelwert - Startup Time (in s)2</t>
-  </si>
-  <si>
-    <t>4 Mittelwert - Startup Time (in s)2</t>
-  </si>
-  <si>
-    <t>Summe - Number Instances</t>
-  </si>
-  <si>
-    <t>Gesamt: Summe - Number Instances</t>
-  </si>
-  <si>
-    <t>Cores</t>
-  </si>
-  <si>
-    <t>m1.large</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Adaptive Scenario</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time for completion for n jobs</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jobs run as soon as a resource becomes available</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># TG</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># Nimbus</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># EC2</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -509,9 +509,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -746,7 +747,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -818,6 +819,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -917,11 +919,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="543987816"/>
-        <c:axId val="543749608"/>
+        <c:axId val="606705656"/>
+        <c:axId val="561211096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="543987816"/>
+        <c:axId val="606705656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -937,14 +939,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="543749608"/>
+        <c:crossAx val="561211096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="543749608"/>
+        <c:axId val="561211096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -973,7 +975,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -990,7 +991,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="543987816"/>
+        <c:crossAx val="606705656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1066,12 +1067,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="499577032"/>
-        <c:axId val="561706376"/>
+        <c:axId val="499618952"/>
+        <c:axId val="625072712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="499577032"/>
+        <c:axId val="499618952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1087,14 +1087,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="561706376"/>
+        <c:crossAx val="625072712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="561706376"/>
+        <c:axId val="625072712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1116,7 +1116,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -1130,7 +1129,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="499577032"/>
+        <c:crossAx val="499618952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1274,56 +1273,6 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.816388888888" refreshedVersion="3" recordCount="16">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A30:D46" sheet="Setup Times"/>
-  </cacheSource>
-  <cacheFields count="4">
-    <cacheField name="Instance" numFmtId="0">
-      <sharedItems count="2">
-        <s v="2 cores"/>
-        <s v="2 core"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Number Instances" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="3">
-        <n v="1"/>
-        <n v="2"/>
-        <n v="4"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Number Cores" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="8" count="3">
-        <n v="2"/>
-        <n v="4"/>
-        <n v="8"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Startup Time (in s)" numFmtId="3">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="276.08450388900002" maxValue="472.14579200700001" count="16">
-        <n v="313.49457287799999"/>
-        <n v="295.03079795000002"/>
-        <n v="276.08450388900002"/>
-        <n v="314.97212505300001"/>
-        <n v="315.11944603900002"/>
-        <n v="305.19036102299998"/>
-        <n v="365.65275192299998"/>
-        <n v="472.14579200700001"/>
-        <n v="397.81742381999999"/>
-        <n v="376.035724878"/>
-        <n v="372.41291689899998"/>
-        <n v="373.65681600599999"/>
-        <n v="362.95128488500001"/>
-        <n v="376.37267208100002"/>
-        <n v="361.68812417999999"/>
-        <n v="381.790049076"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.819236111114" refreshedVersion="3" recordCount="20">
   <cacheSource type="worksheet">
     <worksheetSource ref="A53:E73" sheet="Setup Times"/>
@@ -1401,6 +1350,56 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.816388888888" refreshedVersion="3" recordCount="16">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A30:D46" sheet="Setup Times"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Instance" numFmtId="0">
+      <sharedItems count="2">
+        <s v="2 cores"/>
+        <s v="2 core"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Number Instances" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="3">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="4"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Number Cores" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="8" count="3">
+        <n v="2"/>
+        <n v="4"/>
+        <n v="8"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Startup Time (in s)" numFmtId="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="276.08450388900002" maxValue="472.14579200700001" count="16">
+        <n v="313.49457287799999"/>
+        <n v="295.03079795000002"/>
+        <n v="276.08450388900002"/>
+        <n v="314.97212505300001"/>
+        <n v="315.11944603900002"/>
+        <n v="305.19036102299998"/>
+        <n v="365.65275192299998"/>
+        <n v="472.14579200700001"/>
+        <n v="397.81742381999999"/>
+        <n v="376.035724878"/>
+        <n v="372.41291689899998"/>
+        <n v="373.65681600599999"/>
+        <n v="362.95128488500001"/>
+        <n v="376.37267208100002"/>
+        <n v="361.68812417999999"/>
+        <n v="381.790049076"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38662.629386574074" refreshedVersion="3" recordCount="39">
   <cacheSource type="worksheet">
@@ -1565,247 +1564,247 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="16">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="4"/>
-  </r>
-  <r>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="20">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="5"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <x v="6"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <x v="7"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <x v="8"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <x v="9"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="10"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="11"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="12"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="13"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="14"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="15"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="16"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="17"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="18"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="19"/>
+    <x v="19"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="20">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="16">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="9"/>
+  </r>
+  <r>
     <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="10"/>
+  </r>
+  <r>
     <x v="1"/>
     <x v="2"/>
     <x v="2"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="4"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="5"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="6"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="7"/>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="8"/>
-    <x v="8"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="9"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="10"/>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
     <x v="11"/>
-    <x v="11"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="12"/>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="13"/>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="14"/>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="15"/>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="16"/>
-    <x v="16"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="17"/>
-    <x v="17"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="18"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="19"/>
-    <x v="19"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -2128,75 +2127,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="G53:I63" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
-  <pivotFields count="5">
-    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" numFmtId="3" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="10">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Mittelwert - Startup Time (in s)" fld="3" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="STABW - Startup Time (in s)" fld="3" subtotal="stdDev" baseField="0" baseItem="0"/>
-  </dataFields>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="G30:J44" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="4">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
@@ -2283,8 +2214,76 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="6" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="G53:I63" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="5">
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" numFmtId="3" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Mittelwert - Startup Time (in s)" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - Startup Time (in s)" fld="3" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="G5:I20" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
@@ -2367,7 +2366,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:I12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
@@ -2786,8 +2785,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50:D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2802,12 +2801,12 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -2815,36 +2814,36 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="39">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2864,7 +2863,7 @@
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -2884,7 +2883,7 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -2904,7 +2903,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2924,7 +2923,7 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -2944,7 +2943,7 @@
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -2964,7 +2963,7 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2984,7 +2983,7 @@
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -3004,7 +3003,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -3024,7 +3023,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3044,7 +3043,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3064,7 +3063,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -3084,7 +3083,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3104,7 +3103,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -3124,7 +3123,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -3144,7 +3143,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -3164,7 +3163,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3195,7 +3194,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3226,7 +3225,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -3257,7 +3256,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -3280,7 +3279,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -3303,7 +3302,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -3324,7 +3323,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -3345,7 +3344,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -3366,7 +3365,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -3387,7 +3386,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -3408,7 +3407,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -3429,7 +3428,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -3450,7 +3449,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -3471,7 +3470,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="B34">
         <v>8</v>
@@ -3492,7 +3491,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="B35">
         <v>8</v>
@@ -3513,7 +3512,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -3534,7 +3533,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -3555,7 +3554,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="44" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="B38" s="44">
         <v>2</v>
@@ -3576,7 +3575,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -3597,7 +3596,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -3618,7 +3617,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -3639,7 +3638,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -3660,7 +3659,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -3681,7 +3680,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -3702,7 +3701,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -3723,7 +3722,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -3754,7 +3753,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -3785,7 +3784,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -3806,7 +3805,7 @@
     </row>
     <row r="49" spans="1:8" s="41" customFormat="1">
       <c r="A49" s="41" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B49" s="41">
         <v>2</v>
@@ -3827,7 +3826,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="39" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B50" s="39">
         <v>4</v>
@@ -3848,7 +3847,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -3869,7 +3868,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -3890,7 +3889,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -3911,7 +3910,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -3932,7 +3931,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -3953,7 +3952,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -3974,7 +3973,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -3995,7 +3994,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -4016,7 +4015,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B59">
         <v>15</v>
@@ -4037,7 +4036,7 @@
     </row>
     <row r="60" spans="1:8" hidden="1">
       <c r="A60" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -4058,7 +4057,7 @@
     </row>
     <row r="61" spans="1:8" hidden="1">
       <c r="A61" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -4070,7 +4069,7 @@
     </row>
     <row r="62" spans="1:8" hidden="1">
       <c r="A62" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -4082,7 +4081,7 @@
     </row>
     <row r="63" spans="1:8" hidden="1">
       <c r="A63" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -4094,7 +4093,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -4115,7 +4114,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -4136,7 +4135,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -4167,7 +4166,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -4198,7 +4197,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -4229,7 +4228,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -4252,7 +4251,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -4275,7 +4274,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -4298,7 +4297,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -4321,7 +4320,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -4344,7 +4343,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -4367,7 +4366,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B75">
         <v>8</v>
@@ -4390,7 +4389,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B76">
         <v>8</v>
@@ -4413,7 +4412,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B77">
         <v>16</v>
@@ -4436,7 +4435,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B78">
         <v>16</v>
@@ -4459,7 +4458,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B79">
         <v>16</v>
@@ -4482,7 +4481,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B80">
         <v>16</v>
@@ -4505,7 +4504,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B81">
         <v>16</v>
@@ -4528,7 +4527,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B82">
         <v>16</v>
@@ -4551,7 +4550,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="B83">
         <v>16</v>
@@ -4574,7 +4573,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -4594,7 +4593,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -4614,7 +4613,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -4634,7 +4633,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -4654,7 +4653,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -4674,7 +4673,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -4694,7 +4693,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -4714,7 +4713,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -4734,7 +4733,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -4754,7 +4753,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="B93">
         <v>4</v>
@@ -4774,7 +4773,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="B94">
         <v>4</v>
@@ -4794,7 +4793,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -4847,45 +4846,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="26" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
       <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="G5" s="11" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4900,7 +4899,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="I6" s="17">
         <v>221.43898490266665</v>
@@ -4908,7 +4907,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4924,7 +4923,7 @@
       </c>
       <c r="G7" s="32"/>
       <c r="H7" s="18" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="I7" s="21">
         <v>27.888301147358074</v>
@@ -4932,7 +4931,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -4948,7 +4947,7 @@
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="18" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="I8" s="21">
         <v>6</v>
@@ -4956,7 +4955,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4974,7 +4973,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="I9" s="17">
         <v>230.1513251065</v>
@@ -4982,7 +4981,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -4998,7 +4997,7 @@
       </c>
       <c r="G10" s="32"/>
       <c r="H10" s="18" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="I10" s="21">
         <v>21.442701960879447</v>
@@ -5006,7 +5005,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5022,7 +5021,7 @@
       </c>
       <c r="G11" s="32"/>
       <c r="H11" s="18" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="I11" s="21">
         <v>4</v>
@@ -5030,7 +5029,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -5048,7 +5047,7 @@
         <v>8</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="I12" s="17">
         <v>524.47522211100011</v>
@@ -5056,7 +5055,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -5072,7 +5071,7 @@
       </c>
       <c r="G13" s="32"/>
       <c r="H13" s="18" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="I13" s="21">
         <v>249.37176975472715</v>
@@ -5080,7 +5079,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -5096,7 +5095,7 @@
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="18" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="I14" s="21">
         <v>32</v>
@@ -5104,7 +5103,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -5122,7 +5121,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="I15" s="17">
         <v>338.08045351500004</v>
@@ -5130,7 +5129,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -5146,7 +5145,7 @@
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="18" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="I16" s="21">
         <v>46.784586737362908</v>
@@ -5154,7 +5153,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -5170,7 +5169,7 @@
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="18" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="I17" s="21">
         <v>16</v>
@@ -5178,7 +5177,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -5193,7 +5192,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="H18" s="33"/>
       <c r="I18" s="17">
@@ -5202,7 +5201,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -5217,7 +5216,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="H19" s="33"/>
       <c r="I19" s="17">
@@ -5226,7 +5225,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -5241,7 +5240,7 @@
         <v>0.75</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>115</v>
+        <v>42</v>
       </c>
       <c r="H20" s="34"/>
       <c r="I20" s="25">
@@ -5250,7 +5249,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -5267,7 +5266,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -5284,7 +5283,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -5301,7 +5300,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -5318,7 +5317,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>44</v>
       </c>
       <c r="B25">
         <v>16</v>
@@ -5335,19 +5334,19 @@
     </row>
     <row r="26" spans="1:10">
       <c r="C26" t="s">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="D26" s="2">
         <f>AVERAGE(D6:D25)</f>
         <v>373.44653231864999</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="C27" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="D27" s="2">
         <f>STDEV(D6:D25)</f>
@@ -5357,42 +5356,42 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="26" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="B29" s="26"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>70</v>
+        <v>122</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>103</v>
+        <v>30</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -5410,7 +5409,7 @@
         <v>2</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>98</v>
+        <v>25</v>
       </c>
       <c r="J31" s="17">
         <v>302.94028916180002</v>
@@ -5418,7 +5417,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -5435,7 +5434,7 @@
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
       <c r="I32" s="18" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="J32" s="21">
         <v>17.23574117758357</v>
@@ -5443,7 +5442,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -5458,7 +5457,7 @@
         <v>0.5625</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="H33" s="33"/>
       <c r="I33" s="33"/>
@@ -5468,7 +5467,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -5483,7 +5482,7 @@
         <v>0.89513888888888893</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -5493,7 +5492,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5514,7 +5513,7 @@
         <v>4</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>98</v>
+        <v>25</v>
       </c>
       <c r="J35" s="17">
         <v>305.19036102299998</v>
@@ -5522,7 +5521,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -5540,7 +5539,7 @@
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
       <c r="I36" s="18" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="J36" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5548,7 +5547,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -5564,7 +5563,7 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>112</v>
+        <v>39</v>
       </c>
       <c r="H37" s="33"/>
       <c r="I37" s="33"/>
@@ -5574,7 +5573,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -5590,7 +5589,7 @@
         <v>0.57916666666666672</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>109</v>
+        <v>36</v>
       </c>
       <c r="H38" s="33"/>
       <c r="I38" s="33"/>
@@ -5600,7 +5599,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -5622,7 +5621,7 @@
         <v>8</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>98</v>
+        <v>25</v>
       </c>
       <c r="J39" s="17">
         <v>384.05235557549997</v>
@@ -5630,7 +5629,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -5648,7 +5647,7 @@
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
       <c r="I40" s="18" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="J40" s="21">
         <v>32.66972061151673</v>
@@ -5656,7 +5655,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -5672,7 +5671,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="33"/>
@@ -5682,7 +5681,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -5697,7 +5696,7 @@
         <v>0.70972222222222225</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="H42" s="33"/>
       <c r="I42" s="33"/>
@@ -5707,7 +5706,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -5722,7 +5721,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
@@ -5732,7 +5731,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -5747,7 +5746,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -5757,7 +5756,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -5774,7 +5773,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -5791,7 +5790,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>29</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -5806,19 +5805,19 @@
     </row>
     <row r="48" spans="1:10">
       <c r="C48" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
       <c r="D48" s="2">
         <f>AVERAGE(D30:D47)</f>
         <v>356.83130192700003</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="C49" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="D49" s="2">
         <f>STDEV(D31:D47)</f>
@@ -5835,37 +5834,37 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="26" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="B52" s="26"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="26" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>70</v>
+        <v>122</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>116</v>
+        <v>43</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>92</v>
+        <v>19</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -5874,7 +5873,7 @@
         <v>8</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>88</v>
+        <v>15</v>
       </c>
       <c r="E54" s="7">
         <v>0.89513888888888893</v>
@@ -5883,7 +5882,7 @@
         <v>4</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="I54" s="17">
         <v>14.1872649193</v>
@@ -5891,7 +5890,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -5907,7 +5906,7 @@
       </c>
       <c r="G55" s="32"/>
       <c r="H55" s="18" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="I55" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5915,7 +5914,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -5933,7 +5932,7 @@
         <v>8</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="I56" s="17">
         <v>44.782275199920001</v>
@@ -5941,7 +5940,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -5957,7 +5956,7 @@
       </c>
       <c r="G57" s="32"/>
       <c r="H57" s="18" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="I57" s="21">
         <v>15.843792242505828</v>
@@ -5965,7 +5964,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -5983,7 +5982,7 @@
         <v>16</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="I58" s="17">
         <v>56.964924156674996</v>
@@ -5991,7 +5990,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -6007,7 +6006,7 @@
       </c>
       <c r="G59" s="32"/>
       <c r="H59" s="18" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="I59" s="21">
         <v>9.4994883808250847</v>
@@ -6015,7 +6014,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -6033,7 +6032,7 @@
         <v>32</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>94</v>
+        <v>21</v>
       </c>
       <c r="I60" s="17">
         <v>187.55037531850999</v>
@@ -6041,7 +6040,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -6057,7 +6056,7 @@
       </c>
       <c r="G61" s="32"/>
       <c r="H61" s="18" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="I61" s="21">
         <v>179.97433590633514</v>
@@ -6065,7 +6064,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -6080,7 +6079,7 @@
         <v>0.59236111111111112</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="H62" s="33"/>
       <c r="I62" s="17">
@@ -6089,7 +6088,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -6104,7 +6103,7 @@
         <v>0.61875000000000002</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="H63" s="34"/>
       <c r="I63" s="25">
@@ -6113,7 +6112,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B64">
         <v>8</v>
@@ -6130,7 +6129,7 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -6147,7 +6146,7 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -6164,7 +6163,7 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B67">
         <v>8</v>
@@ -6181,7 +6180,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B68">
         <v>8</v>
@@ -6198,7 +6197,7 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -6215,7 +6214,7 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B70">
         <v>8</v>
@@ -6232,7 +6231,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -6249,7 +6248,7 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -6266,7 +6265,7 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -6281,7 +6280,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B74">
         <v>2</v>
@@ -6296,19 +6295,19 @@
     </row>
     <row r="75" spans="1:5">
       <c r="C75" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="D75" s="2">
         <f>AVERAGE(D55:D74)</f>
         <v>117.073104536535</v>
       </c>
       <c r="E75" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="C76" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="D76" s="2">
         <f>STDEV(D55:D74)</f>
@@ -6321,7 +6320,6 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -6336,8 +6334,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -6353,69 +6351,69 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="28" t="s">
-        <v>119</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="30" t="s">
-        <v>120</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" ht="39" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="B5" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>25</v>
-      </c>
       <c r="F5" s="29" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="K5" s="28" t="s">
-        <v>122</v>
+        <v>49</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>123</v>
+        <v>50</v>
       </c>
       <c r="M5" s="28" t="s">
-        <v>124</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -6450,13 +6448,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -6491,13 +6489,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="B8" s="31">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -6532,7 +6530,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -6570,7 +6568,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -6605,7 +6603,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>32</v>
@@ -6646,7 +6644,7 @@
     </row>
     <row r="12" spans="1:14" s="49" customFormat="1" ht="14" thickBot="1">
       <c r="A12" s="49" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B12" s="49">
         <v>32</v>
@@ -6687,7 +6685,7 @@
     </row>
     <row r="13" spans="1:14" ht="40" thickTop="1">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -6718,12 +6716,12 @@
         <v>2</v>
       </c>
       <c r="N13" s="52" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="39">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -6754,12 +6752,12 @@
         <v>2</v>
       </c>
       <c r="N14" s="52" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="39">
       <c r="A15" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="B15" s="41">
         <v>16</v>
@@ -6790,12 +6788,12 @@
         <v>1</v>
       </c>
       <c r="N15" s="52" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="39">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -6826,12 +6824,12 @@
         <v>0</v>
       </c>
       <c r="N16" s="52" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>32</v>
@@ -6864,7 +6862,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B18">
         <v>32</v>
@@ -6897,7 +6895,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>32</v>
@@ -6938,7 +6936,6 @@
   <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -6951,57 +6948,57 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="53" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="54" customFormat="1" ht="39">
       <c r="A5" s="54" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="F5" s="54" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="G5" s="54" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="H5" s="54" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="I5" s="54" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="J5" s="54" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="K5" s="54" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -7038,6 +7035,150 @@
       </c>
       <c r="K6">
         <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>45</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7" s="35">
+        <v>2182.05676103</v>
+      </c>
+      <c r="H7">
+        <f>G7/60</f>
+        <v>36.367612683833336</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>45</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8" s="35">
+        <v>469.38359808899997</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ref="H8:H10" si="0">G8/60</f>
+        <v>7.8230599681499999</v>
+      </c>
+      <c r="I8">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>45</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9" s="55">
+        <v>2614.1951420300002</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>43.569919033833337</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>45</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10" s="35">
+        <v>2685.3280220000001</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>44.755467033333339</v>
+      </c>
+      <c r="I10">
+        <v>8</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -7083,10 +7224,10 @@
   <sheetData>
     <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -7098,7 +7239,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="11" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
@@ -7122,12 +7263,12 @@
         <v>32</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
@@ -7144,7 +7285,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="18" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="20">
@@ -7161,7 +7302,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="18" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
@@ -7182,7 +7323,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="18" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
       <c r="B8" s="19">
         <v>2070.8984270000001</v>
@@ -7199,7 +7340,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="B9" s="19">
         <v>1095.4940549999999</v>
@@ -7226,7 +7367,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="18" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
@@ -7247,7 +7388,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="18" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -7268,7 +7409,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="22" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="B12" s="23">
         <v>1583.1962410000001</v>

</xml_diff>

<commit_message>
Some Typos Added BigJob description Description of Deadline experiment started
git-svn-id: file://localhost/tmp/svn2git/svn@1811 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="220" windowWidth="35740" windowHeight="22200" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="220" yWindow="220" windowWidth="35740" windowHeight="22200" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NAMD Runtimes" sheetId="1" r:id="rId1"/>
@@ -970,7 +970,7 @@
                     <a:latin typeface="+mn-lt"/>
                     <a:cs typeface="Times"/>
                   </a:rPr>
-                  <a:t>Waiting Time (in sec)</a:t>
+                  <a:t>Startup Time (in sec)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1117,6 +1117,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -4816,7 +4817,6 @@
       <c r="A98" s="1"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -4832,8 +4832,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O56" sqref="O56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -6952,11 +6952,14 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="3" max="3" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="53" t="s">
@@ -7102,10 +7105,10 @@
         <v>7.8230599681499999</v>
       </c>
       <c r="I8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -7439,6 +7442,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Related Work Performance scenario II detailed
git-svn-id: file://localhost/tmp/svn2git/svn@1820 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -2796,7 +2796,7 @@
   <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:D25"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -3753,7 +3753,7 @@
         <v>611.88485693899997</v>
       </c>
       <c r="H46" s="2">
-        <f t="shared" ref="H46:H66" si="0">G46-D46</f>
+        <f>G46-D46</f>
         <v>7.9553459389999261</v>
       </c>
       <c r="I46" s="27">
@@ -3784,7 +3784,7 @@
         <v>640.46440601300003</v>
       </c>
       <c r="H47" s="2">
-        <f t="shared" ref="H47" si="1">G47-D47</f>
+        <f>G47-D47</f>
         <v>8.0167670130000488</v>
       </c>
       <c r="I47" s="27">
@@ -4166,7 +4166,7 @@
         <v>560.973680973</v>
       </c>
       <c r="H66" s="2">
-        <f t="shared" si="0"/>
+        <f>G66-D66</f>
         <v>12.070587972999988</v>
       </c>
       <c r="I66" s="27">
@@ -4197,7 +4197,7 @@
         <v>550.83944201500003</v>
       </c>
       <c r="H67" s="2">
-        <f t="shared" ref="H67" si="2">G67-D67</f>
+        <f>G67-D67</f>
         <v>8.2021750150000798</v>
       </c>
       <c r="I67" s="27">
@@ -4228,7 +4228,7 @@
         <v>600.412503958</v>
       </c>
       <c r="H68" s="2">
-        <f t="shared" ref="H68" si="3">G68-D68</f>
+        <f>G68-D68</f>
         <v>15.355416957999978</v>
       </c>
       <c r="I68" s="27">
@@ -4840,7 +4840,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
@@ -6345,7 +6345,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -6943,6 +6943,7 @@
       <c r="I21" s="47"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -6960,7 +6961,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -7440,6 +7441,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Further enhancements of BigJob section in particular the Cloud BigJob Refined BigJob figure with different backends
git-svn-id: file://localhost/tmp/svn2git/svn@1880 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -31,6 +31,186 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="127">
   <si>
+    <t>Ergebnis</t>
+  </si>
+  <si>
+    <t>Mittelwert - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>STABW - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>Gesamt: Mittelwert - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>Gesamt: STABW - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>Mittelwert - Startup Time (in s)2</t>
+  </si>
+  <si>
+    <t>Gesamt: Mittelwert - Startup Time (in s)2</t>
+  </si>
+  <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon (CHARM)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 core</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Cores</t>
+  </si>
+  <si>
+    <t>Number Cores</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nodes</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Cores</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>m1.large</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 STABW - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>2 STABW - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>4 STABW - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>1 Mittelwert - Startup Time (in s)2</t>
+  </si>
+  <si>
+    <t>2 Mittelwert - Startup Time (in s)2</t>
+  </si>
+  <si>
+    <t>4 Mittelwert - Startup Time (in s)2</t>
+  </si>
+  <si>
+    <t>Summe - Number Instances</t>
+  </si>
+  <si>
+    <t>Gesamt: Summe - Number Instances</t>
+  </si>
+  <si>
+    <t>Cores</t>
+  </si>
+  <si>
+    <t>m1.large</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adaptive Scenario</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time for completion for n jobs</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jobs run as soon as a resource becomes available</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t># TG</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t># Nimbus</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t># EC2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC2 m1.large</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nimbus</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI 16 core
+Nimbus 16 core</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Run ID</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Replicas</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAX_RUNTIME (in min)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Check Period (in min)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max Cloud Pilots</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cloud Pilot Size</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Runtime (in min)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Runtime (in sec)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t># Nimbus</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t># Poseidon</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t># Cloud Pilots</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start Pilot if not sufficient progress is made</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
     <t>Deadline Scenario</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -332,186 +512,6 @@
   </si>
   <si>
     <t>Daten</t>
-  </si>
-  <si>
-    <t>Ergebnis</t>
-  </si>
-  <si>
-    <t>Mittelwert - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>STABW - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>Gesamt: Mittelwert - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>Gesamt: STABW - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>Mittelwert - Startup Time (in s)2</t>
-  </si>
-  <si>
-    <t>Gesamt: Mittelwert - Startup Time (in s)2</t>
-  </si>
-  <si>
-    <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poseidon (CHARM)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 core</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Cores</t>
-  </si>
-  <si>
-    <t>Number Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nodes</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>m1.large</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 STABW - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>2 STABW - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>4 STABW - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>1 Mittelwert - Startup Time (in s)2</t>
-  </si>
-  <si>
-    <t>2 Mittelwert - Startup Time (in s)2</t>
-  </si>
-  <si>
-    <t>4 Mittelwert - Startup Time (in s)2</t>
-  </si>
-  <si>
-    <t>Summe - Number Instances</t>
-  </si>
-  <si>
-    <t>Gesamt: Summe - Number Instances</t>
-  </si>
-  <si>
-    <t>Cores</t>
-  </si>
-  <si>
-    <t>m1.large</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Adaptive Scenario</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time for completion for n jobs</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jobs run as soon as a resource becomes available</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># TG</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># Nimbus</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># EC2</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Average</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>EC2 m1.large</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nimbus</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>LONI 16 core
-Nimbus 16 core</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Run ID</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Replicas</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>MAX_RUNTIME (in min)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Check Period (in min)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Max Cloud Pilots</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cloud Pilot Size</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Runtime (in min)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Runtime (in sec)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># Nimbus</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># Cloud Pilots</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Start Pilot if not sufficient progress is made</t>
-    <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -927,11 +927,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="632319608"/>
-        <c:axId val="632322696"/>
+        <c:axId val="645061624"/>
+        <c:axId val="645066472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="632319608"/>
+        <c:axId val="645061624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -947,14 +947,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="632322696"/>
+        <c:crossAx val="645066472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="632322696"/>
+        <c:axId val="645066472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -983,7 +983,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -1000,7 +999,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="632319608"/>
+        <c:crossAx val="645061624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1076,11 +1075,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="631343448"/>
-        <c:axId val="631367256"/>
+        <c:axId val="644520504"/>
+        <c:axId val="644524008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="631343448"/>
+        <c:axId val="644520504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1096,14 +1095,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="631367256"/>
+        <c:crossAx val="644524008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="631367256"/>
+        <c:axId val="644524008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,7 +1124,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -1139,7 +1137,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="631343448"/>
+        <c:crossAx val="644520504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1283,56 +1281,6 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.816388888888" refreshedVersion="3" recordCount="16">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A30:D46" sheet="Setup Times"/>
-  </cacheSource>
-  <cacheFields count="4">
-    <cacheField name="Instance" numFmtId="0">
-      <sharedItems count="2">
-        <s v="2 cores"/>
-        <s v="2 core"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Number Instances" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="3">
-        <n v="1"/>
-        <n v="2"/>
-        <n v="4"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Number Cores" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="8" count="3">
-        <n v="2"/>
-        <n v="4"/>
-        <n v="8"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Startup Time (in s)" numFmtId="3">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="276.08450388900002" maxValue="472.14579200700001" count="16">
-        <n v="313.49457287799999"/>
-        <n v="295.03079795000002"/>
-        <n v="276.08450388900002"/>
-        <n v="314.97212505300001"/>
-        <n v="315.11944603900002"/>
-        <n v="305.19036102299998"/>
-        <n v="365.65275192299998"/>
-        <n v="472.14579200700001"/>
-        <n v="397.81742381999999"/>
-        <n v="376.035724878"/>
-        <n v="372.41291689899998"/>
-        <n v="373.65681600599999"/>
-        <n v="362.95128488500001"/>
-        <n v="376.37267208100002"/>
-        <n v="361.68812417999999"/>
-        <n v="381.790049076"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.819236111114" refreshedVersion="3" recordCount="20">
   <cacheSource type="worksheet">
     <worksheetSource ref="A53:E73" sheet="Setup Times"/>
@@ -1410,6 +1358,56 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.816388888888" refreshedVersion="3" recordCount="16">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A30:D46" sheet="Setup Times"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Instance" numFmtId="0">
+      <sharedItems count="2">
+        <s v="2 cores"/>
+        <s v="2 core"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Number Instances" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="3">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="4"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Number Cores" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="8" count="3">
+        <n v="2"/>
+        <n v="4"/>
+        <n v="8"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Startup Time (in s)" numFmtId="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="276.08450388900002" maxValue="472.14579200700001" count="16">
+        <n v="313.49457287799999"/>
+        <n v="295.03079795000002"/>
+        <n v="276.08450388900002"/>
+        <n v="314.97212505300001"/>
+        <n v="315.11944603900002"/>
+        <n v="305.19036102299998"/>
+        <n v="365.65275192299998"/>
+        <n v="472.14579200700001"/>
+        <n v="397.81742381999999"/>
+        <n v="376.035724878"/>
+        <n v="372.41291689899998"/>
+        <n v="373.65681600599999"/>
+        <n v="362.95128488500001"/>
+        <n v="376.37267208100002"/>
+        <n v="361.68812417999999"/>
+        <n v="381.790049076"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38662.629386574074" refreshedVersion="3" recordCount="39">
   <cacheSource type="worksheet">
@@ -1574,247 +1572,247 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="16">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="4"/>
-  </r>
-  <r>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="20">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="5"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <x v="6"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <x v="7"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <x v="8"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <x v="9"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="10"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="11"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="12"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="13"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="14"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="15"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="16"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="17"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="18"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="19"/>
+    <x v="19"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="20">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="16">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="9"/>
+  </r>
+  <r>
     <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="10"/>
+  </r>
+  <r>
     <x v="1"/>
     <x v="2"/>
     <x v="2"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="4"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="5"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="6"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="7"/>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="8"/>
-    <x v="8"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="9"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="10"/>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
     <x v="11"/>
-    <x v="11"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="12"/>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="13"/>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="14"/>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="15"/>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="16"/>
-    <x v="16"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="17"/>
-    <x v="17"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="18"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="19"/>
-    <x v="19"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -2137,75 +2135,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="G53:I63" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
-  <pivotFields count="5">
-    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" numFmtId="3" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="10">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Mittelwert - Startup Time (in s)" fld="3" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="STABW - Startup Time (in s)" fld="3" subtotal="stdDev" baseField="0" baseItem="0"/>
-  </dataFields>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="G30:J44" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="4">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
@@ -2287,6 +2217,74 @@
   </colItems>
   <dataFields count="2">
     <dataField name="Mittelwert - Startup Time (in s)2" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - Startup Time (in s)" fld="3" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="G53:I63" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="5">
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" numFmtId="3" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Mittelwert - Startup Time (in s)" fld="3" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="STABW - Startup Time (in s)" fld="3" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
 </pivotTableDefinition>
@@ -2811,12 +2809,12 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -2824,36 +2822,36 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="39">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2873,7 +2871,7 @@
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -2893,7 +2891,7 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -2913,7 +2911,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2933,7 +2931,7 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -2953,7 +2951,7 @@
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -2973,7 +2971,7 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2993,7 +2991,7 @@
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -3013,7 +3011,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -3033,7 +3031,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3053,7 +3051,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3073,7 +3071,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -3093,7 +3091,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3113,7 +3111,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -3133,7 +3131,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -3153,7 +3151,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -3173,7 +3171,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3204,7 +3202,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3235,7 +3233,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -3266,7 +3264,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -3289,7 +3287,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -3312,7 +3310,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -3333,7 +3331,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -3354,7 +3352,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -3375,7 +3373,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -3396,7 +3394,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -3417,7 +3415,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -3438,7 +3436,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -3459,7 +3457,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -3480,7 +3478,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B34">
         <v>8</v>
@@ -3501,7 +3499,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B35">
         <v>8</v>
@@ -3522,7 +3520,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -3543,7 +3541,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -3564,7 +3562,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="44" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="B38" s="44">
         <v>2</v>
@@ -3585,7 +3583,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -3606,7 +3604,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -3627,7 +3625,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -3648,7 +3646,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -3669,7 +3667,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -3690,7 +3688,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -3711,7 +3709,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -3732,7 +3730,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -3763,7 +3761,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -3794,7 +3792,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -3815,7 +3813,7 @@
     </row>
     <row r="49" spans="1:8" s="41" customFormat="1">
       <c r="A49" s="41" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B49" s="41">
         <v>2</v>
@@ -3836,7 +3834,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="39" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B50" s="39">
         <v>4</v>
@@ -3857,7 +3855,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -3878,7 +3876,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -3899,7 +3897,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -3920,7 +3918,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -3941,7 +3939,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -3962,7 +3960,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -3983,7 +3981,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -4004,7 +4002,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -4025,7 +4023,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="B59">
         <v>15</v>
@@ -4046,7 +4044,7 @@
     </row>
     <row r="60" spans="1:8" hidden="1">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -4067,7 +4065,7 @@
     </row>
     <row r="61" spans="1:8" hidden="1">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -4079,7 +4077,7 @@
     </row>
     <row r="62" spans="1:8" hidden="1">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -4091,7 +4089,7 @@
     </row>
     <row r="63" spans="1:8" hidden="1">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -4103,7 +4101,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -4124,7 +4122,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -4145,7 +4143,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -4176,7 +4174,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -4207,7 +4205,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -4238,7 +4236,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -4261,7 +4259,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -4284,7 +4282,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -4307,7 +4305,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -4330,7 +4328,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -4353,7 +4351,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -4376,7 +4374,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B75">
         <v>8</v>
@@ -4399,7 +4397,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B76">
         <v>8</v>
@@ -4422,7 +4420,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B77">
         <v>16</v>
@@ -4445,7 +4443,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B78">
         <v>16</v>
@@ -4468,7 +4466,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B79">
         <v>16</v>
@@ -4491,7 +4489,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B80">
         <v>16</v>
@@ -4514,7 +4512,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B81">
         <v>16</v>
@@ -4537,7 +4535,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B82">
         <v>16</v>
@@ -4560,7 +4558,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B83">
         <v>16</v>
@@ -4583,7 +4581,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -4603,7 +4601,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -4623,7 +4621,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -4643,7 +4641,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -4663,7 +4661,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -4683,7 +4681,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -4703,7 +4701,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -4723,7 +4721,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -4743,7 +4741,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -4763,7 +4761,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="B93">
         <v>4</v>
@@ -4783,7 +4781,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="B94">
         <v>4</v>
@@ -4803,7 +4801,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -4856,45 +4854,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="26" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4909,7 +4907,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="I6" s="17">
         <v>221.43898490266665</v>
@@ -4917,7 +4915,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4933,7 +4931,7 @@
       </c>
       <c r="G7" s="32"/>
       <c r="H7" s="18" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="I7" s="21">
         <v>27.888301147358074</v>
@@ -4941,7 +4939,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -4957,7 +4955,7 @@
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="18" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="I8" s="21">
         <v>6</v>
@@ -4965,7 +4963,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4983,7 +4981,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="I9" s="17">
         <v>230.1513251065</v>
@@ -4991,7 +4989,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5007,7 +5005,7 @@
       </c>
       <c r="G10" s="32"/>
       <c r="H10" s="18" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="I10" s="21">
         <v>21.442701960879447</v>
@@ -5015,7 +5013,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5031,7 +5029,7 @@
       </c>
       <c r="G11" s="32"/>
       <c r="H11" s="18" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="I11" s="21">
         <v>4</v>
@@ -5039,7 +5037,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -5057,7 +5055,7 @@
         <v>8</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="I12" s="17">
         <v>524.47522211100011</v>
@@ -5065,7 +5063,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -5081,7 +5079,7 @@
       </c>
       <c r="G13" s="32"/>
       <c r="H13" s="18" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="I13" s="21">
         <v>249.37176975472715</v>
@@ -5089,7 +5087,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -5105,7 +5103,7 @@
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="18" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="I14" s="21">
         <v>32</v>
@@ -5113,7 +5111,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -5131,7 +5129,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="I15" s="17">
         <v>338.08045351500004</v>
@@ -5139,7 +5137,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -5155,7 +5153,7 @@
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="18" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="I16" s="21">
         <v>46.784586737362908</v>
@@ -5163,7 +5161,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -5179,7 +5177,7 @@
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="18" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="I17" s="21">
         <v>16</v>
@@ -5187,7 +5185,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -5202,7 +5200,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="H18" s="33"/>
       <c r="I18" s="17">
@@ -5211,7 +5209,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -5226,7 +5224,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>82</v>
+        <v>4</v>
       </c>
       <c r="H19" s="33"/>
       <c r="I19" s="17">
@@ -5235,7 +5233,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -5250,7 +5248,7 @@
         <v>0.75</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="H20" s="34"/>
       <c r="I20" s="25">
@@ -5259,7 +5257,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -5276,7 +5274,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -5293,7 +5291,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -5310,7 +5308,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>14</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -5327,7 +5325,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>16</v>
@@ -5344,19 +5342,19 @@
     </row>
     <row r="26" spans="1:10">
       <c r="C26" t="s">
-        <v>110</v>
+        <v>32</v>
       </c>
       <c r="D26" s="2">
         <f>AVERAGE(D6:D25)</f>
         <v>373.44653231864999</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>111</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="C27" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="D27" s="2">
         <f>STDEV(D6:D25)</f>
@@ -5366,42 +5364,42 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="26" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="B29" s="26"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
-        <v>34</v>
+        <v>83</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>91</v>
+        <v>13</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>88</v>
+        <v>10</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -5419,7 +5417,7 @@
         <v>2</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="J31" s="17">
         <v>302.94028916180002</v>
@@ -5427,7 +5425,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -5444,7 +5442,7 @@
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
       <c r="I32" s="18" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="J32" s="21">
         <v>17.23574117758357</v>
@@ -5452,7 +5450,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -5467,7 +5465,7 @@
         <v>0.5625</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>96</v>
+        <v>18</v>
       </c>
       <c r="H33" s="33"/>
       <c r="I33" s="33"/>
@@ -5477,7 +5475,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -5492,7 +5490,7 @@
         <v>0.89513888888888893</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -5502,7 +5500,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5523,7 +5521,7 @@
         <v>4</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="J35" s="17">
         <v>305.19036102299998</v>
@@ -5531,7 +5529,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -5549,7 +5547,7 @@
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
       <c r="I36" s="18" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="J36" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5557,7 +5555,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -5573,7 +5571,7 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="H37" s="33"/>
       <c r="I37" s="33"/>
@@ -5583,7 +5581,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -5599,7 +5597,7 @@
         <v>0.57916666666666672</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="H38" s="33"/>
       <c r="I38" s="33"/>
@@ -5609,7 +5607,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -5631,7 +5629,7 @@
         <v>8</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="J39" s="17">
         <v>384.05235557549997</v>
@@ -5639,7 +5637,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -5657,7 +5655,7 @@
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
       <c r="I40" s="18" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="J40" s="21">
         <v>32.66972061151673</v>
@@ -5665,7 +5663,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -5681,7 +5679,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="33"/>
@@ -5691,7 +5689,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -5706,7 +5704,7 @@
         <v>0.70972222222222225</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="H42" s="33"/>
       <c r="I42" s="33"/>
@@ -5716,7 +5714,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -5731,7 +5729,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>84</v>
+        <v>6</v>
       </c>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
@@ -5741,7 +5739,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -5756,7 +5754,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>82</v>
+        <v>4</v>
       </c>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -5766,7 +5764,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -5783,7 +5781,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -5800,7 +5798,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -5815,19 +5813,19 @@
     </row>
     <row r="48" spans="1:10">
       <c r="C48" t="s">
-        <v>67</v>
+        <v>116</v>
       </c>
       <c r="D48" s="2">
         <f>AVERAGE(D30:D47)</f>
         <v>356.83130192700003</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>112</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="C49" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="D49" s="2">
         <f>STDEV(D31:D47)</f>
@@ -5844,37 +5842,37 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="26" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
       <c r="B52" s="26"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="26" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>90</v>
+        <v>12</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>101</v>
+        <v>23</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -5883,7 +5881,7 @@
         <v>8</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="E54" s="7">
         <v>0.89513888888888893</v>
@@ -5892,7 +5890,7 @@
         <v>4</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="I54" s="17">
         <v>14.1872649193</v>
@@ -5900,7 +5898,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -5916,7 +5914,7 @@
       </c>
       <c r="G55" s="32"/>
       <c r="H55" s="18" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="I55" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5924,7 +5922,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -5942,7 +5940,7 @@
         <v>8</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="I56" s="17">
         <v>44.782275199920001</v>
@@ -5950,7 +5948,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -5966,7 +5964,7 @@
       </c>
       <c r="G57" s="32"/>
       <c r="H57" s="18" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="I57" s="21">
         <v>15.843792242505828</v>
@@ -5974,7 +5972,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -5992,7 +5990,7 @@
         <v>16</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="I58" s="17">
         <v>56.964924156674996</v>
@@ -6000,7 +5998,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -6016,7 +6014,7 @@
       </c>
       <c r="G59" s="32"/>
       <c r="H59" s="18" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="I59" s="21">
         <v>9.4994883808250847</v>
@@ -6024,7 +6022,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -6042,7 +6040,7 @@
         <v>32</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="I60" s="17">
         <v>187.55037531850999</v>
@@ -6050,7 +6048,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -6066,7 +6064,7 @@
       </c>
       <c r="G61" s="32"/>
       <c r="H61" s="18" t="s">
-        <v>80</v>
+        <v>2</v>
       </c>
       <c r="I61" s="21">
         <v>179.97433590633514</v>
@@ -6074,7 +6072,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -6089,7 +6087,7 @@
         <v>0.59236111111111112</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="H62" s="33"/>
       <c r="I62" s="17">
@@ -6098,7 +6096,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -6113,7 +6111,7 @@
         <v>0.61875000000000002</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>82</v>
+        <v>4</v>
       </c>
       <c r="H63" s="34"/>
       <c r="I63" s="25">
@@ -6122,7 +6120,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B64">
         <v>8</v>
@@ -6139,7 +6137,7 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -6156,7 +6154,7 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -6173,7 +6171,7 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B67">
         <v>8</v>
@@ -6190,7 +6188,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B68">
         <v>8</v>
@@ -6207,7 +6205,7 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -6224,7 +6222,7 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B70">
         <v>8</v>
@@ -6241,7 +6239,7 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -6258,7 +6256,7 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -6275,7 +6273,7 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -6290,7 +6288,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B74">
         <v>2</v>
@@ -6305,19 +6303,19 @@
     </row>
     <row r="75" spans="1:5">
       <c r="C75" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="D75" s="2">
         <f>AVERAGE(D55:D74)</f>
         <v>117.073104536535</v>
       </c>
       <c r="E75" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="C76" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="D76" s="2">
         <f>STDEV(D55:D74)</f>
@@ -6361,69 +6359,69 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="28" t="s">
-        <v>104</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="30" t="s">
-        <v>105</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" ht="39" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>62</v>
+        <v>111</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="K5" s="28" t="s">
-        <v>107</v>
+        <v>29</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>108</v>
+        <v>30</v>
       </c>
       <c r="M5" s="28" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>115</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -6458,13 +6456,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -6499,13 +6497,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="B8" s="31">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>115</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -6540,7 +6538,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -6578,7 +6576,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -6613,7 +6611,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>32</v>
@@ -6654,7 +6652,7 @@
     </row>
     <row r="12" spans="1:14" s="49" customFormat="1" ht="14" thickBot="1">
       <c r="A12" s="49" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B12" s="49">
         <v>32</v>
@@ -6695,7 +6693,7 @@
     </row>
     <row r="13" spans="1:14" ht="40" thickTop="1">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -6726,12 +6724,12 @@
         <v>2</v>
       </c>
       <c r="N13" s="52" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="39">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -6762,12 +6760,12 @@
         <v>2</v>
       </c>
       <c r="N14" s="52" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="39">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="B15" s="41">
         <v>16</v>
@@ -6798,12 +6796,12 @@
         <v>1</v>
       </c>
       <c r="N15" s="52" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="39">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -6834,12 +6832,12 @@
         <v>0</v>
       </c>
       <c r="N16" s="52" t="s">
-        <v>114</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B17">
         <v>32</v>
@@ -6872,7 +6870,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B18">
         <v>32</v>
@@ -6905,7 +6903,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="B19">
         <v>32</v>
@@ -6961,7 +6959,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="H9" sqref="H9:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -6971,50 +6969,50 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="53" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="54" customFormat="1" ht="39">
       <c r="A5" s="54" t="s">
-        <v>115</v>
+        <v>37</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>116</v>
+        <v>38</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>117</v>
+        <v>39</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>118</v>
+        <v>40</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="F5" s="54" t="s">
-        <v>120</v>
+        <v>42</v>
       </c>
       <c r="G5" s="54" t="s">
-        <v>122</v>
+        <v>44</v>
       </c>
       <c r="H5" s="54" t="s">
-        <v>121</v>
+        <v>43</v>
       </c>
       <c r="I5" s="54" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
       <c r="J5" s="54" t="s">
-        <v>124</v>
+        <v>46</v>
       </c>
       <c r="K5" s="54" t="s">
-        <v>125</v>
+        <v>47</v>
       </c>
       <c r="L5" s="54" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -7053,7 +7051,7 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -7164,7 +7162,7 @@
         <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -7203,7 +7201,7 @@
         <v>3</v>
       </c>
       <c r="L10" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -7444,7 +7442,6 @@
   <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7483,10 +7480,10 @@
   <sheetData>
     <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -7498,7 +7495,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="11" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
@@ -7522,12 +7519,12 @@
         <v>32</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
@@ -7544,7 +7541,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="18" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="20">
@@ -7561,7 +7558,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="18" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
@@ -7582,7 +7579,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="18" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="B8" s="19">
         <v>2070.8984270000001</v>
@@ -7599,7 +7596,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="B9" s="19">
         <v>1095.4940549999999</v>
@@ -7626,7 +7623,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="18" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
@@ -7647,7 +7644,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="18" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -7668,7 +7665,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="22" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="B12" s="23">
         <v>1583.1962410000001</v>
@@ -7696,7 +7693,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
included preliminary condor data in graph
git-svn-id: file://localhost/tmp/svn2git/svn@1894 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="220" windowWidth="35740" windowHeight="22200" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="35740" windowHeight="22200" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NAMD Runtimes" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,270 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="133">
+  <si>
+    <t>Average (drop maxima)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon (Grid - adjusted)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon (Grid)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Machine</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nimbus (Chicago)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC2 (c1.xlarge)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC2 (m2.4xlarge)</t>
+  </si>
+  <si>
+    <t>EC2 (m2.4xlarge)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC2 (m2.4xlarge)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Walltime (in sec)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Startup Times</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Startup Time (in s)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Instance</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>m1.large</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Instances</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 cores</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI 8 core
+Nimbus 8 core</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI 8 core 
+Nimbus 16 core</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI 16 core
+Nimbus 8 core</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Startup Time (in s)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Instance</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>m1.large</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>QB (MPI)</t>
+  </si>
+  <si>
+    <t>QB (MPI)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>QB (CHARM)</t>
+  </si>
+  <si>
+    <t>QB (CHARM)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mittelwert - Walltime (in sec)</t>
+  </si>
+  <si>
+    <t>Number Cores (Total)</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>Gesamtergebnis</t>
+  </si>
+  <si>
+    <t>EC2 (c1.xlarge)</t>
+  </si>
+  <si>
+    <t>EC2 (m1.large)</t>
+  </si>
+  <si>
+    <t>EUCA (Indiana)</t>
+  </si>
+  <si>
+    <t>Nimbus (Chicago)</t>
+  </si>
+  <si>
+    <t>CPU Time (in sec)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cores</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Queue Time
+Nimbus</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>n/a</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Poseidon </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>TG</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nimbus Number Cores</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Cores</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC2 Number Cores</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Jobs</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>n/a</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stddev</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time-to-Completion (in s)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>m1.large</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 cores</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Startup Time (in s)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memory (in MB)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Instances</t>
+  </si>
+  <si>
+    <t>Daten</t>
+  </si>
+  <si>
+    <t>LONI/Condor</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resource</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oliver</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon (Condor)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stdev (drop maxima)</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
   <si>
     <t>Ergebnis</t>
   </si>
@@ -151,10 +414,6 @@
   </si>
   <si>
     <t>Nimbus</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poseidon</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
@@ -277,241 +536,6 @@
   <si>
     <t>EC2 (m1.large)</t>
     <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Machine</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nimbus (Chicago)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>EC2 (c1.xlarge)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>EC2 (m2.4xlarge)</t>
-  </si>
-  <si>
-    <t>EC2 (m2.4xlarge)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>EC2 (m2.4xlarge)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Walltime (in sec)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Startup Times</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Startup Time (in s)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Instance</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>m1.large</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Instances</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>LONI 8 core
-Nimbus 8 core</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>LONI 8 core 
-Nimbus 16 core</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>LONI 16 core
-Nimbus 8 core</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Startup Time (in s)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Instance</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Date</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>m1.large</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>QB (MPI)</t>
-  </si>
-  <si>
-    <t>QB (MPI)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>QB (CHARM)</t>
-  </si>
-  <si>
-    <t>QB (CHARM)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mittelwert - Walltime (in sec)</t>
-  </si>
-  <si>
-    <t>Number Cores (Total)</t>
-  </si>
-  <si>
-    <t>Machine</t>
-  </si>
-  <si>
-    <t>Gesamtergebnis</t>
-  </si>
-  <si>
-    <t>EC2 (c1.xlarge)</t>
-  </si>
-  <si>
-    <t>EC2 (m1.large)</t>
-  </si>
-  <si>
-    <t>EUCA (Indiana)</t>
-  </si>
-  <si>
-    <t>Nimbus (Chicago)</t>
-  </si>
-  <si>
-    <t>CPU Time (in sec)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>LONI</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Date</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resource</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Queue Time
-Nimbus</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>n/a</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Poseidon </t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>TG</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nimbus Number Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>EC2</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>EC2 Number Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Jobs</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>n/a</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Average</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stddev</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time-to-Completion (in s)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>m1.large</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Average</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Startup Time (in s)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Memory (in MB)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Instances</t>
-  </si>
-  <si>
-    <t>Daten</t>
   </si>
 </sst>
 </file>
@@ -856,10 +880,10 @@
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>('Setup Times'!$D$27,'Setup Times'!$D$49,'Setup Times'!$D$76)</c:f>
+                <c:f>('Setup Times'!$D$27,'Setup Times'!$D$49,'Setup Times'!$D$75,'Setup Times'!$I$75,'Setup Times'!$D$86)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
+                  <c:ptCount val="5"/>
                   <c:pt idx="0">
                     <c:v>206.4680035082333</c:v>
                   </c:pt>
@@ -869,15 +893,21 @@
                   <c:pt idx="2">
                     <c:v>143.9351872602122</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>22.86065415500533</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.629955639676583</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>('Setup Times'!$D$27,'Setup Times'!$D$49,'Setup Times'!$D$76)</c:f>
+                <c:f>('Setup Times'!$D$27,'Setup Times'!$D$49,'Setup Times'!$D$75,'Setup Times'!$I$75,'Setup Times'!$D$86)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
+                  <c:ptCount val="5"/>
                   <c:pt idx="0">
                     <c:v>206.4680035082333</c:v>
                   </c:pt>
@@ -887,15 +917,21 @@
                   <c:pt idx="2">
                     <c:v>143.9351872602122</c:v>
                   </c:pt>
+                  <c:pt idx="3">
+                    <c:v>22.86065415500533</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.629955639676583</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:minus>
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>('Setup Times'!$E$26,'Setup Times'!$E$48,'Setup Times'!$E$75)</c:f>
+              <c:f>('Setup Times'!$E$26,'Setup Times'!$E$48,'Setup Times'!$E$74,'Setup Times'!$J$74,'Setup Times'!$E$85)</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>EC2 m1.large</c:v>
                 </c:pt>
@@ -903,17 +939,23 @@
                   <c:v>Nimbus</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Poseidon</c:v>
+                  <c:v>Poseidon (Grid)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Poseidon (Grid - adjusted)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Poseidon (Condor)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Setup Times'!$D$26,'Setup Times'!$D$48,'Setup Times'!$D$75)</c:f>
+              <c:f>('Setup Times'!$D$26,'Setup Times'!$D$48,'Setup Times'!$D$74,'Setup Times'!$I$74,'Setup Times'!$D$85)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>373.44653231865</c:v>
                 </c:pt>
@@ -923,15 +965,21 @@
                 <c:pt idx="2">
                   <c:v>117.073104536535</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>53.00379177929375</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>331.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="645061624"/>
-        <c:axId val="645066472"/>
+        <c:axId val="664477800"/>
+        <c:axId val="664479336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="645061624"/>
+        <c:axId val="664477800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -947,14 +995,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="645066472"/>
+        <c:crossAx val="664479336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="645066472"/>
+        <c:axId val="664479336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -983,6 +1031,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -999,7 +1048,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="645061624"/>
+        <c:crossAx val="664477800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1075,11 +1124,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="644520504"/>
-        <c:axId val="644524008"/>
+        <c:axId val="664596600"/>
+        <c:axId val="664587624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="644520504"/>
+        <c:axId val="664596600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1095,14 +1144,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="644524008"/>
+        <c:crossAx val="664587624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="644524008"/>
+        <c:axId val="664587624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1124,6 +1173,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -1137,7 +1187,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="644520504"/>
+        <c:crossAx val="664596600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1168,7 +1218,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -1281,6 +1331,56 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.816388888888" refreshedVersion="3" recordCount="16">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A30:D46" sheet="Setup Times"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Instance" numFmtId="0">
+      <sharedItems count="2">
+        <s v="2 cores"/>
+        <s v="2 core"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Number Instances" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="3">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="4"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Number Cores" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="8" count="3">
+        <n v="2"/>
+        <n v="4"/>
+        <n v="8"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Startup Time (in s)" numFmtId="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="276.08450388900002" maxValue="472.14579200700001" count="16">
+        <n v="313.49457287799999"/>
+        <n v="295.03079795000002"/>
+        <n v="276.08450388900002"/>
+        <n v="314.97212505300001"/>
+        <n v="315.11944603900002"/>
+        <n v="305.19036102299998"/>
+        <n v="365.65275192299998"/>
+        <n v="472.14579200700001"/>
+        <n v="397.81742381999999"/>
+        <n v="376.035724878"/>
+        <n v="372.41291689899998"/>
+        <n v="373.65681600599999"/>
+        <n v="362.95128488500001"/>
+        <n v="376.37267208100002"/>
+        <n v="361.68812417999999"/>
+        <n v="381.790049076"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.819236111114" refreshedVersion="3" recordCount="20">
   <cacheSource type="worksheet">
     <worksheetSource ref="A53:E73" sheet="Setup Times"/>
@@ -1358,56 +1458,6 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.816388888888" refreshedVersion="3" recordCount="16">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A30:D46" sheet="Setup Times"/>
-  </cacheSource>
-  <cacheFields count="4">
-    <cacheField name="Instance" numFmtId="0">
-      <sharedItems count="2">
-        <s v="2 cores"/>
-        <s v="2 core"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Number Instances" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="3">
-        <n v="1"/>
-        <n v="2"/>
-        <n v="4"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Number Cores" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="8" count="3">
-        <n v="2"/>
-        <n v="4"/>
-        <n v="8"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Startup Time (in s)" numFmtId="3">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="276.08450388900002" maxValue="472.14579200700001" count="16">
-        <n v="313.49457287799999"/>
-        <n v="295.03079795000002"/>
-        <n v="276.08450388900002"/>
-        <n v="314.97212505300001"/>
-        <n v="315.11944603900002"/>
-        <n v="305.19036102299998"/>
-        <n v="365.65275192299998"/>
-        <n v="472.14579200700001"/>
-        <n v="397.81742381999999"/>
-        <n v="376.035724878"/>
-        <n v="372.41291689899998"/>
-        <n v="373.65681600599999"/>
-        <n v="362.95128488500001"/>
-        <n v="376.37267208100002"/>
-        <n v="361.68812417999999"/>
-        <n v="381.790049076"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-</pivotCacheDefinition>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38662.629386574074" refreshedVersion="3" recordCount="39">
   <cacheSource type="worksheet">
@@ -1572,247 +1622,247 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="20">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="16">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="9"/>
+  </r>
+  <r>
     <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="10"/>
+  </r>
+  <r>
     <x v="1"/>
     <x v="2"/>
     <x v="2"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="4"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="5"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="6"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="7"/>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="8"/>
-    <x v="8"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="9"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="10"/>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
     <x v="11"/>
-    <x v="11"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="12"/>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="13"/>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="14"/>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
     <x v="15"/>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="16"/>
-    <x v="16"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="17"/>
-    <x v="17"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="18"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="19"/>
-    <x v="19"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="16">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="4"/>
-  </r>
-  <r>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="20">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
     <x v="0"/>
     <x v="1"/>
     <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="5"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <x v="6"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <x v="7"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <x v="8"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
     <x v="2"/>
     <x v="9"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="10"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="11"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="12"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="13"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="14"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="15"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="16"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="17"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="18"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="19"/>
+    <x v="19"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -2135,7 +2185,75 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="G53:I63" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="5">
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" numFmtId="3" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Mittelwert - Startup Time (in s)" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - Startup Time (in s)" fld="3" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="G30:J44" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="4">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
@@ -2217,74 +2335,6 @@
   </colItems>
   <dataFields count="2">
     <dataField name="Mittelwert - Startup Time (in s)2" fld="3" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="STABW - Startup Time (in s)" fld="3" subtotal="stdDev" baseField="0" baseItem="0"/>
-  </dataFields>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="G53:I63" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
-  <pivotFields count="5">
-    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" numFmtId="3" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="10">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Mittelwert - Startup Time (in s)" fld="3" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="STABW - Startup Time (in s)" fld="3" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
 </pivotTableDefinition>
@@ -2794,7 +2844,7 @@
   <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="A23" sqref="A23:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2809,12 +2859,12 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>128</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -2822,36 +2872,36 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="39">
       <c r="A4" s="3" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>63</v>
+        <v>130</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>64</v>
+        <v>131</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>124</v>
+        <v>60</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>53</v>
+        <v>120</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>54</v>
+        <v>121</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2871,7 +2921,7 @@
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -2891,7 +2941,7 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -2911,7 +2961,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2931,7 +2981,7 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -2951,7 +3001,7 @@
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -2971,7 +3021,7 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2991,7 +3041,7 @@
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -3011,7 +3061,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -3031,7 +3081,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3051,7 +3101,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3071,7 +3121,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -3091,7 +3141,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3111,7 +3161,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -3131,7 +3181,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -3151,7 +3201,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -3171,7 +3221,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>43</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3202,7 +3252,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>43</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3233,7 +3283,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>43</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -3264,7 +3314,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -3287,7 +3337,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -3310,7 +3360,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -3331,7 +3381,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -3352,7 +3402,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -3373,7 +3423,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -3394,7 +3444,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -3415,7 +3465,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -3436,7 +3486,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -3457,7 +3507,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -3478,7 +3528,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="B34">
         <v>8</v>
@@ -3499,7 +3549,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="B35">
         <v>8</v>
@@ -3520,7 +3570,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -3541,7 +3591,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -3562,7 +3612,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="44" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="B38" s="44">
         <v>2</v>
@@ -3583,7 +3633,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -3604,7 +3654,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -3625,7 +3675,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -3646,7 +3696,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -3667,7 +3717,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -3688,7 +3738,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -3709,7 +3759,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -3730,7 +3780,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -3761,7 +3811,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -3792,7 +3842,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -3813,7 +3863,7 @@
     </row>
     <row r="49" spans="1:8" s="41" customFormat="1">
       <c r="A49" s="41" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B49" s="41">
         <v>2</v>
@@ -3834,7 +3884,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="39" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B50" s="39">
         <v>4</v>
@@ -3855,7 +3905,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -3876,7 +3926,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -3897,7 +3947,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -3918,7 +3968,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -3939,7 +3989,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -3960,7 +4010,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -3981,7 +4031,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -4002,7 +4052,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -4023,7 +4073,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="B59">
         <v>15</v>
@@ -4044,7 +4094,7 @@
     </row>
     <row r="60" spans="1:8" hidden="1">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -4065,7 +4115,7 @@
     </row>
     <row r="61" spans="1:8" hidden="1">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -4077,7 +4127,7 @@
     </row>
     <row r="62" spans="1:8" hidden="1">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -4089,7 +4139,7 @@
     </row>
     <row r="63" spans="1:8" hidden="1">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -4101,7 +4151,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -4122,7 +4172,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -4143,7 +4193,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -4174,7 +4224,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -4205,7 +4255,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -4236,7 +4286,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -4259,7 +4309,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -4282,7 +4332,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -4305,7 +4355,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -4328,7 +4378,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -4351,7 +4401,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -4374,7 +4424,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B75">
         <v>8</v>
@@ -4397,7 +4447,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B76">
         <v>8</v>
@@ -4420,7 +4470,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B77">
         <v>16</v>
@@ -4443,7 +4493,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B78">
         <v>16</v>
@@ -4466,7 +4516,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B79">
         <v>16</v>
@@ -4489,7 +4539,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B80">
         <v>16</v>
@@ -4512,7 +4562,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B81">
         <v>16</v>
@@ -4535,7 +4585,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B82">
         <v>16</v>
@@ -4558,7 +4608,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="B83">
         <v>16</v>
@@ -4581,7 +4631,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -4601,7 +4651,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -4621,7 +4671,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -4641,7 +4691,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -4661,7 +4711,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -4681,7 +4731,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -4701,7 +4751,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -4721,7 +4771,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -4741,7 +4791,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -4761,7 +4811,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="B93">
         <v>4</v>
@@ -4781,7 +4831,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="B94">
         <v>4</v>
@@ -4801,7 +4851,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>69</v>
+        <v>6</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -4823,6 +4873,7 @@
       <c r="A98" s="1"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -4836,10 +4887,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J88"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4854,45 +4905,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="26" t="s">
-        <v>58</v>
+        <v>125</v>
       </c>
       <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>74</v>
-      </c>
       <c r="E5" s="6" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>126</v>
+        <v>62</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4907,7 +4958,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="I6" s="17">
         <v>221.43898490266665</v>
@@ -4915,7 +4966,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4931,7 +4982,7 @@
       </c>
       <c r="G7" s="32"/>
       <c r="H7" s="18" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="I7" s="21">
         <v>27.888301147358074</v>
@@ -4939,7 +4990,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -4955,7 +5006,7 @@
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="18" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="I8" s="21">
         <v>6</v>
@@ -4963,7 +5014,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -4981,7 +5032,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="I9" s="17">
         <v>230.1513251065</v>
@@ -4989,7 +5040,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5005,7 +5056,7 @@
       </c>
       <c r="G10" s="32"/>
       <c r="H10" s="18" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="I10" s="21">
         <v>21.442701960879447</v>
@@ -5013,7 +5064,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5029,7 +5080,7 @@
       </c>
       <c r="G11" s="32"/>
       <c r="H11" s="18" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="I11" s="21">
         <v>4</v>
@@ -5037,7 +5088,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -5055,7 +5106,7 @@
         <v>8</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="I12" s="17">
         <v>524.47522211100011</v>
@@ -5063,7 +5114,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -5079,7 +5130,7 @@
       </c>
       <c r="G13" s="32"/>
       <c r="H13" s="18" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="I13" s="21">
         <v>249.37176975472715</v>
@@ -5087,7 +5138,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -5103,7 +5154,7 @@
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="18" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="I14" s="21">
         <v>32</v>
@@ -5111,7 +5162,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -5129,7 +5180,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="I15" s="17">
         <v>338.08045351500004</v>
@@ -5137,7 +5188,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -5153,7 +5204,7 @@
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="18" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="I16" s="21">
         <v>46.784586737362908</v>
@@ -5161,7 +5212,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -5177,7 +5228,7 @@
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="18" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="I17" s="21">
         <v>16</v>
@@ -5185,7 +5236,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -5200,7 +5251,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="H18" s="33"/>
       <c r="I18" s="17">
@@ -5209,7 +5260,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -5224,7 +5275,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="H19" s="33"/>
       <c r="I19" s="17">
@@ -5233,7 +5284,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -5248,7 +5299,7 @@
         <v>0.75</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="H20" s="34"/>
       <c r="I20" s="25">
@@ -5257,7 +5308,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -5274,7 +5325,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -5291,7 +5342,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -5308,7 +5359,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -5325,7 +5376,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>92</v>
       </c>
       <c r="B25">
         <v>16</v>
@@ -5342,19 +5393,19 @@
     </row>
     <row r="26" spans="1:10">
       <c r="C26" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="D26" s="2">
         <f>AVERAGE(D6:D25)</f>
         <v>373.44653231864999</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="C27" t="s">
-        <v>117</v>
+        <v>53</v>
       </c>
       <c r="D27" s="2">
         <f>STDEV(D6:D25)</f>
@@ -5364,42 +5415,42 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="26" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="B29" s="26"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>82</v>
+        <v>19</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>102</v>
+        <v>39</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>125</v>
+        <v>61</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>126</v>
+        <v>62</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -5417,7 +5468,7 @@
         <v>2</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="J31" s="17">
         <v>302.94028916180002</v>
@@ -5425,7 +5476,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -5442,7 +5493,7 @@
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
       <c r="I32" s="18" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="J32" s="21">
         <v>17.23574117758357</v>
@@ -5450,7 +5501,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -5465,7 +5516,7 @@
         <v>0.5625</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="H33" s="33"/>
       <c r="I33" s="33"/>
@@ -5475,7 +5526,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -5490,7 +5541,7 @@
         <v>0.89513888888888893</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -5500,7 +5551,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5521,7 +5572,7 @@
         <v>4</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="J35" s="17">
         <v>305.19036102299998</v>
@@ -5529,7 +5580,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -5547,7 +5598,7 @@
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
       <c r="I36" s="18" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="J36" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5555,7 +5606,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>126</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -5571,7 +5622,7 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="H37" s="33"/>
       <c r="I37" s="33"/>
@@ -5581,7 +5632,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -5597,7 +5648,7 @@
         <v>0.57916666666666672</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="H38" s="33"/>
       <c r="I38" s="33"/>
@@ -5607,7 +5658,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -5629,7 +5680,7 @@
         <v>8</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="J39" s="17">
         <v>384.05235557549997</v>
@@ -5637,7 +5688,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -5655,7 +5706,7 @@
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
       <c r="I40" s="18" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="J40" s="21">
         <v>32.66972061151673</v>
@@ -5663,7 +5714,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -5679,7 +5730,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="33"/>
@@ -5689,7 +5740,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -5704,7 +5755,7 @@
         <v>0.70972222222222225</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="H42" s="33"/>
       <c r="I42" s="33"/>
@@ -5714,7 +5765,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -5729,7 +5780,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
@@ -5739,7 +5790,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -5754,7 +5805,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -5764,7 +5815,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -5781,7 +5832,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -5798,7 +5849,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -5813,19 +5864,19 @@
     </row>
     <row r="48" spans="1:10">
       <c r="C48" t="s">
-        <v>116</v>
+        <v>52</v>
       </c>
       <c r="D48" s="2">
         <f>AVERAGE(D30:D47)</f>
         <v>356.83130192700003</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="C49" t="s">
-        <v>117</v>
+        <v>53</v>
       </c>
       <c r="D49" s="2">
         <f>STDEV(D31:D47)</f>
@@ -5842,37 +5893,40 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="26" t="s">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="B52" s="26"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="26" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>104</v>
+        <v>40</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>102</v>
+        <v>39</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>126</v>
+        <v>62</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>0</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>101</v>
+        <v>38</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -5880,8 +5934,8 @@
       <c r="C54">
         <v>8</v>
       </c>
-      <c r="D54" s="6" t="s">
-        <v>122</v>
+      <c r="D54" s="2">
+        <v>24.626098156000001</v>
       </c>
       <c r="E54" s="7">
         <v>0.89513888888888893</v>
@@ -5890,7 +5944,7 @@
         <v>4</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="I54" s="17">
         <v>14.1872649193</v>
@@ -5898,7 +5952,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>101</v>
+        <v>38</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -5907,14 +5961,14 @@
         <v>8</v>
       </c>
       <c r="D55" s="2">
-        <v>24.626098156000001</v>
+        <v>44.588248014500003</v>
       </c>
       <c r="E55" s="7">
         <v>0.90208333333333324</v>
       </c>
       <c r="G55" s="32"/>
       <c r="H55" s="18" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="I55" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5922,7 +5976,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>101</v>
+        <v>38</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -5931,7 +5985,7 @@
         <v>4</v>
       </c>
       <c r="D56" s="2">
-        <v>44.588248014500003</v>
+        <v>14.1872649193</v>
       </c>
       <c r="E56" s="7">
         <v>0.90972222222222221</v>
@@ -5940,7 +5994,7 @@
         <v>8</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="I56" s="17">
         <v>44.782275199920001</v>
@@ -5948,7 +6002,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -5957,14 +6011,14 @@
         <v>8</v>
       </c>
       <c r="D57" s="2">
-        <v>14.1872649193</v>
+        <v>35.098526954699999</v>
       </c>
       <c r="E57" s="7">
         <v>0.93125000000000002</v>
       </c>
       <c r="G57" s="32"/>
       <c r="H57" s="18" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="I57" s="21">
         <v>15.843792242505828</v>
@@ -5972,7 +6026,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -5981,7 +6035,7 @@
         <v>8</v>
       </c>
       <c r="D58" s="2">
-        <v>35.098526954699999</v>
+        <v>64.947054863000005</v>
       </c>
       <c r="E58" s="7">
         <v>0.93888888888888899</v>
@@ -5990,7 +6044,7 @@
         <v>16</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="I58" s="17">
         <v>56.964924156674996</v>
@@ -5998,7 +6052,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -6007,14 +6061,14 @@
         <v>8</v>
       </c>
       <c r="D59" s="2">
-        <v>64.947054863000005</v>
+        <v>54.651448011399999</v>
       </c>
       <c r="E59" s="7">
         <v>0.95000000000000007</v>
       </c>
       <c r="G59" s="32"/>
       <c r="H59" s="18" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="I59" s="21">
         <v>9.4994883808250847</v>
@@ -6022,7 +6076,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -6031,7 +6085,7 @@
         <v>16</v>
       </c>
       <c r="D60" s="2">
-        <v>54.651448011399999</v>
+        <v>55.051728963899997</v>
       </c>
       <c r="E60" s="7">
         <v>0.96527777777777779</v>
@@ -6040,7 +6094,7 @@
         <v>32</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="I60" s="17">
         <v>187.55037531850999</v>
@@ -6048,7 +6102,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -6057,14 +6111,14 @@
         <v>16</v>
       </c>
       <c r="D61" s="2">
-        <v>55.051728963899997</v>
+        <v>50.9480149746</v>
       </c>
       <c r="E61" s="7">
         <v>0.58402777777777781</v>
       </c>
       <c r="G61" s="32"/>
       <c r="H61" s="18" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="I61" s="21">
         <v>179.97433590633514</v>
@@ -6072,7 +6126,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -6081,13 +6135,13 @@
         <v>16</v>
       </c>
       <c r="D62" s="2">
-        <v>50.9480149746</v>
+        <v>70.915316820100003</v>
       </c>
       <c r="E62" s="7">
         <v>0.59236111111111112</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="H62" s="33"/>
       <c r="I62" s="17">
@@ -6096,7 +6150,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -6105,13 +6159,13 @@
         <v>16</v>
       </c>
       <c r="D63" s="2">
-        <v>70.915316820100003</v>
+        <v>50.944635868100001</v>
       </c>
       <c r="E63" s="7">
         <v>0.61875000000000002</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="H63" s="34"/>
       <c r="I63" s="25">
@@ -6120,7 +6174,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B64">
         <v>8</v>
@@ -6129,15 +6183,15 @@
         <v>32</v>
       </c>
       <c r="D64" s="2">
-        <v>50.944635868100001</v>
+        <v>266.05073404299998</v>
       </c>
       <c r="E64" s="7">
         <v>0.625</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -6146,15 +6200,15 @@
         <v>32</v>
       </c>
       <c r="D65" s="2">
-        <v>266.05073404299998</v>
+        <v>35.081162929500003</v>
       </c>
       <c r="E65" s="7">
         <v>0.67013888888888884</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -6163,15 +6217,15 @@
         <v>32</v>
       </c>
       <c r="D66" s="2">
-        <v>35.081162929500003</v>
+        <v>24.897548914000001</v>
       </c>
       <c r="E66" s="7">
         <v>0.71388888888888891</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B67">
         <v>8</v>
@@ -6180,15 +6234,15 @@
         <v>32</v>
       </c>
       <c r="D67" s="2">
-        <v>24.897548914000001</v>
+        <v>325.77829599400002</v>
       </c>
       <c r="E67" s="7">
         <v>0.73749999999999993</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B68">
         <v>8</v>
@@ -6197,15 +6251,15 @@
         <v>32</v>
       </c>
       <c r="D68" s="2">
-        <v>325.77829599400002</v>
+        <v>75.1672639847</v>
       </c>
       <c r="E68" s="7">
         <v>0.75</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -6214,15 +6268,15 @@
         <v>32</v>
       </c>
       <c r="D69" s="2">
-        <v>75.1672639847</v>
+        <v>65.186727047000005</v>
       </c>
       <c r="E69" s="7">
         <v>0.76388888888888884</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B70">
         <v>8</v>
@@ -6231,15 +6285,15 @@
         <v>32</v>
       </c>
       <c r="D70" s="2">
-        <v>65.186727047000005</v>
+        <v>86.636376142499998</v>
       </c>
       <c r="E70" s="7">
         <v>0.7715277777777777</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -6248,15 +6302,15 @@
         <v>32</v>
       </c>
       <c r="D71" s="2">
-        <v>86.636376142499998</v>
+        <v>576.54629802700003</v>
       </c>
       <c r="E71" s="7">
         <v>0.78819444444444453</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -6265,15 +6319,15 @@
         <v>32</v>
       </c>
       <c r="D72" s="2">
-        <v>576.54629802700003</v>
+        <v>325.02609419800001</v>
       </c>
       <c r="E72" s="7">
         <v>0.8125</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -6282,52 +6336,153 @@
         <v>32</v>
       </c>
       <c r="D73" s="2">
-        <v>325.02609419800001</v>
+        <v>95.133251905400002</v>
       </c>
       <c r="E73" s="7"/>
     </row>
-    <row r="74" spans="1:5">
-      <c r="A74" t="s">
-        <v>7</v>
-      </c>
-      <c r="B74">
+    <row r="74" spans="1:10">
+      <c r="C74" t="s">
+        <v>57</v>
+      </c>
+      <c r="D74" s="2">
+        <f>AVERAGE(D54:D73)</f>
+        <v>117.073104536535</v>
+      </c>
+      <c r="E74" t="s">
         <v>2</v>
       </c>
-      <c r="C74">
-        <v>4</v>
-      </c>
-      <c r="D74" s="2">
-        <v>95.133251905400002</v>
-      </c>
-      <c r="E74" s="7"/>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="H74" t="s">
+        <v>0</v>
+      </c>
+      <c r="I74" s="55">
+        <f>AVERAGE(D54:D63,D65:D66,D68:D70,D73)</f>
+        <v>53.003791779293749</v>
+      </c>
+      <c r="J74" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="C75" t="s">
-        <v>121</v>
+        <v>53</v>
       </c>
       <c r="D75" s="2">
-        <f>AVERAGE(D55:D74)</f>
-        <v>117.073104536535</v>
-      </c>
-      <c r="E75" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="C76" t="s">
-        <v>117</v>
-      </c>
-      <c r="D76" s="2">
-        <f>STDEV(D55:D74)</f>
+        <f>STDEV(D54:D73)</f>
         <v>143.93518726021225</v>
       </c>
-    </row>
-    <row r="88" spans="8:8">
-      <c r="H88" s="2"/>
+      <c r="H75" t="s">
+        <v>67</v>
+      </c>
+      <c r="I75" s="55">
+        <f>STDEV(D54:D63,D65:D66,D68:D70,D73)</f>
+        <v>22.860654155005328</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="D76" s="55"/>
+      <c r="I76" s="55"/>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="D77" s="55"/>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B80" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C80" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" t="s">
+        <v>38</v>
+      </c>
+      <c r="B81">
+        <v>2</v>
+      </c>
+      <c r="C81">
+        <v>8</v>
+      </c>
+      <c r="D81">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" t="s">
+        <v>65</v>
+      </c>
+      <c r="B82">
+        <v>4</v>
+      </c>
+      <c r="C82">
+        <v>8</v>
+      </c>
+      <c r="D82">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" t="s">
+        <v>38</v>
+      </c>
+      <c r="B83">
+        <v>8</v>
+      </c>
+      <c r="C83">
+        <v>4</v>
+      </c>
+      <c r="D83">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" t="s">
+        <v>36</v>
+      </c>
+      <c r="B84">
+        <v>16</v>
+      </c>
+      <c r="C84">
+        <v>8</v>
+      </c>
+      <c r="D84">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="D85">
+        <f>AVERAGE(D81:D84)</f>
+        <v>331.25</v>
+      </c>
+      <c r="E85" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="D86" s="55">
+        <f>STDEV(D81:D84)</f>
+        <v>2.6299556396765835</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="H89" s="2"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId4"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -6343,7 +6498,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -6359,69 +6514,69 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="28" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="30" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" ht="39" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>109</v>
+        <v>45</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>111</v>
+        <v>47</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>112</v>
+        <v>48</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>113</v>
+        <v>49</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>114</v>
+        <v>50</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>50</v>
+        <v>117</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>118</v>
+        <v>54</v>
       </c>
       <c r="K5" s="28" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="M5" s="28" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>115</v>
+        <v>51</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -6456,13 +6611,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -6497,13 +6652,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="B8" s="31">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>51</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -6538,7 +6693,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -6576,7 +6731,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -6611,7 +6766,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B11">
         <v>32</v>
@@ -6652,7 +6807,7 @@
     </row>
     <row r="12" spans="1:14" s="49" customFormat="1" ht="14" thickBot="1">
       <c r="A12" s="49" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B12" s="49">
         <v>32</v>
@@ -6693,7 +6848,7 @@
     </row>
     <row r="13" spans="1:14" ht="40" thickTop="1">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -6724,12 +6879,12 @@
         <v>2</v>
       </c>
       <c r="N13" s="52" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="39">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -6760,12 +6915,12 @@
         <v>2</v>
       </c>
       <c r="N14" s="52" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="39">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="B15" s="41">
         <v>16</v>
@@ -6796,12 +6951,12 @@
         <v>1</v>
       </c>
       <c r="N15" s="52" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="39">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -6832,12 +6987,12 @@
         <v>0</v>
       </c>
       <c r="N16" s="52" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B17">
         <v>32</v>
@@ -6870,7 +7025,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B18">
         <v>32</v>
@@ -6903,7 +7058,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B19">
         <v>32</v>
@@ -6958,8 +7113,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9:H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="A6:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -6969,50 +7124,50 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="53" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="54" customFormat="1" ht="39">
       <c r="A5" s="54" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>40</v>
+        <v>107</v>
       </c>
       <c r="E5" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="F5" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="I5" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="J5" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="K5" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="L5" s="54" t="s">
         <v>41</v>
-      </c>
-      <c r="F5" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="54" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" s="54" t="s">
-        <v>46</v>
-      </c>
-      <c r="K5" s="54" t="s">
-        <v>47</v>
-      </c>
-      <c r="L5" s="54" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -7051,7 +7206,7 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -7162,7 +7317,7 @@
         <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -7201,7 +7356,7 @@
         <v>3</v>
       </c>
       <c r="L10" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -7480,10 +7635,10 @@
   <sheetData>
     <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -7495,7 +7650,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="11" t="s">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
@@ -7519,12 +7674,12 @@
         <v>32</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>93</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
@@ -7541,7 +7696,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="18" t="s">
-        <v>95</v>
+        <v>32</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="20">
@@ -7558,7 +7713,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="18" t="s">
-        <v>69</v>
+        <v>6</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
@@ -7579,7 +7734,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="18" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="B8" s="19">
         <v>2070.8984270000001</v>
@@ -7596,7 +7751,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="B9" s="19">
         <v>1095.4940549999999</v>
@@ -7623,7 +7778,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="18" t="s">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
@@ -7644,7 +7799,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="18" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -7665,7 +7820,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="22" t="s">
-        <v>93</v>
+        <v>30</v>
       </c>
       <c r="B12" s="23">
         <v>1583.1962410000001</v>
@@ -7693,6 +7848,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Performance Sections renamed in BigJob Overheads and refined Small changes here and there
git-svn-id: file://localhost/tmp/svn2git/svn@1916 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="35740" windowHeight="22200" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="-200" windowWidth="35980" windowHeight="21780" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NAMD Runtimes" sheetId="1" r:id="rId1"/>
     <sheet name="Setup Times" sheetId="3" r:id="rId2"/>
     <sheet name="Adaptive" sheetId="7" r:id="rId3"/>
-    <sheet name="Deadline" sheetId="8" r:id="rId4"/>
-    <sheet name="Pivot" sheetId="4" r:id="rId5"/>
+    <sheet name="Fixed" sheetId="9" r:id="rId4"/>
+    <sheet name="Deadline" sheetId="8" r:id="rId5"/>
+    <sheet name="Pivot" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="130404" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
-    <pivotCache cacheId="2" r:id="rId7"/>
-    <pivotCache cacheId="1" r:id="rId8"/>
-    <pivotCache cacheId="3" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="2" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
+    <pivotCache cacheId="3" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -29,114 +30,379 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="144">
+  <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Condor Ressourcen</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Condor Number Cores</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Job Size</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixed</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Runtime (in sec)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon (CHARM)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 core</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Cores</t>
+  </si>
+  <si>
+    <t>Number Cores</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nodes</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Cores</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>m1.large</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 STABW - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>2 STABW - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>4 STABW - Startup Time (in s)</t>
+  </si>
+  <si>
+    <t>1 Mittelwert - Startup Time (in s)2</t>
+  </si>
+  <si>
+    <t>2 Mittelwert - Startup Time (in s)2</t>
+  </si>
+  <si>
+    <t>4 Mittelwert - Startup Time (in s)2</t>
+  </si>
+  <si>
+    <t>Summe - Number Instances</t>
+  </si>
+  <si>
+    <t>Gesamt: Summe - Number Instances</t>
+  </si>
+  <si>
+    <t>Cores</t>
+  </si>
+  <si>
+    <t>m1.large</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adaptive Scenario</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time for completion for n jobs</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jobs run as soon as a resource becomes available</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t># TG</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t># Nimbus</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t># EC2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC2 m1.large</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nimbus</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI 16 core
+Nimbus 16 core</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Run ID</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Replicas</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAX_RUNTIME (in min)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Check Period (in min)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max Cloud Pilots</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cloud Pilot Size</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Runtime (in min)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Runtime (in sec)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t># Nimbus</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t># Poseidon</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t># Cloud Pilots</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start Pilot if not sufficient progress is made</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deadline Scenario</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Job Size Cloud (in Cores)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Job Size TG (in Cores)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>n/a</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>SAGA Pilot Sub-Job Runtime</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overhead (in s)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overhead (in %)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 cores</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nimbus</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon </t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 cores</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>EUCA (Indiana)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Number Steps: </t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAMD Run</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Nodes</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Cores (Total)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>EC2 (m1.large)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Runs a Workload of 8 replicas in a fixed distribution</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t># TG</t>
+  </si>
+  <si>
+    <t># Nimbus</t>
+  </si>
+  <si>
+    <t># Condor</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number Cores</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
   <si>
     <t>Average (drop maxima)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon (Grid - adjusted)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon (Grid)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Machine</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Nimbus (Chicago)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>EC2 (c1.xlarge)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>EC2 (m2.4xlarge)</t>
   </si>
   <si>
     <t>EC2 (m2.4xlarge)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>EC2 (m2.4xlarge)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Walltime (in sec)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Startup Times</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Startup Time (in s)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Instance</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>m1.large</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Number Instances</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>2 cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>LONI 8 core
 Nimbus 8 core</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>LONI 8 core 
 Nimbus 16 core</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>LONI 16 core
 Nimbus 8 core</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Startup Time (in s)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Instance</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Date</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>m1.large</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>QB (MPI)</t>
   </si>
   <si>
     <t>QB (MPI)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>QB (CHARM)</t>
   </si>
   <si>
     <t>QB (CHARM)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Mittelwert - Walltime (in sec)</t>
@@ -164,108 +430,108 @@
   </si>
   <si>
     <t>CPU Time (in sec)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>LONI</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Date</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Queue Time
 Nimbus</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>n/a</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Poseidon </t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>TG</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Nimbus Number Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Number Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>EC2</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>EC2 Number Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Number Jobs</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>n/a</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Average</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Stddev</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Time-to-Completion (in s)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>m1.large</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>2 cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Average</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Startup Time (in s)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Memory (in MB)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Number Instances</t>
@@ -275,23 +541,23 @@
   </si>
   <si>
     <t>LONI/Condor</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Resource</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Oliver</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon (Condor)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Stdev (drop maxima)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
+    <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
     <t>Ergebnis</t>
@@ -313,229 +579,6 @@
   </si>
   <si>
     <t>Gesamt: Mittelwert - Startup Time (in s)2</t>
-  </si>
-  <si>
-    <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poseidon (CHARM)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 core</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Cores</t>
-  </si>
-  <si>
-    <t>Number Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nodes</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>m1.large</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 STABW - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>2 STABW - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>4 STABW - Startup Time (in s)</t>
-  </si>
-  <si>
-    <t>1 Mittelwert - Startup Time (in s)2</t>
-  </si>
-  <si>
-    <t>2 Mittelwert - Startup Time (in s)2</t>
-  </si>
-  <si>
-    <t>4 Mittelwert - Startup Time (in s)2</t>
-  </si>
-  <si>
-    <t>Summe - Number Instances</t>
-  </si>
-  <si>
-    <t>Gesamt: Summe - Number Instances</t>
-  </si>
-  <si>
-    <t>Cores</t>
-  </si>
-  <si>
-    <t>m1.large</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Adaptive Scenario</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time for completion for n jobs</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jobs run as soon as a resource becomes available</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># TG</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># Nimbus</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># EC2</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Average</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>EC2 m1.large</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nimbus</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>LONI 16 core
-Nimbus 16 core</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Run ID</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Replicas</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>MAX_RUNTIME (in min)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Check Period (in min)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Max Cloud Pilots</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cloud Pilot Size</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Runtime (in min)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Runtime (in sec)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># Nimbus</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># Poseidon</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># Cloud Pilots</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Start Pilot if not sufficient progress is made</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deadline Scenario</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Job Size Cloud (in Cores)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Job Size TG (in Cores)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>n/a</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>SAGA Pilot Sub-Job Runtime</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overhead (in s)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overhead (in %)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Nimbus</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Amazon </t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>2 cores</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>EUCA (Indiana)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Number Steps: </t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>NAMD Run</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Nodes</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number Cores (Total)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>EC2 (m1.large)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -546,8 +589,13 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -779,23 +827,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -814,20 +862,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -847,11 +895,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -880,7 +935,7 @@
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>('Setup Times'!$D$27,'Setup Times'!$D$49,'Setup Times'!$D$75,'Setup Times'!$I$75,'Setup Times'!$D$86)</c:f>
+                <c:f>('Setup Times'!$D$27,'Setup Times'!$D$49,'Setup Times'!$D$75,'Setup Times'!$I$75,'Setup Times'!$D$96)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -897,14 +952,14 @@
                     <c:v>22.86065415500533</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.629955639676583</c:v>
+                    <c:v>1.528124613752805</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>('Setup Times'!$D$27,'Setup Times'!$D$49,'Setup Times'!$D$75,'Setup Times'!$I$75,'Setup Times'!$D$86)</c:f>
+                <c:f>('Setup Times'!$D$27,'Setup Times'!$D$49,'Setup Times'!$D$75,'Setup Times'!$I$75,'Setup Times'!$D$96)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -921,7 +976,7 @@
                     <c:v>22.86065415500533</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.629955639676583</c:v>
+                    <c:v>1.528124613752805</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -929,7 +984,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>('Setup Times'!$E$26,'Setup Times'!$E$48,'Setup Times'!$E$74,'Setup Times'!$J$74,'Setup Times'!$E$85)</c:f>
+              <c:f>('Setup Times'!$E$26,'Setup Times'!$E$48,'Setup Times'!$E$74,'Setup Times'!$J$74,'Setup Times'!$E$95)</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -952,7 +1007,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Setup Times'!$D$26,'Setup Times'!$D$48,'Setup Times'!$D$74,'Setup Times'!$I$74,'Setup Times'!$D$85)</c:f>
+              <c:f>('Setup Times'!$D$26,'Setup Times'!$D$48,'Setup Times'!$D$74,'Setup Times'!$I$74,'Setup Times'!$D$95)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -969,17 +1024,17 @@
                   <c:v>53.00379177929375</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>331.25</c:v>
+                  <c:v>331.2142857142857</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="664477800"/>
-        <c:axId val="664479336"/>
+        <c:axId val="467237992"/>
+        <c:axId val="467248024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="664477800"/>
+        <c:axId val="467237992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -995,14 +1050,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="664479336"/>
+        <c:crossAx val="467248024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="664479336"/>
+        <c:axId val="467248024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1048,7 +1103,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="664477800"/>
+        <c:crossAx val="467237992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1124,11 +1179,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="664596600"/>
-        <c:axId val="664587624"/>
+        <c:axId val="467289880"/>
+        <c:axId val="467280888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="664596600"/>
+        <c:axId val="467289880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1144,14 +1199,14 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="664587624"/>
+        <c:crossAx val="467280888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="664587624"/>
+        <c:axId val="467280888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1187,7 +1242,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="664596600"/>
+        <c:crossAx val="467289880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1246,16 +1301,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>939800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1331,56 +1386,6 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.816388888888" refreshedVersion="3" recordCount="16">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A30:D46" sheet="Setup Times"/>
-  </cacheSource>
-  <cacheFields count="4">
-    <cacheField name="Instance" numFmtId="0">
-      <sharedItems count="2">
-        <s v="2 cores"/>
-        <s v="2 core"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Number Instances" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="3">
-        <n v="1"/>
-        <n v="2"/>
-        <n v="4"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Number Cores" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="8" count="3">
-        <n v="2"/>
-        <n v="4"/>
-        <n v="8"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Startup Time (in s)" numFmtId="3">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="276.08450388900002" maxValue="472.14579200700001" count="16">
-        <n v="313.49457287799999"/>
-        <n v="295.03079795000002"/>
-        <n v="276.08450388900002"/>
-        <n v="314.97212505300001"/>
-        <n v="315.11944603900002"/>
-        <n v="305.19036102299998"/>
-        <n v="365.65275192299998"/>
-        <n v="472.14579200700001"/>
-        <n v="397.81742381999999"/>
-        <n v="376.035724878"/>
-        <n v="372.41291689899998"/>
-        <n v="373.65681600599999"/>
-        <n v="362.95128488500001"/>
-        <n v="376.37267208100002"/>
-        <n v="361.68812417999999"/>
-        <n v="381.790049076"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.819236111114" refreshedVersion="3" recordCount="20">
   <cacheSource type="worksheet">
     <worksheetSource ref="A53:E73" sheet="Setup Times"/>
@@ -1458,6 +1463,56 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38663.816388888888" refreshedVersion="3" recordCount="16">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A30:D46" sheet="Setup Times"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Instance" numFmtId="0">
+      <sharedItems count="2">
+        <s v="2 cores"/>
+        <s v="2 core"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Number Instances" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="3">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="4"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Number Cores" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="8" count="3">
+        <n v="2"/>
+        <n v="4"/>
+        <n v="8"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Startup Time (in s)" numFmtId="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="276.08450388900002" maxValue="472.14579200700001" count="16">
+        <n v="313.49457287799999"/>
+        <n v="295.03079795000002"/>
+        <n v="276.08450388900002"/>
+        <n v="314.97212505300001"/>
+        <n v="315.11944603900002"/>
+        <n v="305.19036102299998"/>
+        <n v="365.65275192299998"/>
+        <n v="472.14579200700001"/>
+        <n v="397.81742381999999"/>
+        <n v="376.035724878"/>
+        <n v="372.41291689899998"/>
+        <n v="373.65681600599999"/>
+        <n v="362.95128488500001"/>
+        <n v="376.37267208100002"/>
+        <n v="361.68812417999999"/>
+        <n v="381.790049076"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Torsten Meier" refreshedDate="38662.629386574074" refreshedVersion="3" recordCount="39">
   <cacheSource type="worksheet">
@@ -1622,6 +1677,151 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="20">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="6"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="7"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="8"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="9"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="10"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="11"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="12"/>
+    <x v="12"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="13"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="14"/>
+    <x v="14"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="15"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="16"/>
+    <x v="16"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="17"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="18"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="19"/>
+    <x v="19"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="16">
   <r>
     <x v="0"/>
@@ -1718,151 +1918,6 @@
     <x v="2"/>
     <x v="2"/>
     <x v="15"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="20">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="3"/>
-    <x v="3"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="4"/>
-    <x v="4"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="5"/>
-    <x v="5"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="6"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="7"/>
-    <x v="7"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="8"/>
-    <x v="8"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="9"/>
-    <x v="9"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="10"/>
-    <x v="10"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="11"/>
-    <x v="11"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="12"/>
-    <x v="12"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="13"/>
-    <x v="13"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="14"/>
-    <x v="14"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="15"/>
-    <x v="15"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="16"/>
-    <x v="16"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="17"/>
-    <x v="17"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="18"/>
-    <x v="18"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="3"/>
-    <x v="19"/>
-    <x v="19"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -2185,75 +2240,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="G53:I63" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
-  <pivotFields count="5">
-    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" numFmtId="3" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
-  </pivotFields>
-  <rowFields count="2">
-    <field x="2"/>
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="10">
-    <i>
-      <x/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Mittelwert - Startup Time (in s)" fld="3" subtotal="average" baseField="0" baseItem="0"/>
-    <dataField name="STABW - Startup Time (in s)" fld="3" subtotal="stdDev" baseField="0" baseItem="0"/>
-  </dataFields>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="G30:J44" firstHeaderRow="1" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="4">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
@@ -2335,6 +2322,74 @@
   </colItems>
   <dataFields count="2">
     <dataField name="Mittelwert - Startup Time (in s)2" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="STABW - Startup Time (in s)" fld="3" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Daten" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="G53:I63" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="5">
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField axis="axisRow" compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" numFmtId="3" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+    <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" includeNewItemsInFilter="1"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+    <i t="grand" i="1">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Mittelwert - Startup Time (in s)" fld="3" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="STABW - Startup Time (in s)" fld="3" subtotal="stdDev" baseField="0" baseItem="0"/>
   </dataFields>
 </pivotTableDefinition>
@@ -2859,12 +2914,12 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>129</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -2872,36 +2927,36 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="39">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>130</v>
+        <v>61</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>131</v>
+        <v>62</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>35</v>
+        <v>104</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>120</v>
+        <v>51</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>121</v>
+        <v>52</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>122</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2921,7 +2976,7 @@
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -2941,7 +2996,7 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -2961,7 +3016,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2981,7 +3036,7 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -3001,7 +3056,7 @@
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -3021,7 +3076,7 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3041,7 +3096,7 @@
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -3061,7 +3116,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -3081,7 +3136,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3101,7 +3156,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3121,7 +3176,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -3141,7 +3196,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3161,7 +3216,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -3181,7 +3236,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -3201,7 +3256,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -3221,7 +3276,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3252,7 +3307,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3283,7 +3338,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -3314,7 +3369,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -3337,7 +3392,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>128</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -3360,7 +3415,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -3381,7 +3436,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -3402,7 +3457,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -3423,7 +3478,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -3444,7 +3499,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -3465,7 +3520,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -3486,7 +3541,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -3507,7 +3562,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -3528,7 +3583,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B34">
         <v>8</v>
@@ -3549,7 +3604,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B35">
         <v>8</v>
@@ -3570,7 +3625,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -3591,7 +3646,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -3612,7 +3667,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="44" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="B38" s="44">
         <v>2</v>
@@ -3633,7 +3688,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -3654,7 +3709,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -3675,7 +3730,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -3696,7 +3751,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -3717,7 +3772,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -3738,7 +3793,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -3759,7 +3814,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -3780,7 +3835,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -3811,7 +3866,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -3842,7 +3897,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -3863,7 +3918,7 @@
     </row>
     <row r="49" spans="1:8" s="41" customFormat="1">
       <c r="A49" s="41" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B49" s="41">
         <v>2</v>
@@ -3884,7 +3939,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="39" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B50" s="39">
         <v>4</v>
@@ -3905,7 +3960,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -3926,7 +3981,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -3947,7 +4002,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -3968,7 +4023,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -3989,7 +4044,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -4010,7 +4065,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -4031,7 +4086,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -4052,7 +4107,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -4073,7 +4128,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B59">
         <v>15</v>
@@ -4094,7 +4149,7 @@
     </row>
     <row r="60" spans="1:8" hidden="1">
       <c r="A60" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -4115,7 +4170,7 @@
     </row>
     <row r="61" spans="1:8" hidden="1">
       <c r="A61" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -4127,7 +4182,7 @@
     </row>
     <row r="62" spans="1:8" hidden="1">
       <c r="A62" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -4139,7 +4194,7 @@
     </row>
     <row r="63" spans="1:8" hidden="1">
       <c r="A63" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -4151,7 +4206,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -4172,7 +4227,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -4193,7 +4248,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -4224,7 +4279,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -4255,7 +4310,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -4286,7 +4341,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -4309,7 +4364,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -4332,7 +4387,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -4355,7 +4410,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -4378,7 +4433,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -4401,7 +4456,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -4424,7 +4479,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B75">
         <v>8</v>
@@ -4447,7 +4502,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B76">
         <v>8</v>
@@ -4470,7 +4525,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B77">
         <v>16</v>
@@ -4493,7 +4548,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B78">
         <v>16</v>
@@ -4516,7 +4571,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B79">
         <v>16</v>
@@ -4539,7 +4594,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B80">
         <v>16</v>
@@ -4562,7 +4617,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B81">
         <v>16</v>
@@ -4585,7 +4640,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B82">
         <v>16</v>
@@ -4608,7 +4663,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B83">
         <v>16</v>
@@ -4631,7 +4686,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -4651,7 +4706,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -4671,7 +4726,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -4691,7 +4746,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -4711,7 +4766,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -4731,7 +4786,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -4751,7 +4806,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -4771,7 +4826,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -4791,7 +4846,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -4811,7 +4866,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="B93">
         <v>4</v>
@@ -4831,7 +4886,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="B94">
         <v>4</v>
@@ -4851,7 +4906,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -4873,8 +4928,7 @@
       <c r="A98" s="1"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -4887,10 +4941,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J89"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="N54" sqref="N54"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4905,45 +4959,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="26" t="s">
-        <v>125</v>
+        <v>56</v>
       </c>
       <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4958,7 +5012,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="I6" s="17">
         <v>221.43898490266665</v>
@@ -4966,7 +5020,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4982,7 +5036,7 @@
       </c>
       <c r="G7" s="32"/>
       <c r="H7" s="18" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="I7" s="21">
         <v>27.888301147358074</v>
@@ -4990,7 +5044,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5006,7 +5060,7 @@
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="18" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="I8" s="21">
         <v>6</v>
@@ -5014,7 +5068,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5032,7 +5086,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="I9" s="17">
         <v>230.1513251065</v>
@@ -5040,7 +5094,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5056,7 +5110,7 @@
       </c>
       <c r="G10" s="32"/>
       <c r="H10" s="18" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="I10" s="21">
         <v>21.442701960879447</v>
@@ -5064,7 +5118,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5080,7 +5134,7 @@
       </c>
       <c r="G11" s="32"/>
       <c r="H11" s="18" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="I11" s="21">
         <v>4</v>
@@ -5088,7 +5142,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -5106,7 +5160,7 @@
         <v>8</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="I12" s="17">
         <v>524.47522211100011</v>
@@ -5114,7 +5168,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -5130,7 +5184,7 @@
       </c>
       <c r="G13" s="32"/>
       <c r="H13" s="18" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="I13" s="21">
         <v>249.37176975472715</v>
@@ -5138,7 +5192,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -5154,7 +5208,7 @@
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="18" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="I14" s="21">
         <v>32</v>
@@ -5162,7 +5216,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -5180,7 +5234,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="I15" s="17">
         <v>338.08045351500004</v>
@@ -5188,7 +5242,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -5204,7 +5258,7 @@
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="18" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="I16" s="21">
         <v>46.784586737362908</v>
@@ -5212,7 +5266,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -5228,7 +5282,7 @@
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="18" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="I17" s="21">
         <v>16</v>
@@ -5236,7 +5290,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -5251,7 +5305,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>71</v>
+        <v>140</v>
       </c>
       <c r="H18" s="33"/>
       <c r="I18" s="17">
@@ -5260,7 +5314,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -5275,7 +5329,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>72</v>
+        <v>141</v>
       </c>
       <c r="H19" s="33"/>
       <c r="I19" s="17">
@@ -5284,7 +5338,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -5299,7 +5353,7 @@
         <v>0.75</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="H20" s="34"/>
       <c r="I20" s="25">
@@ -5308,7 +5362,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -5325,7 +5379,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -5342,7 +5396,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>124</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -5359,7 +5413,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -5376,7 +5430,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>16</v>
@@ -5393,19 +5447,19 @@
     </row>
     <row r="26" spans="1:10">
       <c r="C26" t="s">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="D26" s="2">
         <f>AVERAGE(D6:D25)</f>
         <v>373.44653231864999</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="C27" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="D27" s="2">
         <f>STDEV(D6:D25)</f>
@@ -5415,42 +5469,42 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="26" t="s">
-        <v>124</v>
+        <v>55</v>
       </c>
       <c r="B29" s="26"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>61</v>
+        <v>130</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -5468,7 +5522,7 @@
         <v>2</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="J31" s="17">
         <v>302.94028916180002</v>
@@ -5476,7 +5530,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -5493,7 +5547,7 @@
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
       <c r="I32" s="18" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="J32" s="21">
         <v>17.23574117758357</v>
@@ -5501,7 +5555,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -5516,7 +5570,7 @@
         <v>0.5625</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="H33" s="33"/>
       <c r="I33" s="33"/>
@@ -5526,7 +5580,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -5541,7 +5595,7 @@
         <v>0.89513888888888893</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -5551,7 +5605,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5572,7 +5626,7 @@
         <v>4</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="J35" s="17">
         <v>305.19036102299998</v>
@@ -5580,7 +5634,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>54</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -5598,7 +5652,7 @@
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
       <c r="I36" s="18" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="J36" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5606,7 +5660,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>126</v>
+        <v>57</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -5622,7 +5676,7 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="H37" s="33"/>
       <c r="I37" s="33"/>
@@ -5632,7 +5686,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -5648,7 +5702,7 @@
         <v>0.57916666666666672</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="H38" s="33"/>
       <c r="I38" s="33"/>
@@ -5658,7 +5712,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -5680,7 +5734,7 @@
         <v>8</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="J39" s="17">
         <v>384.05235557549997</v>
@@ -5688,7 +5742,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -5706,7 +5760,7 @@
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
       <c r="I40" s="18" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="J40" s="21">
         <v>32.66972061151673</v>
@@ -5714,7 +5768,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -5730,7 +5784,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="33"/>
@@ -5740,7 +5794,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -5755,7 +5809,7 @@
         <v>0.70972222222222225</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="H42" s="33"/>
       <c r="I42" s="33"/>
@@ -5765,7 +5819,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -5780,7 +5834,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>74</v>
+        <v>143</v>
       </c>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
@@ -5790,7 +5844,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -5805,7 +5859,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>72</v>
+        <v>141</v>
       </c>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -5815,7 +5869,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -5832,7 +5886,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -5849,7 +5903,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>8</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -5864,19 +5918,19 @@
     </row>
     <row r="48" spans="1:10">
       <c r="C48" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="D48" s="2">
         <f>AVERAGE(D30:D47)</f>
         <v>356.83130192700003</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="C49" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="D49" s="2">
         <f>STDEV(D31:D47)</f>
@@ -5893,40 +5947,40 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="26" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="B52" s="26"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="26" t="s">
-        <v>64</v>
+        <v>133</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -5944,7 +5998,7 @@
         <v>4</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="I54" s="17">
         <v>14.1872649193</v>
@@ -5952,7 +6006,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -5968,7 +6022,7 @@
       </c>
       <c r="G55" s="32"/>
       <c r="H55" s="18" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="I55" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5976,7 +6030,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -5994,7 +6048,7 @@
         <v>8</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="I56" s="17">
         <v>44.782275199920001</v>
@@ -6002,7 +6056,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -6018,7 +6072,7 @@
       </c>
       <c r="G57" s="32"/>
       <c r="H57" s="18" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="I57" s="21">
         <v>15.843792242505828</v>
@@ -6026,7 +6080,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -6044,7 +6098,7 @@
         <v>16</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="I58" s="17">
         <v>56.964924156674996</v>
@@ -6052,7 +6106,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -6068,7 +6122,7 @@
       </c>
       <c r="G59" s="32"/>
       <c r="H59" s="18" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="I59" s="21">
         <v>9.4994883808250847</v>
@@ -6076,7 +6130,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -6094,7 +6148,7 @@
         <v>32</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="I60" s="17">
         <v>187.55037531850999</v>
@@ -6102,7 +6156,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -6118,7 +6172,7 @@
       </c>
       <c r="G61" s="32"/>
       <c r="H61" s="18" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="I61" s="21">
         <v>179.97433590633514</v>
@@ -6126,7 +6180,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -6141,7 +6195,7 @@
         <v>0.59236111111111112</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>71</v>
+        <v>140</v>
       </c>
       <c r="H62" s="33"/>
       <c r="I62" s="17">
@@ -6150,7 +6204,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -6165,7 +6219,7 @@
         <v>0.61875000000000002</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>72</v>
+        <v>141</v>
       </c>
       <c r="H63" s="34"/>
       <c r="I63" s="25">
@@ -6174,7 +6228,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B64">
         <v>8</v>
@@ -6191,7 +6245,7 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -6208,7 +6262,7 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -6225,7 +6279,7 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B67">
         <v>8</v>
@@ -6242,7 +6296,7 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B68">
         <v>8</v>
@@ -6259,7 +6313,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -6276,7 +6330,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B70">
         <v>8</v>
@@ -6293,7 +6347,7 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -6310,7 +6364,7 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -6327,7 +6381,7 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -6342,36 +6396,36 @@
     </row>
     <row r="74" spans="1:10">
       <c r="C74" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="D74" s="2">
         <f>AVERAGE(D54:D73)</f>
         <v>117.073104536535</v>
       </c>
       <c r="E74" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="H74" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="I74" s="55">
         <f>AVERAGE(D54:D63,D65:D66,D68:D70,D73)</f>
         <v>53.003791779293749</v>
       </c>
       <c r="J74" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="C75" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="D75" s="2">
         <f>STDEV(D54:D73)</f>
         <v>143.93518726021225</v>
       </c>
       <c r="H75" t="s">
-        <v>67</v>
+        <v>136</v>
       </c>
       <c r="I75" s="55">
         <f>STDEV(D54:D63,D65:D66,D68:D70,D73)</f>
@@ -6387,26 +6441,26 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>63</v>
+        <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="26" t="s">
-        <v>64</v>
+        <v>133</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="C80" s="26" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -6418,9 +6472,9 @@
         <v>329</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>65</v>
+        <v>134</v>
       </c>
       <c r="B82">
         <v>4</v>
@@ -6432,9 +6486,9 @@
         <v>331</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="B83">
         <v>8</v>
@@ -6446,9 +6500,9 @@
         <v>330</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="B84">
         <v>16</v>
@@ -6460,27 +6514,167 @@
         <v>335</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>105</v>
+      </c>
+      <c r="B85">
+        <v>2</v>
+      </c>
+      <c r="C85">
+        <v>8</v>
+      </c>
       <c r="D85">
-        <f>AVERAGE(D81:D84)</f>
-        <v>331.25</v>
-      </c>
-      <c r="E85" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
-      <c r="D86" s="55">
-        <f>STDEV(D81:D84)</f>
-        <v>2.6299556396765835</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
-      <c r="H89" s="2"/>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>105</v>
+      </c>
+      <c r="B86">
+        <v>2</v>
+      </c>
+      <c r="C86">
+        <v>8</v>
+      </c>
+      <c r="D86">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>105</v>
+      </c>
+      <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="C87">
+        <v>8</v>
+      </c>
+      <c r="D87">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>105</v>
+      </c>
+      <c r="B88">
+        <v>2</v>
+      </c>
+      <c r="C88">
+        <v>8</v>
+      </c>
+      <c r="D88">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>105</v>
+      </c>
+      <c r="B89">
+        <v>2</v>
+      </c>
+      <c r="C89">
+        <v>8</v>
+      </c>
+      <c r="D89">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>105</v>
+      </c>
+      <c r="B90">
+        <v>2</v>
+      </c>
+      <c r="C90">
+        <v>8</v>
+      </c>
+      <c r="D90">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>105</v>
+      </c>
+      <c r="B91">
+        <v>2</v>
+      </c>
+      <c r="C91">
+        <v>8</v>
+      </c>
+      <c r="D91">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>105</v>
+      </c>
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="C92">
+        <v>8</v>
+      </c>
+      <c r="D92">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>105</v>
+      </c>
+      <c r="B93">
+        <v>2</v>
+      </c>
+      <c r="C93">
+        <v>8</v>
+      </c>
+      <c r="D93">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>105</v>
+      </c>
+      <c r="B94">
+        <v>2</v>
+      </c>
+      <c r="C94">
+        <v>8</v>
+      </c>
+      <c r="D94">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="D95">
+        <f>AVERAGE(D81:D94)</f>
+        <v>331.21428571428572</v>
+      </c>
+      <c r="E95" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="D96" s="55">
+        <f>STDEV(D81:D94)</f>
+        <v>1.5281246137528048</v>
+      </c>
+    </row>
+    <row r="109" spans="8:8">
+      <c r="H109" s="2"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId4"/>
@@ -6495,16 +6689,16 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="A16" sqref="A16:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
@@ -6514,69 +6708,69 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="28" t="s">
-        <v>94</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="30" t="s">
-        <v>95</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" ht="39" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
       <c r="C5" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="I5" s="29" t="s">
-        <v>117</v>
-      </c>
       <c r="J5" s="29" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="K5" s="28" t="s">
-        <v>97</v>
+        <v>28</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="M5" s="28" t="s">
-        <v>99</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -6611,13 +6805,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>119</v>
+        <v>50</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -6652,13 +6846,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="B8" s="31">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>120</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -6693,7 +6887,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -6731,7 +6925,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -6766,7 +6960,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>32</v>
@@ -6807,7 +7001,7 @@
     </row>
     <row r="12" spans="1:14" s="49" customFormat="1" ht="14" thickBot="1">
       <c r="A12" s="49" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B12" s="49">
         <v>32</v>
@@ -6848,7 +7042,7 @@
     </row>
     <row r="13" spans="1:14" ht="40" thickTop="1">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -6879,12 +7073,12 @@
         <v>2</v>
       </c>
       <c r="N13" s="52" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="39">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -6915,12 +7109,12 @@
         <v>2</v>
       </c>
       <c r="N14" s="52" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="39">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="B15" s="41">
         <v>16</v>
@@ -6951,12 +7145,12 @@
         <v>1</v>
       </c>
       <c r="N15" s="52" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="39">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -6987,12 +7181,12 @@
         <v>0</v>
       </c>
       <c r="N16" s="52" t="s">
-        <v>103</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B17">
         <v>32</v>
@@ -7025,7 +7219,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B18">
         <v>32</v>
@@ -7058,7 +7252,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="B19">
         <v>32</v>
@@ -7095,10 +7289,22 @@
     <row r="21" spans="1:13">
       <c r="I21" s="47"/>
     </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -7109,6 +7315,213 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:J22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="58" customFormat="1" ht="39">
+      <c r="A8" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f>C9*2</f>
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9" s="55">
+        <v>1050.4892129899999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <f>C10*2</f>
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="D11">
+        <f t="shared" ref="D11:D22" si="0">C11*2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L16"/>
@@ -7124,50 +7537,50 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="53" t="s">
-        <v>116</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="54" customFormat="1" ht="39">
       <c r="A5" s="54" t="s">
-        <v>104</v>
+        <v>35</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>105</v>
+        <v>36</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>106</v>
+        <v>37</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>107</v>
+        <v>38</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>108</v>
+        <v>39</v>
       </c>
       <c r="F5" s="54" t="s">
-        <v>109</v>
+        <v>40</v>
       </c>
       <c r="G5" s="54" t="s">
-        <v>111</v>
+        <v>42</v>
       </c>
       <c r="H5" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="54" t="s">
         <v>110</v>
-      </c>
-      <c r="I5" s="54" t="s">
-        <v>112</v>
-      </c>
-      <c r="J5" s="54" t="s">
-        <v>113</v>
-      </c>
-      <c r="K5" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="L5" s="54" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -7206,7 +7619,7 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -7317,7 +7730,7 @@
         <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -7356,7 +7769,7 @@
         <v>3</v>
       </c>
       <c r="L10" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -7594,8 +8007,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -7605,7 +8017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A3:I12"/>
@@ -7635,10 +8047,10 @@
   <sheetData>
     <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -7650,7 +8062,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="11" t="s">
-        <v>29</v>
+        <v>98</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
@@ -7674,12 +8086,12 @@
         <v>32</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
@@ -7696,7 +8108,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="18" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="20">
@@ -7713,7 +8125,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="18" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
@@ -7734,7 +8146,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="18" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
       <c r="B8" s="19">
         <v>2070.8984270000001</v>
@@ -7751,7 +8163,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="B9" s="19">
         <v>1095.4940549999999</v>
@@ -7778,7 +8190,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="18" t="s">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
@@ -7799,7 +8211,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="18" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -7820,7 +8232,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="22" t="s">
-        <v>30</v>
+        <v>99</v>
       </c>
       <c r="B12" s="23">
         <v>1583.1962410000001</v>
@@ -7849,7 +8261,7 @@
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
Working on Scenario I
git-svn-id: file://localhost/tmp/svn2git/svn@1918 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="147">
   <si>
     <t>Poseidon</t>
     <phoneticPr fontId="10" type="noConversion"/>
@@ -53,6 +53,18 @@
   </si>
   <si>
     <t>Runtime (in sec)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon, Oliver</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oliver</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
@@ -2899,7 +2911,7 @@
   <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:D25"/>
+      <selection activeCell="D50" sqref="D50:D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2914,12 +2926,12 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -2927,36 +2939,36 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="39">
       <c r="A4" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2976,7 +2988,7 @@
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -2996,7 +3008,7 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -3016,7 +3028,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3036,7 +3048,7 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -3056,7 +3068,7 @@
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -3076,7 +3088,7 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3096,7 +3108,7 @@
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -3116,7 +3128,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -3136,7 +3148,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3156,7 +3168,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3176,7 +3188,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -3196,7 +3208,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3216,7 +3228,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -3236,7 +3248,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -3256,7 +3268,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -3276,7 +3288,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3307,7 +3319,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3338,7 +3350,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -3369,7 +3381,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -3392,7 +3404,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -3415,7 +3427,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -3436,7 +3448,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -3457,7 +3469,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -3478,7 +3490,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -3499,7 +3511,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -3520,7 +3532,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -3541,7 +3553,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -3562,7 +3574,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -3583,7 +3595,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B34">
         <v>8</v>
@@ -3604,7 +3616,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B35">
         <v>8</v>
@@ -3625,7 +3637,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -3646,7 +3658,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -3667,7 +3679,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="44" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B38" s="44">
         <v>2</v>
@@ -3688,7 +3700,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -3709,7 +3721,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -3730,7 +3742,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -3751,7 +3763,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -3772,7 +3784,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -3793,7 +3805,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -3814,7 +3826,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -3835,7 +3847,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -3866,7 +3878,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -3897,7 +3909,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -3918,7 +3930,7 @@
     </row>
     <row r="49" spans="1:8" s="41" customFormat="1">
       <c r="A49" s="41" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B49" s="41">
         <v>2</v>
@@ -3939,7 +3951,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="39" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B50" s="39">
         <v>4</v>
@@ -3960,7 +3972,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -3981,7 +3993,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -4002,7 +4014,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -4023,7 +4035,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -4044,7 +4056,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -4065,7 +4077,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -4086,7 +4098,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -4107,7 +4119,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -4128,7 +4140,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B59">
         <v>15</v>
@@ -4149,7 +4161,7 @@
     </row>
     <row r="60" spans="1:8" hidden="1">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -4170,7 +4182,7 @@
     </row>
     <row r="61" spans="1:8" hidden="1">
       <c r="A61" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -4182,7 +4194,7 @@
     </row>
     <row r="62" spans="1:8" hidden="1">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -4194,7 +4206,7 @@
     </row>
     <row r="63" spans="1:8" hidden="1">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -4206,7 +4218,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -4227,7 +4239,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -4248,7 +4260,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -4279,7 +4291,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -4310,7 +4322,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -4341,7 +4353,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -4364,7 +4376,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -4387,7 +4399,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -4410,7 +4422,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -4433,7 +4445,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -4456,7 +4468,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -4479,7 +4491,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B75">
         <v>8</v>
@@ -4502,7 +4514,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B76">
         <v>8</v>
@@ -4525,7 +4537,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B77">
         <v>16</v>
@@ -4548,7 +4560,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B78">
         <v>16</v>
@@ -4571,7 +4583,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B79">
         <v>16</v>
@@ -4594,7 +4606,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B80">
         <v>16</v>
@@ -4617,7 +4629,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B81">
         <v>16</v>
@@ -4640,7 +4652,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B82">
         <v>16</v>
@@ -4663,7 +4675,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B83">
         <v>16</v>
@@ -4686,7 +4698,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -4706,7 +4718,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -4726,7 +4738,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -4746,7 +4758,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -4766,7 +4778,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -4786,7 +4798,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -4806,7 +4818,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -4826,7 +4838,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -4846,7 +4858,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -4866,7 +4878,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B93">
         <v>4</v>
@@ -4886,7 +4898,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B94">
         <v>4</v>
@@ -4906,7 +4918,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -4943,8 +4955,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4959,45 +4971,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="26" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>80</v>
-      </c>
       <c r="E5" s="6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5012,7 +5024,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I6" s="17">
         <v>221.43898490266665</v>
@@ -5020,7 +5032,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5036,7 +5048,7 @@
       </c>
       <c r="G7" s="32"/>
       <c r="H7" s="18" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="I7" s="21">
         <v>27.888301147358074</v>
@@ -5044,7 +5056,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5060,7 +5072,7 @@
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I8" s="21">
         <v>6</v>
@@ -5068,7 +5080,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5086,7 +5098,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I9" s="17">
         <v>230.1513251065</v>
@@ -5094,7 +5106,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5110,7 +5122,7 @@
       </c>
       <c r="G10" s="32"/>
       <c r="H10" s="18" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="I10" s="21">
         <v>21.442701960879447</v>
@@ -5118,7 +5130,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5134,7 +5146,7 @@
       </c>
       <c r="G11" s="32"/>
       <c r="H11" s="18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I11" s="21">
         <v>4</v>
@@ -5142,7 +5154,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -5160,7 +5172,7 @@
         <v>8</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I12" s="17">
         <v>524.47522211100011</v>
@@ -5168,7 +5180,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -5184,7 +5196,7 @@
       </c>
       <c r="G13" s="32"/>
       <c r="H13" s="18" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="I13" s="21">
         <v>249.37176975472715</v>
@@ -5192,7 +5204,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -5208,7 +5220,7 @@
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I14" s="21">
         <v>32</v>
@@ -5216,7 +5228,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -5234,7 +5246,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I15" s="17">
         <v>338.08045351500004</v>
@@ -5242,7 +5254,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -5258,7 +5270,7 @@
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="18" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="I16" s="21">
         <v>46.784586737362908</v>
@@ -5266,7 +5278,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -5282,7 +5294,7 @@
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I17" s="21">
         <v>16</v>
@@ -5290,7 +5302,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -5305,7 +5317,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="H18" s="33"/>
       <c r="I18" s="17">
@@ -5314,7 +5326,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -5329,7 +5341,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H19" s="33"/>
       <c r="I19" s="17">
@@ -5338,7 +5350,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -5353,7 +5365,7 @@
         <v>0.75</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H20" s="34"/>
       <c r="I20" s="25">
@@ -5362,7 +5374,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -5379,7 +5391,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -5396,7 +5408,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -5413,7 +5425,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -5430,7 +5442,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>16</v>
@@ -5447,19 +5459,19 @@
     </row>
     <row r="26" spans="1:10">
       <c r="C26" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D26" s="2">
         <f>AVERAGE(D6:D25)</f>
         <v>373.44653231864999</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="C27" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D27" s="2">
         <f>STDEV(D6:D25)</f>
@@ -5469,42 +5481,42 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="26" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B29" s="26"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C30" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="H30" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>9</v>
-      </c>
       <c r="I30" s="11" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -5522,7 +5534,7 @@
         <v>2</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="J31" s="17">
         <v>302.94028916180002</v>
@@ -5530,7 +5542,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -5547,7 +5559,7 @@
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
       <c r="I32" s="18" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="J32" s="21">
         <v>17.23574117758357</v>
@@ -5555,7 +5567,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -5570,7 +5582,7 @@
         <v>0.5625</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H33" s="33"/>
       <c r="I33" s="33"/>
@@ -5580,7 +5592,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -5595,7 +5607,7 @@
         <v>0.89513888888888893</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -5605,7 +5617,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5626,7 +5638,7 @@
         <v>4</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="J35" s="17">
         <v>305.19036102299998</v>
@@ -5634,7 +5646,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -5652,7 +5664,7 @@
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
       <c r="I36" s="18" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="J36" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5660,7 +5672,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -5676,7 +5688,7 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H37" s="33"/>
       <c r="I37" s="33"/>
@@ -5686,7 +5698,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -5702,7 +5714,7 @@
         <v>0.57916666666666672</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H38" s="33"/>
       <c r="I38" s="33"/>
@@ -5712,7 +5724,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -5734,7 +5746,7 @@
         <v>8</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="J39" s="17">
         <v>384.05235557549997</v>
@@ -5742,7 +5754,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -5760,7 +5772,7 @@
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
       <c r="I40" s="18" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="J40" s="21">
         <v>32.66972061151673</v>
@@ -5768,7 +5780,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -5784,7 +5796,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="33"/>
@@ -5794,7 +5806,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -5809,7 +5821,7 @@
         <v>0.70972222222222225</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H42" s="33"/>
       <c r="I42" s="33"/>
@@ -5819,7 +5831,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -5834,7 +5846,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
@@ -5844,7 +5856,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -5859,7 +5871,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -5869,7 +5881,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -5886,7 +5898,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -5903,7 +5915,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -5918,19 +5930,19 @@
     </row>
     <row r="48" spans="1:10">
       <c r="C48" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D48" s="2">
         <f>AVERAGE(D30:D47)</f>
         <v>356.83130192700003</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="C49" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D49" s="2">
         <f>STDEV(D31:D47)</f>
@@ -5947,40 +5959,40 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="26" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B52" s="26"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="26" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -5998,7 +6010,7 @@
         <v>4</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I54" s="17">
         <v>14.1872649193</v>
@@ -6006,7 +6018,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -6022,7 +6034,7 @@
       </c>
       <c r="G55" s="32"/>
       <c r="H55" s="18" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="I55" s="21" t="e">
         <v>#DIV/0!</v>
@@ -6030,7 +6042,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -6048,7 +6060,7 @@
         <v>8</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I56" s="17">
         <v>44.782275199920001</v>
@@ -6056,7 +6068,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -6072,7 +6084,7 @@
       </c>
       <c r="G57" s="32"/>
       <c r="H57" s="18" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="I57" s="21">
         <v>15.843792242505828</v>
@@ -6080,7 +6092,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -6098,7 +6110,7 @@
         <v>16</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I58" s="17">
         <v>56.964924156674996</v>
@@ -6106,7 +6118,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -6122,7 +6134,7 @@
       </c>
       <c r="G59" s="32"/>
       <c r="H59" s="18" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="I59" s="21">
         <v>9.4994883808250847</v>
@@ -6130,7 +6142,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -6148,7 +6160,7 @@
         <v>32</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I60" s="17">
         <v>187.55037531850999</v>
@@ -6156,7 +6168,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -6172,7 +6184,7 @@
       </c>
       <c r="G61" s="32"/>
       <c r="H61" s="18" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="I61" s="21">
         <v>179.97433590633514</v>
@@ -6180,7 +6192,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -6195,7 +6207,7 @@
         <v>0.59236111111111112</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="H62" s="33"/>
       <c r="I62" s="17">
@@ -6204,7 +6216,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -6219,7 +6231,7 @@
         <v>0.61875000000000002</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H63" s="34"/>
       <c r="I63" s="25">
@@ -6228,7 +6240,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B64">
         <v>8</v>
@@ -6245,7 +6257,7 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -6262,7 +6274,7 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -6279,7 +6291,7 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B67">
         <v>8</v>
@@ -6296,7 +6308,7 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B68">
         <v>8</v>
@@ -6313,7 +6325,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -6330,7 +6342,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B70">
         <v>8</v>
@@ -6347,7 +6359,7 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -6364,7 +6376,7 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -6381,7 +6393,7 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -6396,36 +6408,36 @@
     </row>
     <row r="74" spans="1:10">
       <c r="C74" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D74" s="2">
         <f>AVERAGE(D54:D73)</f>
         <v>117.073104536535</v>
       </c>
       <c r="E74" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H74" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I74" s="55">
         <f>AVERAGE(D54:D63,D65:D66,D68:D70,D73)</f>
         <v>53.003791779293749</v>
       </c>
       <c r="J74" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="C75" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D75" s="2">
         <f>STDEV(D54:D73)</f>
         <v>143.93518726021225</v>
       </c>
       <c r="H75" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="I75" s="55">
         <f>STDEV(D54:D63,D65:D66,D68:D70,D73)</f>
@@ -6441,26 +6453,26 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="26" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C80" s="26" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -6474,7 +6486,7 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B82">
         <v>4</v>
@@ -6488,7 +6500,7 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B83">
         <v>8</v>
@@ -6502,7 +6514,7 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B84">
         <v>16</v>
@@ -6516,7 +6528,7 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -6530,7 +6542,7 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B86">
         <v>2</v>
@@ -6544,7 +6556,7 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B87">
         <v>2</v>
@@ -6558,7 +6570,7 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B88">
         <v>2</v>
@@ -6572,7 +6584,7 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -6586,7 +6598,7 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -6600,7 +6612,7 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -6614,7 +6626,7 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -6628,7 +6640,7 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B93">
         <v>2</v>
@@ -6642,7 +6654,7 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -6660,7 +6672,7 @@
         <v>331.21428571428572</v>
       </c>
       <c r="E95" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -6673,7 +6685,6 @@
       <c r="H109" s="2"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6708,69 +6719,69 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="28" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="30" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" ht="39" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D5" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="E5" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>115</v>
-      </c>
       <c r="G5" s="29" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="K5" s="28" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M5" s="28" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -6805,13 +6816,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -6846,13 +6857,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B8" s="31">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -6887,7 +6898,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -6925,7 +6936,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -6960,7 +6971,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>32</v>
@@ -7001,7 +7012,7 @@
     </row>
     <row r="12" spans="1:14" s="49" customFormat="1" ht="14" thickBot="1">
       <c r="A12" s="49" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B12" s="49">
         <v>32</v>
@@ -7042,7 +7053,7 @@
     </row>
     <row r="13" spans="1:14" ht="40" thickTop="1">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -7073,12 +7084,12 @@
         <v>2</v>
       </c>
       <c r="N13" s="52" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="39">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -7109,12 +7120,12 @@
         <v>2</v>
       </c>
       <c r="N14" s="52" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="39">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B15" s="41">
         <v>16</v>
@@ -7145,12 +7156,12 @@
         <v>1</v>
       </c>
       <c r="N15" s="52" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="39">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -7181,12 +7192,12 @@
         <v>0</v>
       </c>
       <c r="N16" s="52" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>32</v>
@@ -7219,7 +7230,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>32</v>
@@ -7252,7 +7263,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B19">
         <v>32</v>
@@ -7291,17 +7302,16 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="28" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7320,7 +7330,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -7332,12 +7342,12 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -7353,16 +7363,16 @@
     </row>
     <row r="8" spans="1:10" s="58" customFormat="1" ht="39">
       <c r="A8" s="29" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>1</v>
@@ -7371,13 +7381,13 @@
         <v>2</v>
       </c>
       <c r="G8" s="57" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H8" s="57" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I8" s="57" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J8" s="58" t="s">
         <v>5</v>
@@ -7398,7 +7408,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F9">
         <v>8</v>
@@ -7431,28 +7441,115 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F10">
         <v>8</v>
       </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10" s="55">
+        <v>990.53072500200005</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
       <c r="D11">
         <f t="shared" ref="D11:D22" si="0">C11*2</f>
         <v>0</v>
       </c>
+      <c r="E11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" s="55">
+        <v>1027.9399099300001</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <v>16</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12" s="55">
+        <v>985.09084010100003</v>
       </c>
     </row>
     <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>8</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -7537,50 +7634,50 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="53" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="54" customFormat="1" ht="39">
       <c r="A5" s="54" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F5" s="54" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G5" s="54" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H5" s="54" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="I5" s="54" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="J5" s="54" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="K5" s="54" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L5" s="54" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -7619,7 +7716,7 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -7730,7 +7827,7 @@
         <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -7769,7 +7866,7 @@
         <v>3</v>
       </c>
       <c r="L10" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -8047,10 +8144,10 @@
   <sheetData>
     <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -8062,7 +8159,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="11" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
@@ -8086,12 +8183,12 @@
         <v>32</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
@@ -8108,7 +8205,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="18" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="20">
@@ -8125,7 +8222,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="18" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
@@ -8146,7 +8243,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="18" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B8" s="19">
         <v>2070.8984270000001</v>
@@ -8163,7 +8260,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B9" s="19">
         <v>1095.4940549999999</v>
@@ -8190,7 +8287,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="18" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
@@ -8211,7 +8308,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="18" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -8232,7 +8329,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="22" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B12" s="23">
         <v>1583.1962410000001</v>
@@ -8260,7 +8357,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Some more data and a new graph for scenario I
git-svn-id: file://localhost/tmp/svn2git/svn@1922 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="-200" windowWidth="35980" windowHeight="21780" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="-200" windowWidth="35980" windowHeight="21780" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NAMD Runtimes" sheetId="1" r:id="rId1"/>
@@ -30,85 +30,117 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="154">
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grid 8/8</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Condor 8/8</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grid 8/6
+Nimbus 8/2</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grid 8/4 
+Condor 8/4</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grid 8/4
+Condor 8/3
+Nimbus 8/1</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Condor Ressourcen</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Condor Number Cores</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Job Size</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Fixed</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Runtime (in sec)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon, Oliver</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Oliver</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Grid (Poseidon)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Grid (Poseidon - adjusted)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Condor (Poseidon)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon (CHARM)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>2 core</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Number Cores</t>
   </si>
   <si>
     <t>Number Cores</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Nodes</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Number Cores</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>m1.large</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>1 STABW - Startup Time (in s)</t>
@@ -139,172 +171,172 @@
   </si>
   <si>
     <t>m1.large</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Adaptive Scenario</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Time for completion for n jobs</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Jobs run as soon as a resource becomes available</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t># TG</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t># Nimbus</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t># EC2</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Average</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>EC2 m1.large</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Nimbus</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>LONI 16 core
 Nimbus 16 core</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Run ID</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Number Replicas</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>MAX_RUNTIME (in min)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Check Period (in min)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Max Cloud Pilots</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Cloud Pilot Size</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Runtime (in min)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Runtime (in sec)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t># Nimbus</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t># Poseidon</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t># Cloud Pilots</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Start Pilot if not sufficient progress is made</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Deadline Scenario</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Job Size Cloud (in Cores)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Job Size TG (in Cores)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>n/a</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>SAGA Pilot Sub-Job Runtime</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Overhead (in s)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Overhead (in %)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>2 cores</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Nimbus</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Amazon </t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>2 cores</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>EUCA (Indiana)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Number Steps: </t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>NAMD Run</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Number Nodes</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Number Cores (Total)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>EC2 (m1.large)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Runs a Workload of 8 replicas in a fixed distribution</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t># TG</t>
@@ -314,111 +346,111 @@
   </si>
   <si>
     <t># Condor</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Number Cores</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Average (drop maxima)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Machine</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Nimbus (Chicago)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>EC2 (c1.xlarge)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>EC2 (m2.4xlarge)</t>
   </si>
   <si>
     <t>EC2 (m2.4xlarge)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>EC2 (m2.4xlarge)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Walltime (in sec)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Startup Times</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Startup Time (in s)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Instance</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>m1.large</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Number Instances</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>2 cores</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>LONI 8 core
 Nimbus 8 core</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>LONI 8 core 
 Nimbus 16 core</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>LONI 16 core
 Nimbus 8 core</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Startup Time (in s)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Instance</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Date</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>m1.large</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>QB (MPI)</t>
   </si>
   <si>
     <t>QB (MPI)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>QB (CHARM)</t>
   </si>
   <si>
     <t>QB (CHARM)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Mittelwert - Walltime (in sec)</t>
@@ -446,108 +478,108 @@
   </si>
   <si>
     <t>CPU Time (in sec)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>LONI</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Date</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Cores</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Queue Time
 Nimbus</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>n/a</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Poseidon </t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>TG</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Nimbus Number Cores</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Number Cores</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>EC2</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>EC2 Number Cores</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Number Jobs</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>n/a</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Average</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Stddev</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Time-to-Completion (in s)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>m1.large</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>2 cores</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Average</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Startup Time (in s)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Poseidon</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Memory (in MB)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Number Instances</t>
@@ -557,19 +589,19 @@
   </si>
   <si>
     <t>LONI/Condor</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Resource</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Oliver</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Stdev (drop maxima)</t>
-    <phoneticPr fontId="10" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Ergebnis</t>
@@ -601,13 +633,17 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -839,23 +875,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -874,20 +910,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -907,8 +943,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -917,6 +953,10 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1274,6 +1314,179 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="de-DE"/>
+  <c:style val="1"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.124673396389476"/>
+          <c:y val="0.0327626436670966"/>
+          <c:w val="0.858558310927597"/>
+          <c:h val="0.78585410931213"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Fixed!$A$54:$A$58</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Grid 8/8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Condor 8/8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Grid 8/6_x000d_Nimbus 8/2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Grid 8/4 _x000d_Condor 8/4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Grid 8/4_x000d_Condor 8/3_x000d_Nimbus 8/1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Fixed!$B$54:$B$58</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1027.93990993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1050.48921299</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1051.73987007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>543.972661972</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>688.6416651936665</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="606356840"/>
+        <c:axId val="606342248"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="606356840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1600"/>
+                  <a:t>Resource #cores/#replicas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="606342248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="606342248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1600"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1600"/>
+                  <a:t>Runtime (in sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="606356840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1327,6 +1540,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="9" name="Diagramm 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>939800</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2926,12 +3174,12 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -2939,36 +3187,36 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="39">
       <c r="A4" s="3" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2988,7 +3236,7 @@
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -3008,7 +3256,7 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -3028,7 +3276,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3048,7 +3296,7 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -3068,7 +3316,7 @@
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -3088,7 +3336,7 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3108,7 +3356,7 @@
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -3128,7 +3376,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -3148,7 +3396,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3168,7 +3416,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3188,7 +3436,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -3208,7 +3456,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3228,7 +3476,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -3248,7 +3496,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -3268,7 +3516,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -3288,7 +3536,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3319,7 +3567,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3350,7 +3598,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -3381,7 +3629,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -3404,7 +3652,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -3427,7 +3675,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -3448,7 +3696,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -3469,7 +3717,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -3490,7 +3738,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -3511,7 +3759,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -3532,7 +3780,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -3553,7 +3801,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -3574,7 +3822,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -3595,7 +3843,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B34">
         <v>8</v>
@@ -3616,7 +3864,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B35">
         <v>8</v>
@@ -3637,7 +3885,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -3658,7 +3906,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -3679,7 +3927,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="44" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B38" s="44">
         <v>2</v>
@@ -3700,7 +3948,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -3721,7 +3969,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -3742,7 +3990,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -3763,7 +4011,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -3784,7 +4032,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -3805,7 +4053,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -3826,7 +4074,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -3847,7 +4095,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -3878,7 +4126,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -3909,7 +4157,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -3930,7 +4178,7 @@
     </row>
     <row r="49" spans="1:8" s="41" customFormat="1">
       <c r="A49" s="41" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B49" s="41">
         <v>2</v>
@@ -3951,7 +4199,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="39" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B50" s="39">
         <v>4</v>
@@ -3972,7 +4220,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -3993,7 +4241,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -4014,7 +4262,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -4035,7 +4283,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -4056,7 +4304,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -4077,7 +4325,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -4098,7 +4346,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -4119,7 +4367,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -4140,7 +4388,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B59">
         <v>15</v>
@@ -4161,7 +4409,7 @@
     </row>
     <row r="60" spans="1:8" hidden="1">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -4182,7 +4430,7 @@
     </row>
     <row r="61" spans="1:8" hidden="1">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -4194,7 +4442,7 @@
     </row>
     <row r="62" spans="1:8" hidden="1">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -4206,7 +4454,7 @@
     </row>
     <row r="63" spans="1:8" hidden="1">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -4218,7 +4466,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -4239,7 +4487,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -4260,7 +4508,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -4291,7 +4539,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -4322,7 +4570,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -4353,7 +4601,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -4376,7 +4624,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -4399,7 +4647,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -4422,7 +4670,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -4445,7 +4693,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -4468,7 +4716,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -4491,7 +4739,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B75">
         <v>8</v>
@@ -4514,7 +4762,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B76">
         <v>8</v>
@@ -4537,7 +4785,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B77">
         <v>16</v>
@@ -4560,7 +4808,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B78">
         <v>16</v>
@@ -4583,7 +4831,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B79">
         <v>16</v>
@@ -4606,7 +4854,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B80">
         <v>16</v>
@@ -4629,7 +4877,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B81">
         <v>16</v>
@@ -4652,7 +4900,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B82">
         <v>16</v>
@@ -4675,7 +4923,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B83">
         <v>16</v>
@@ -4698,7 +4946,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -4718,7 +4966,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -4738,7 +4986,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -4758,7 +5006,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -4778,7 +5026,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -4798,7 +5046,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -4818,7 +5066,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -4838,7 +5086,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -4858,7 +5106,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -4878,7 +5126,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B93">
         <v>4</v>
@@ -4898,7 +5146,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B94">
         <v>4</v>
@@ -4918,7 +5166,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -4940,7 +5188,7 @@
       <c r="A98" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -4955,7 +5203,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
@@ -4971,45 +5219,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="26" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5024,7 +5272,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="I6" s="17">
         <v>221.43898490266665</v>
@@ -5032,7 +5280,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5048,7 +5296,7 @@
       </c>
       <c r="G7" s="32"/>
       <c r="H7" s="18" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="I7" s="21">
         <v>27.888301147358074</v>
@@ -5056,7 +5304,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5072,7 +5320,7 @@
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="18" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="I8" s="21">
         <v>6</v>
@@ -5080,7 +5328,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5098,7 +5346,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="I9" s="17">
         <v>230.1513251065</v>
@@ -5106,7 +5354,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5122,7 +5370,7 @@
       </c>
       <c r="G10" s="32"/>
       <c r="H10" s="18" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="I10" s="21">
         <v>21.442701960879447</v>
@@ -5130,7 +5378,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5146,7 +5394,7 @@
       </c>
       <c r="G11" s="32"/>
       <c r="H11" s="18" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="I11" s="21">
         <v>4</v>
@@ -5154,7 +5402,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -5172,7 +5420,7 @@
         <v>8</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="I12" s="17">
         <v>524.47522211100011</v>
@@ -5180,7 +5428,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -5196,7 +5444,7 @@
       </c>
       <c r="G13" s="32"/>
       <c r="H13" s="18" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="I13" s="21">
         <v>249.37176975472715</v>
@@ -5204,7 +5452,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -5220,7 +5468,7 @@
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="18" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="I14" s="21">
         <v>32</v>
@@ -5228,7 +5476,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -5246,7 +5494,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="I15" s="17">
         <v>338.08045351500004</v>
@@ -5254,7 +5502,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -5270,7 +5518,7 @@
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="18" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="I16" s="21">
         <v>46.784586737362908</v>
@@ -5278,7 +5526,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -5294,7 +5542,7 @@
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="18" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="I17" s="21">
         <v>16</v>
@@ -5302,7 +5550,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -5317,7 +5565,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="H18" s="33"/>
       <c r="I18" s="17">
@@ -5326,7 +5574,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -5341,7 +5589,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="H19" s="33"/>
       <c r="I19" s="17">
@@ -5350,7 +5598,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -5365,7 +5613,7 @@
         <v>0.75</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="H20" s="34"/>
       <c r="I20" s="25">
@@ -5374,7 +5622,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -5391,7 +5639,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -5408,7 +5656,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -5425,7 +5673,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -5442,7 +5690,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B25">
         <v>16</v>
@@ -5459,19 +5707,19 @@
     </row>
     <row r="26" spans="1:10">
       <c r="C26" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D26" s="2">
         <f>AVERAGE(D6:D25)</f>
         <v>373.44653231864999</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="C27" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D27" s="2">
         <f>STDEV(D6:D25)</f>
@@ -5481,42 +5729,42 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="26" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B29" s="26"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -5534,7 +5782,7 @@
         <v>2</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="J31" s="17">
         <v>302.94028916180002</v>
@@ -5542,7 +5790,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -5559,7 +5807,7 @@
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
       <c r="I32" s="18" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="J32" s="21">
         <v>17.23574117758357</v>
@@ -5567,7 +5815,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -5582,7 +5830,7 @@
         <v>0.5625</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H33" s="33"/>
       <c r="I33" s="33"/>
@@ -5592,7 +5840,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -5607,7 +5855,7 @@
         <v>0.89513888888888893</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -5617,7 +5865,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5638,7 +5886,7 @@
         <v>4</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="J35" s="17">
         <v>305.19036102299998</v>
@@ -5646,7 +5894,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -5664,7 +5912,7 @@
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
       <c r="I36" s="18" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="J36" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5672,7 +5920,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -5688,7 +5936,7 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="H37" s="33"/>
       <c r="I37" s="33"/>
@@ -5698,7 +5946,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -5714,7 +5962,7 @@
         <v>0.57916666666666672</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H38" s="33"/>
       <c r="I38" s="33"/>
@@ -5724,7 +5972,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -5746,7 +5994,7 @@
         <v>8</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="J39" s="17">
         <v>384.05235557549997</v>
@@ -5754,7 +6002,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -5772,7 +6020,7 @@
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
       <c r="I40" s="18" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="J40" s="21">
         <v>32.66972061151673</v>
@@ -5780,7 +6028,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -5796,7 +6044,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="33"/>
@@ -5806,7 +6054,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -5821,7 +6069,7 @@
         <v>0.70972222222222225</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="H42" s="33"/>
       <c r="I42" s="33"/>
@@ -5831,7 +6079,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -5846,7 +6094,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
@@ -5856,7 +6104,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -5871,7 +6119,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -5881,7 +6129,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -5898,7 +6146,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -5915,7 +6163,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -5930,19 +6178,19 @@
     </row>
     <row r="48" spans="1:10">
       <c r="C48" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D48" s="2">
         <f>AVERAGE(D30:D47)</f>
         <v>356.83130192700003</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="C49" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D49" s="2">
         <f>STDEV(D31:D47)</f>
@@ -5959,40 +6207,40 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="26" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B52" s="26"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="26" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -6010,7 +6258,7 @@
         <v>4</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="I54" s="17">
         <v>14.1872649193</v>
@@ -6018,7 +6266,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -6034,7 +6282,7 @@
       </c>
       <c r="G55" s="32"/>
       <c r="H55" s="18" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="I55" s="21" t="e">
         <v>#DIV/0!</v>
@@ -6042,7 +6290,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -6060,7 +6308,7 @@
         <v>8</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="I56" s="17">
         <v>44.782275199920001</v>
@@ -6068,7 +6316,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -6084,7 +6332,7 @@
       </c>
       <c r="G57" s="32"/>
       <c r="H57" s="18" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="I57" s="21">
         <v>15.843792242505828</v>
@@ -6092,7 +6340,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -6110,7 +6358,7 @@
         <v>16</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="I58" s="17">
         <v>56.964924156674996</v>
@@ -6118,7 +6366,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -6134,7 +6382,7 @@
       </c>
       <c r="G59" s="32"/>
       <c r="H59" s="18" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="I59" s="21">
         <v>9.4994883808250847</v>
@@ -6142,7 +6390,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -6160,7 +6408,7 @@
         <v>32</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="I60" s="17">
         <v>187.55037531850999</v>
@@ -6168,7 +6416,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -6184,7 +6432,7 @@
       </c>
       <c r="G61" s="32"/>
       <c r="H61" s="18" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="I61" s="21">
         <v>179.97433590633514</v>
@@ -6192,7 +6440,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -6207,7 +6455,7 @@
         <v>0.59236111111111112</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="H62" s="33"/>
       <c r="I62" s="17">
@@ -6216,7 +6464,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -6231,7 +6479,7 @@
         <v>0.61875000000000002</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="H63" s="34"/>
       <c r="I63" s="25">
@@ -6240,7 +6488,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B64">
         <v>8</v>
@@ -6257,7 +6505,7 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -6274,7 +6522,7 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -6291,7 +6539,7 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B67">
         <v>8</v>
@@ -6308,7 +6556,7 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B68">
         <v>8</v>
@@ -6325,7 +6573,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -6342,7 +6590,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B70">
         <v>8</v>
@@ -6359,7 +6607,7 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -6376,7 +6624,7 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -6393,7 +6641,7 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -6408,36 +6656,36 @@
     </row>
     <row r="74" spans="1:10">
       <c r="C74" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D74" s="2">
         <f>AVERAGE(D54:D73)</f>
         <v>117.073104536535</v>
       </c>
       <c r="E74" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H74" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="I74" s="55">
         <f>AVERAGE(D54:D63,D65:D66,D68:D70,D73)</f>
         <v>53.003791779293749</v>
       </c>
       <c r="J74" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="C75" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D75" s="2">
         <f>STDEV(D54:D73)</f>
         <v>143.93518726021225</v>
       </c>
       <c r="H75" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="I75" s="55">
         <f>STDEV(D54:D63,D65:D66,D68:D70,D73)</f>
@@ -6453,26 +6701,26 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="26" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C80" s="26" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -6486,7 +6734,7 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B82">
         <v>4</v>
@@ -6500,7 +6748,7 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B83">
         <v>8</v>
@@ -6514,7 +6762,7 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B84">
         <v>16</v>
@@ -6528,7 +6776,7 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -6542,7 +6790,7 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B86">
         <v>2</v>
@@ -6556,7 +6804,7 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B87">
         <v>2</v>
@@ -6570,7 +6818,7 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B88">
         <v>2</v>
@@ -6584,7 +6832,7 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -6598,7 +6846,7 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -6612,7 +6860,7 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -6626,7 +6874,7 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -6640,7 +6888,7 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B93">
         <v>2</v>
@@ -6654,7 +6902,7 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -6672,7 +6920,7 @@
         <v>331.21428571428572</v>
       </c>
       <c r="E95" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -6686,7 +6934,7 @@
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId4"/>
@@ -6704,7 +6952,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD17"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -6720,69 +6968,69 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="28" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="30" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" ht="39" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="E5" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="I5" s="29" t="s">
-        <v>54</v>
-      </c>
       <c r="J5" s="29" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="K5" s="28" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="M5" s="28" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -6817,13 +7065,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -6858,13 +7106,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B8" s="31">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -6899,7 +7147,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -6937,7 +7185,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -6972,7 +7220,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>32</v>
@@ -7013,7 +7261,7 @@
     </row>
     <row r="12" spans="1:14" s="49" customFormat="1" ht="14" thickBot="1">
       <c r="A12" s="49" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B12" s="49">
         <v>32</v>
@@ -7054,7 +7302,7 @@
     </row>
     <row r="13" spans="1:14" ht="40" thickTop="1">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -7085,12 +7333,12 @@
         <v>2</v>
       </c>
       <c r="N13" s="52" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="39">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -7121,12 +7369,12 @@
         <v>2</v>
       </c>
       <c r="N14" s="52" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="39">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B15" s="41">
         <v>16</v>
@@ -7157,12 +7405,12 @@
         <v>1</v>
       </c>
       <c r="N15" s="52" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="39">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -7193,12 +7441,12 @@
         <v>0</v>
       </c>
       <c r="N16" s="52" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>32</v>
@@ -7231,7 +7479,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>32</v>
@@ -7264,7 +7512,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>32</v>
@@ -7303,17 +7551,18 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="28" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
@@ -7328,27 +7577,30 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="S55" sqref="S55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="56" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -7356,7 +7608,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -7364,97 +7616,99 @@
     </row>
     <row r="8" spans="1:10" s="58" customFormat="1" ht="39">
       <c r="A8" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" s="58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="58" customFormat="1">
+      <c r="A9" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="29" t="s">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9">
         <v>2</v>
       </c>
-      <c r="G8" s="57" t="s">
-        <v>71</v>
-      </c>
-      <c r="H8" s="57" t="s">
-        <v>72</v>
-      </c>
-      <c r="I8" s="57" t="s">
-        <v>73</v>
-      </c>
-      <c r="J8" s="58" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
+      <c r="I9" s="60">
         <v>0</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <f>C9*2</f>
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>111</v>
-      </c>
-      <c r="F9">
-        <v>8</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>8</v>
-      </c>
-      <c r="J9" s="55">
-        <v>1050.4892129899999</v>
+      <c r="J9" s="51">
+        <v>1051.7398700700001</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <f>C10*2</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="F10">
         <v>8</v>
       </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
       <c r="H10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J10" s="55">
-        <v>990.53072500200005</v>
+        <v>1050.4892129899999</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -7462,70 +7716,67 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11:D22" si="0">C11*2</f>
-        <v>0</v>
+        <f>C11*2</f>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
         <v>8</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J11" s="55">
-        <v>1027.9399099300001</v>
+        <v>990.53072500200005</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>8</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E12" t="s">
-        <v>7</v>
+        <f t="shared" ref="D12:D23" si="0">C12*2</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J12" s="55">
-        <v>985.09084010100003</v>
+        <v>1027.9399099300001</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -7538,80 +7789,408 @@
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F13">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="J13" s="55">
+        <v>985.09084010100003</v>
       </c>
     </row>
     <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14">
+        <v>8</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14" s="55">
+        <v>692.35480594600006</v>
       </c>
     </row>
     <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15" s="55">
+        <v>677.63002896299997</v>
       </c>
     </row>
     <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16" s="55">
+        <v>736.197400808</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17" s="55">
+        <v>691.674695015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18" s="55">
+        <v>691.32184195499997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="J19" s="55">
+        <v>662.85133695599995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+      <c r="J20" s="55">
+        <v>677.42435908300001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21">
+        <v>8</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21" s="55">
+        <v>676.69090104099996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
       <c r="D22">
         <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22">
+        <v>8</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+      <c r="J22" s="55">
+        <v>691.62961697599997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23">
+        <v>8</v>
+      </c>
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23">
         <v>0</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23" s="55">
+        <v>543.97266197199997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="55">
+        <f>J12</f>
+        <v>1027.9399099300001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="55">
+        <f>J10</f>
+        <v>1050.4892129899999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="26">
+      <c r="A56" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" s="55">
+        <f>J9</f>
+        <v>1051.7398700700001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="26">
+      <c r="A57" s="52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57" s="55">
+        <f>J23</f>
+        <v>543.97266197199997</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="39">
+      <c r="A58" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="55">
+        <f>AVERAGE(J14:J22)</f>
+        <v>688.64166519366654</v>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="B58" formulaRange="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7636,50 +8215,50 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="53" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="54" customFormat="1" ht="39">
       <c r="A5" s="54" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F5" s="54" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="G5" s="54" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="H5" s="54" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="I5" s="54" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="J5" s="54" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="K5" s="54" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="L5" s="54" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -7718,7 +8297,7 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -7829,7 +8408,7 @@
         <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -7868,7 +8447,7 @@
         <v>3</v>
       </c>
       <c r="L10" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -8107,7 +8686,7 @@
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -8147,10 +8726,10 @@
   <sheetData>
     <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -8162,7 +8741,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="11" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
@@ -8186,12 +8765,12 @@
         <v>32</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
@@ -8208,7 +8787,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="18" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="20">
@@ -8225,7 +8804,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="18" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
@@ -8246,7 +8825,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="18" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B8" s="19">
         <v>2070.8984270000001</v>
@@ -8263,7 +8842,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B9" s="19">
         <v>1095.4940549999999</v>
@@ -8290,7 +8869,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="18" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
@@ -8311,7 +8890,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="18" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -8332,7 +8911,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="22" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B12" s="23">
         <v>1583.1962410000001</v>
@@ -8361,7 +8940,7 @@
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
some notes on fluctuation on typical Grid resources typos
git-svn-id: file://localhost/tmp/svn2git/svn@1925 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="156">
   <si>
     <t>-</t>
     <phoneticPr fontId="11" type="noConversion"/>
@@ -57,6 +57,14 @@
     <t>Grid 8/4
 Condor 8/3
 Nimbus 8/1</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stddev</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
@@ -1377,7 +1385,7 @@
                   <c:v>1051.73987007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>543.972661972</c:v>
+                  <c:v>621.08587497475</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>688.6416651936665</c:v>
@@ -3174,12 +3182,12 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -3187,36 +3195,36 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="39">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3236,7 +3244,7 @@
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -3256,7 +3264,7 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -3276,7 +3284,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3296,7 +3304,7 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -3316,7 +3324,7 @@
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -3336,7 +3344,7 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3356,7 +3364,7 @@
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -3376,7 +3384,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -3396,7 +3404,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3416,7 +3424,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3436,7 +3444,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -3456,7 +3464,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3476,7 +3484,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -3496,7 +3504,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -3516,7 +3524,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -3536,7 +3544,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3567,7 +3575,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3598,7 +3606,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -3629,7 +3637,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -3652,7 +3660,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -3675,7 +3683,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -3696,7 +3704,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -3717,7 +3725,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -3738,7 +3746,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -3759,7 +3767,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -3780,7 +3788,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -3801,7 +3809,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -3822,7 +3830,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -3843,7 +3851,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B34">
         <v>8</v>
@@ -3864,7 +3872,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B35">
         <v>8</v>
@@ -3885,7 +3893,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -3906,7 +3914,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -3927,7 +3935,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="44" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B38" s="44">
         <v>2</v>
@@ -3948,7 +3956,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -3969,7 +3977,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -3990,7 +3998,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -4011,7 +4019,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -4032,7 +4040,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -4053,7 +4061,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -4074,7 +4082,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -4095,7 +4103,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -4126,7 +4134,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -4157,7 +4165,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -4178,7 +4186,7 @@
     </row>
     <row r="49" spans="1:8" s="41" customFormat="1">
       <c r="A49" s="41" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B49" s="41">
         <v>2</v>
@@ -4199,7 +4207,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="39" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B50" s="39">
         <v>4</v>
@@ -4220,7 +4228,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -4241,7 +4249,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -4262,7 +4270,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -4283,7 +4291,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -4304,7 +4312,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -4325,7 +4333,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -4346,7 +4354,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -4367,7 +4375,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -4388,7 +4396,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B59">
         <v>15</v>
@@ -4409,7 +4417,7 @@
     </row>
     <row r="60" spans="1:8" hidden="1">
       <c r="A60" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -4430,7 +4438,7 @@
     </row>
     <row r="61" spans="1:8" hidden="1">
       <c r="A61" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -4442,7 +4450,7 @@
     </row>
     <row r="62" spans="1:8" hidden="1">
       <c r="A62" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -4454,7 +4462,7 @@
     </row>
     <row r="63" spans="1:8" hidden="1">
       <c r="A63" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -4466,7 +4474,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -4487,7 +4495,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -4508,7 +4516,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -4539,7 +4547,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -4570,7 +4578,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -4601,7 +4609,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -4624,7 +4632,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -4647,7 +4655,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -4670,7 +4678,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -4693,7 +4701,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -4716,7 +4724,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -4739,7 +4747,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B75">
         <v>8</v>
@@ -4762,7 +4770,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B76">
         <v>8</v>
@@ -4785,7 +4793,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B77">
         <v>16</v>
@@ -4808,7 +4816,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B78">
         <v>16</v>
@@ -4831,7 +4839,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B79">
         <v>16</v>
@@ -4854,7 +4862,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B80">
         <v>16</v>
@@ -4877,7 +4885,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B81">
         <v>16</v>
@@ -4900,7 +4908,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B82">
         <v>16</v>
@@ -4923,7 +4931,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B83">
         <v>16</v>
@@ -4946,7 +4954,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -4966,7 +4974,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -4986,7 +4994,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -5006,7 +5014,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -5026,7 +5034,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -5046,7 +5054,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -5066,7 +5074,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -5086,7 +5094,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -5106,7 +5114,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -5126,7 +5134,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B93">
         <v>4</v>
@@ -5146,7 +5154,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B94">
         <v>4</v>
@@ -5166,7 +5174,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -5188,6 +5196,7 @@
       <c r="A98" s="1"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -5219,45 +5228,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="26" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5272,7 +5281,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I6" s="17">
         <v>221.43898490266665</v>
@@ -5280,7 +5289,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5296,7 +5305,7 @@
       </c>
       <c r="G7" s="32"/>
       <c r="H7" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I7" s="21">
         <v>27.888301147358074</v>
@@ -5304,7 +5313,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5320,7 +5329,7 @@
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I8" s="21">
         <v>6</v>
@@ -5328,7 +5337,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5346,7 +5355,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I9" s="17">
         <v>230.1513251065</v>
@@ -5354,7 +5363,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5370,7 +5379,7 @@
       </c>
       <c r="G10" s="32"/>
       <c r="H10" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I10" s="21">
         <v>21.442701960879447</v>
@@ -5378,7 +5387,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5394,7 +5403,7 @@
       </c>
       <c r="G11" s="32"/>
       <c r="H11" s="18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I11" s="21">
         <v>4</v>
@@ -5402,7 +5411,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -5420,7 +5429,7 @@
         <v>8</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I12" s="17">
         <v>524.47522211100011</v>
@@ -5428,7 +5437,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -5444,7 +5453,7 @@
       </c>
       <c r="G13" s="32"/>
       <c r="H13" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I13" s="21">
         <v>249.37176975472715</v>
@@ -5452,7 +5461,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -5468,7 +5477,7 @@
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I14" s="21">
         <v>32</v>
@@ -5476,7 +5485,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -5494,7 +5503,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I15" s="17">
         <v>338.08045351500004</v>
@@ -5502,7 +5511,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -5518,7 +5527,7 @@
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I16" s="21">
         <v>46.784586737362908</v>
@@ -5526,7 +5535,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -5542,7 +5551,7 @@
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I17" s="21">
         <v>16</v>
@@ -5550,7 +5559,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -5565,7 +5574,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H18" s="33"/>
       <c r="I18" s="17">
@@ -5574,7 +5583,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -5589,7 +5598,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H19" s="33"/>
       <c r="I19" s="17">
@@ -5598,7 +5607,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -5613,7 +5622,7 @@
         <v>0.75</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H20" s="34"/>
       <c r="I20" s="25">
@@ -5622,7 +5631,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -5639,7 +5648,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -5656,7 +5665,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -5673,7 +5682,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -5690,7 +5699,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B25">
         <v>16</v>
@@ -5707,19 +5716,19 @@
     </row>
     <row r="26" spans="1:10">
       <c r="C26" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D26" s="2">
         <f>AVERAGE(D6:D25)</f>
         <v>373.44653231864999</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="C27" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D27" s="2">
         <f>STDEV(D6:D25)</f>
@@ -5729,42 +5738,42 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="26" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B29" s="26"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -5782,7 +5791,7 @@
         <v>2</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J31" s="17">
         <v>302.94028916180002</v>
@@ -5790,7 +5799,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -5807,7 +5816,7 @@
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
       <c r="I32" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J32" s="21">
         <v>17.23574117758357</v>
@@ -5815,7 +5824,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -5830,7 +5839,7 @@
         <v>0.5625</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H33" s="33"/>
       <c r="I33" s="33"/>
@@ -5840,7 +5849,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -5855,7 +5864,7 @@
         <v>0.89513888888888893</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -5865,7 +5874,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5886,7 +5895,7 @@
         <v>4</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J35" s="17">
         <v>305.19036102299998</v>
@@ -5894,7 +5903,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -5912,7 +5921,7 @@
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
       <c r="I36" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J36" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5920,7 +5929,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -5936,7 +5945,7 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H37" s="33"/>
       <c r="I37" s="33"/>
@@ -5946,7 +5955,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -5962,7 +5971,7 @@
         <v>0.57916666666666672</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H38" s="33"/>
       <c r="I38" s="33"/>
@@ -5972,7 +5981,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -5994,7 +6003,7 @@
         <v>8</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J39" s="17">
         <v>384.05235557549997</v>
@@ -6002,7 +6011,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -6020,7 +6029,7 @@
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
       <c r="I40" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J40" s="21">
         <v>32.66972061151673</v>
@@ -6028,7 +6037,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -6044,7 +6053,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="33"/>
@@ -6054,7 +6063,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -6069,7 +6078,7 @@
         <v>0.70972222222222225</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H42" s="33"/>
       <c r="I42" s="33"/>
@@ -6079,7 +6088,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -6094,7 +6103,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
@@ -6104,7 +6113,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -6119,7 +6128,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -6129,7 +6138,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -6146,7 +6155,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -6163,7 +6172,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -6178,19 +6187,19 @@
     </row>
     <row r="48" spans="1:10">
       <c r="C48" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D48" s="2">
         <f>AVERAGE(D30:D47)</f>
         <v>356.83130192700003</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="C49" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D49" s="2">
         <f>STDEV(D31:D47)</f>
@@ -6207,40 +6216,40 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="26" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B52" s="26"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H53" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B53" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G53" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="H53" s="11" t="s">
-        <v>142</v>
-      </c>
       <c r="I53" s="14" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -6258,7 +6267,7 @@
         <v>4</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I54" s="17">
         <v>14.1872649193</v>
@@ -6266,7 +6275,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -6282,7 +6291,7 @@
       </c>
       <c r="G55" s="32"/>
       <c r="H55" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I55" s="21" t="e">
         <v>#DIV/0!</v>
@@ -6290,7 +6299,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -6308,7 +6317,7 @@
         <v>8</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I56" s="17">
         <v>44.782275199920001</v>
@@ -6316,7 +6325,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -6332,7 +6341,7 @@
       </c>
       <c r="G57" s="32"/>
       <c r="H57" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I57" s="21">
         <v>15.843792242505828</v>
@@ -6340,7 +6349,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -6358,7 +6367,7 @@
         <v>16</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I58" s="17">
         <v>56.964924156674996</v>
@@ -6366,7 +6375,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -6382,7 +6391,7 @@
       </c>
       <c r="G59" s="32"/>
       <c r="H59" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I59" s="21">
         <v>9.4994883808250847</v>
@@ -6390,7 +6399,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -6408,7 +6417,7 @@
         <v>32</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I60" s="17">
         <v>187.55037531850999</v>
@@ -6416,7 +6425,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -6432,7 +6441,7 @@
       </c>
       <c r="G61" s="32"/>
       <c r="H61" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I61" s="21">
         <v>179.97433590633514</v>
@@ -6440,7 +6449,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -6455,7 +6464,7 @@
         <v>0.59236111111111112</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H62" s="33"/>
       <c r="I62" s="17">
@@ -6464,7 +6473,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -6479,7 +6488,7 @@
         <v>0.61875000000000002</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H63" s="34"/>
       <c r="I63" s="25">
@@ -6488,7 +6497,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B64">
         <v>8</v>
@@ -6505,7 +6514,7 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -6522,7 +6531,7 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -6539,7 +6548,7 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B67">
         <v>8</v>
@@ -6556,7 +6565,7 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B68">
         <v>8</v>
@@ -6573,7 +6582,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -6590,7 +6599,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B70">
         <v>8</v>
@@ -6607,7 +6616,7 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -6624,7 +6633,7 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -6641,7 +6650,7 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -6656,36 +6665,36 @@
     </row>
     <row r="74" spans="1:10">
       <c r="C74" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D74" s="2">
         <f>AVERAGE(D54:D73)</f>
         <v>117.073104536535</v>
       </c>
       <c r="E74" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H74" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I74" s="55">
         <f>AVERAGE(D54:D63,D65:D66,D68:D70,D73)</f>
         <v>53.003791779293749</v>
       </c>
       <c r="J74" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="C75" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D75" s="2">
         <f>STDEV(D54:D73)</f>
         <v>143.93518726021225</v>
       </c>
       <c r="H75" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I75" s="55">
         <f>STDEV(D54:D63,D65:D66,D68:D70,D73)</f>
@@ -6701,26 +6710,26 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="26" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C80" s="26" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -6734,7 +6743,7 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B82">
         <v>4</v>
@@ -6748,7 +6757,7 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B83">
         <v>8</v>
@@ -6762,7 +6771,7 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B84">
         <v>16</v>
@@ -6776,7 +6785,7 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -6790,7 +6799,7 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B86">
         <v>2</v>
@@ -6804,7 +6813,7 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B87">
         <v>2</v>
@@ -6818,7 +6827,7 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B88">
         <v>2</v>
@@ -6832,7 +6841,7 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -6846,7 +6855,7 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -6860,7 +6869,7 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -6874,7 +6883,7 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -6888,7 +6897,7 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B93">
         <v>2</v>
@@ -6902,7 +6911,7 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -6920,7 +6929,7 @@
         <v>331.21428571428572</v>
       </c>
       <c r="E95" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -6968,69 +6977,69 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="28" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="30" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" ht="39" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C5" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>126</v>
-      </c>
       <c r="G5" s="29" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K5" s="28" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M5" s="28" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -7065,13 +7074,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -7106,13 +7115,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B8" s="31">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -7147,7 +7156,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -7185,7 +7194,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -7220,7 +7229,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>32</v>
@@ -7261,7 +7270,7 @@
     </row>
     <row r="12" spans="1:14" s="49" customFormat="1" ht="14" thickBot="1">
       <c r="A12" s="49" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B12" s="49">
         <v>32</v>
@@ -7302,7 +7311,7 @@
     </row>
     <row r="13" spans="1:14" ht="40" thickTop="1">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -7333,12 +7342,12 @@
         <v>2</v>
       </c>
       <c r="N13" s="52" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="39">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -7369,12 +7378,12 @@
         <v>2</v>
       </c>
       <c r="N14" s="52" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="39">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" s="41">
         <v>16</v>
@@ -7405,12 +7414,12 @@
         <v>1</v>
       </c>
       <c r="N15" s="52" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="39">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -7441,12 +7450,12 @@
         <v>0</v>
       </c>
       <c r="N16" s="52" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>32</v>
@@ -7479,7 +7488,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>32</v>
@@ -7512,7 +7521,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>32</v>
@@ -7551,13 +7560,13 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="28" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -7579,8 +7588,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="S55" sqref="S55"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -7590,17 +7599,17 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="56" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -7608,7 +7617,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -7616,39 +7625,39 @@
     </row>
     <row r="8" spans="1:10" s="58" customFormat="1" ht="39">
       <c r="A8" s="29" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B8" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="57" t="s">
-        <v>78</v>
-      </c>
-      <c r="H8" s="57" t="s">
-        <v>79</v>
-      </c>
       <c r="I8" s="57" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J8" s="58" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="58" customFormat="1">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -7660,7 +7669,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -7680,7 +7689,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -7693,7 +7702,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F10">
         <v>8</v>
@@ -7713,7 +7722,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -7726,7 +7735,7 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F11">
         <v>8</v>
@@ -7743,7 +7752,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>8</v>
@@ -7752,7 +7761,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:D23" si="0">C12*2</f>
+        <f t="shared" ref="D12:D26" si="0">C12*2</f>
         <v>0</v>
       </c>
       <c r="E12" s="59" t="s">
@@ -7776,7 +7785,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -7789,7 +7798,7 @@
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F13">
         <v>16</v>
@@ -7809,7 +7818,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -7822,7 +7831,7 @@
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F14">
         <v>8</v>
@@ -7842,7 +7851,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>8</v>
@@ -7855,7 +7864,7 @@
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F15">
         <v>8</v>
@@ -7875,7 +7884,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>8</v>
@@ -7888,7 +7897,7 @@
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F16">
         <v>8</v>
@@ -7908,7 +7917,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>8</v>
@@ -7921,7 +7930,7 @@
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F17">
         <v>8</v>
@@ -7941,7 +7950,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -7954,7 +7963,7 @@
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F18">
         <v>8</v>
@@ -7974,7 +7983,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B19">
         <v>8</v>
@@ -7987,7 +7996,7 @@
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F19">
         <v>8</v>
@@ -8007,7 +8016,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -8020,7 +8029,7 @@
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F20">
         <v>8</v>
@@ -8040,7 +8049,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B21">
         <v>8</v>
@@ -8053,7 +8062,7 @@
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F21">
         <v>8</v>
@@ -8073,7 +8082,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -8086,7 +8095,7 @@
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F22">
         <v>8</v>
@@ -8106,7 +8115,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -8119,7 +8128,7 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F23">
         <v>8</v>
@@ -8137,7 +8146,114 @@
         <v>543.97266197199997</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24">
+        <v>8</v>
+      </c>
+      <c r="G24">
+        <v>4</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+      <c r="J24" s="55">
+        <v>866.94245719900005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25">
+        <v>8</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>4</v>
+      </c>
+      <c r="J25" s="55">
+        <v>529.44632291799996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <v>8</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>4</v>
+      </c>
+      <c r="J26" s="55">
+        <v>543.98205781000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" s="58" t="s">
         <v>1</v>
       </c>
@@ -8146,7 +8262,7 @@
         <v>1027.9399099300001</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -8155,7 +8271,7 @@
         <v>1050.4892129899999</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="26">
+    <row r="56" spans="1:3" ht="26">
       <c r="A56" s="52" t="s">
         <v>3</v>
       </c>
@@ -8164,16 +8280,20 @@
         <v>1051.7398700700001</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="26">
+    <row r="57" spans="1:3" ht="26">
       <c r="A57" s="52" t="s">
         <v>4</v>
       </c>
       <c r="B57" s="55">
-        <f>J23</f>
-        <v>543.97266197199997</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="39">
+        <f>AVERAGE(J23:J26)</f>
+        <v>621.08587497474991</v>
+      </c>
+      <c r="C57">
+        <f>STDEV(J23:J26)</f>
+        <v>164.04746545348206</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="39">
       <c r="A58" s="52" t="s">
         <v>5</v>
       </c>
@@ -8181,9 +8301,12 @@
         <f>AVERAGE(J14:J22)</f>
         <v>688.64166519366654</v>
       </c>
+      <c r="C58" s="55">
+        <f>STDEV(J14:J22)</f>
+        <v>20.480758532664797</v>
+      </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -8215,50 +8338,50 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="53" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="54" customFormat="1" ht="39">
       <c r="A5" s="54" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F5" s="54" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G5" s="54" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H5" s="54" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I5" s="54" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J5" s="54" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K5" s="54" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L5" s="54" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -8297,7 +8420,7 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -8408,7 +8531,7 @@
         <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -8447,7 +8570,7 @@
         <v>3</v>
       </c>
       <c r="L10" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -8685,7 +8808,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -8726,10 +8848,10 @@
   <sheetData>
     <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -8741,7 +8863,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="11" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
@@ -8765,12 +8887,12 @@
         <v>32</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
@@ -8787,7 +8909,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="18" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="20">
@@ -8804,7 +8926,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
@@ -8825,7 +8947,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="18" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B8" s="19">
         <v>2070.8984270000001</v>
@@ -8842,7 +8964,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B9" s="19">
         <v>1095.4940549999999</v>
@@ -8869,7 +8991,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="18" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
@@ -8890,7 +9012,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="18" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -8911,7 +9033,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B12" s="23">
         <v>1583.1962410000001</v>
@@ -8939,7 +9061,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
updated figures to conventions just discussed
git-svn-id: file://localhost/tmp/svn2git/svn@1928 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="-200" windowWidth="35980" windowHeight="21780" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="20" yWindow="-200" windowWidth="35980" windowHeight="21780" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NAMD Runtimes" sheetId="1" r:id="rId1"/>
@@ -30,41 +30,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="157">
   <si>
     <t>-</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>Grid 8/8</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Condor 8/8</t>
+    <t>Average</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stddev</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grid (Poseidon - adjusted)</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI 8/8</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Grid 8/6
-Nimbus 8/2</t>
+Science Cloud 8/2</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grid 8/4
+Condor Pool 8/3
+Science Cloud 8/1</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Condor Pool 8/8</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Grid 8/4 
-Condor 8/4</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Grid 8/4
-Condor 8/3
-Nimbus 8/1</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Average</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stddev</t>
+Condor Pool 8/4</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Science Cloud</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Condor Pool</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
@@ -101,18 +117,6 @@
   </si>
   <si>
     <t>Oliver</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Grid (Poseidon)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Grid (Poseidon - adjusted)</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Condor (Poseidon)</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
@@ -1044,33 +1048,30 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>('Setup Times'!$E$26,'Setup Times'!$E$48,'Setup Times'!$E$74,'Setup Times'!$J$74,'Setup Times'!$E$95)</c:f>
+              <c:f>('Setup Times'!$E$26,'Setup Times'!$E$48,'Setup Times'!$E$74,'Setup Times'!$E$95)</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>EC2 m1.large</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Nimbus</c:v>
+                  <c:v>Science Cloud</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Grid (Poseidon)</c:v>
+                  <c:v>LONI</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Grid (Poseidon - adjusted)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Condor (Poseidon)</c:v>
+                  <c:v>Condor Pool</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Setup Times'!$D$26,'Setup Times'!$D$48,'Setup Times'!$D$74,'Setup Times'!$I$74,'Setup Times'!$D$95)</c:f>
+              <c:f>('Setup Times'!$D$26,'Setup Times'!$D$48,'Setup Times'!$D$74,'Setup Times'!$D$95)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>373.44653231865</c:v>
                 </c:pt>
@@ -1080,10 +1081,7 @@
                 <c:pt idx="2">
                   <c:v>117.073104536535</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>53.00379177929375</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="3" formatCode="General">
                   <c:v>331.2142857142857</c:v>
                 </c:pt>
               </c:numCache>
@@ -1348,30 +1346,30 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Fixed!$A$54:$A$58</c:f>
+              <c:f>Fixed!$A$59:$A$63</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Grid 8/8</c:v>
+                  <c:v>LONI 8/8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Condor 8/8</c:v>
+                  <c:v>Condor Pool 8/8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Grid 8/6_x000d_Nimbus 8/2</c:v>
+                  <c:v>Grid 8/6_x000d_Science Cloud 8/2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Grid 8/4 _x000d_Condor 8/4</c:v>
+                  <c:v>Grid 8/4 _x000d_Condor Pool 8/4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Grid 8/4_x000d_Condor 8/3_x000d_Nimbus 8/1</c:v>
+                  <c:v>Grid 8/4_x000d_Condor Pool 8/3_x000d_Science Cloud 8/1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Fixed!$B$54:$B$58</c:f>
+              <c:f>Fixed!$B$59:$B$63</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1500,14 +1498,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1571,13 +1569,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>939800</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3182,12 +3180,12 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -3195,36 +3193,36 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="39">
       <c r="A4" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3244,7 +3242,7 @@
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -3264,7 +3262,7 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -3284,7 +3282,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3304,7 +3302,7 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -3324,7 +3322,7 @@
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -3344,7 +3342,7 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3364,7 +3362,7 @@
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -3384,7 +3382,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -3404,7 +3402,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3424,7 +3422,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3444,7 +3442,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -3464,7 +3462,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3484,7 +3482,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -3504,7 +3502,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -3524,7 +3522,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -3544,7 +3542,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3575,7 +3573,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3606,7 +3604,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -3637,7 +3635,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -3660,7 +3658,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -3683,7 +3681,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -3704,7 +3702,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -3725,7 +3723,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -3746,7 +3744,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -3767,7 +3765,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -3788,7 +3786,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -3809,7 +3807,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -3830,7 +3828,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -3851,7 +3849,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B34">
         <v>8</v>
@@ -3872,7 +3870,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B35">
         <v>8</v>
@@ -3893,7 +3891,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -3914,7 +3912,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -3935,7 +3933,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="44" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B38" s="44">
         <v>2</v>
@@ -3956,7 +3954,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -3977,7 +3975,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -3998,7 +3996,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -4019,7 +4017,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -4040,7 +4038,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -4061,7 +4059,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -4082,7 +4080,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -4103,7 +4101,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -4134,7 +4132,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -4165,7 +4163,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -4186,7 +4184,7 @@
     </row>
     <row r="49" spans="1:8" s="41" customFormat="1">
       <c r="A49" s="41" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B49" s="41">
         <v>2</v>
@@ -4207,7 +4205,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="39" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B50" s="39">
         <v>4</v>
@@ -4228,7 +4226,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -4249,7 +4247,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -4270,7 +4268,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -4291,7 +4289,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -4312,7 +4310,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -4333,7 +4331,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -4354,7 +4352,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -4375,7 +4373,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -4396,7 +4394,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B59">
         <v>15</v>
@@ -4417,7 +4415,7 @@
     </row>
     <row r="60" spans="1:8" hidden="1">
       <c r="A60" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -4438,7 +4436,7 @@
     </row>
     <row r="61" spans="1:8" hidden="1">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -4450,7 +4448,7 @@
     </row>
     <row r="62" spans="1:8" hidden="1">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -4462,7 +4460,7 @@
     </row>
     <row r="63" spans="1:8" hidden="1">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -4474,7 +4472,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -4495,7 +4493,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -4516,7 +4514,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -4547,7 +4545,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -4578,7 +4576,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -4609,7 +4607,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -4632,7 +4630,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -4655,7 +4653,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -4678,7 +4676,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -4701,7 +4699,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -4724,7 +4722,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -4747,7 +4745,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B75">
         <v>8</v>
@@ -4770,7 +4768,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B76">
         <v>8</v>
@@ -4793,7 +4791,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B77">
         <v>16</v>
@@ -4816,7 +4814,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B78">
         <v>16</v>
@@ -4839,7 +4837,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B79">
         <v>16</v>
@@ -4862,7 +4860,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B80">
         <v>16</v>
@@ -4885,7 +4883,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B81">
         <v>16</v>
@@ -4908,7 +4906,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B82">
         <v>16</v>
@@ -4931,7 +4929,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B83">
         <v>16</v>
@@ -4954,7 +4952,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -4974,7 +4972,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -4994,7 +4992,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -5014,7 +5012,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -5034,7 +5032,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -5054,7 +5052,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -5074,7 +5072,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -5094,7 +5092,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -5114,7 +5112,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -5134,7 +5132,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B93">
         <v>4</v>
@@ -5154,7 +5152,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B94">
         <v>4</v>
@@ -5174,7 +5172,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -5196,7 +5194,6 @@
       <c r="A98" s="1"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -5212,8 +5209,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E96" sqref="E96"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="P60" sqref="P60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -5228,45 +5225,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="E5" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>24</v>
-      </c>
       <c r="H5" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5281,7 +5278,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I6" s="17">
         <v>221.43898490266665</v>
@@ -5289,7 +5286,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5305,7 +5302,7 @@
       </c>
       <c r="G7" s="32"/>
       <c r="H7" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I7" s="21">
         <v>27.888301147358074</v>
@@ -5313,7 +5310,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5329,7 +5326,7 @@
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I8" s="21">
         <v>6</v>
@@ -5337,7 +5334,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5355,7 +5352,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I9" s="17">
         <v>230.1513251065</v>
@@ -5363,7 +5360,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5379,7 +5376,7 @@
       </c>
       <c r="G10" s="32"/>
       <c r="H10" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I10" s="21">
         <v>21.442701960879447</v>
@@ -5387,7 +5384,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5403,7 +5400,7 @@
       </c>
       <c r="G11" s="32"/>
       <c r="H11" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I11" s="21">
         <v>4</v>
@@ -5411,7 +5408,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -5429,7 +5426,7 @@
         <v>8</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I12" s="17">
         <v>524.47522211100011</v>
@@ -5437,7 +5434,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -5453,7 +5450,7 @@
       </c>
       <c r="G13" s="32"/>
       <c r="H13" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I13" s="21">
         <v>249.37176975472715</v>
@@ -5461,7 +5458,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -5477,7 +5474,7 @@
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I14" s="21">
         <v>32</v>
@@ -5485,7 +5482,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -5503,7 +5500,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I15" s="17">
         <v>338.08045351500004</v>
@@ -5511,7 +5508,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -5527,7 +5524,7 @@
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I16" s="21">
         <v>46.784586737362908</v>
@@ -5535,7 +5532,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -5551,7 +5548,7 @@
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I17" s="21">
         <v>16</v>
@@ -5559,7 +5556,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -5574,7 +5571,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H18" s="33"/>
       <c r="I18" s="17">
@@ -5583,7 +5580,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -5598,7 +5595,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H19" s="33"/>
       <c r="I19" s="17">
@@ -5607,7 +5604,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -5622,7 +5619,7 @@
         <v>0.75</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H20" s="34"/>
       <c r="I20" s="25">
@@ -5631,7 +5628,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -5648,7 +5645,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -5665,7 +5662,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -5682,7 +5679,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -5699,7 +5696,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25">
         <v>16</v>
@@ -5716,19 +5713,19 @@
     </row>
     <row r="26" spans="1:10">
       <c r="C26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D26" s="2">
         <f>AVERAGE(D6:D25)</f>
         <v>373.44653231864999</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="C27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D27" s="2">
         <f>STDEV(D6:D25)</f>
@@ -5738,42 +5735,42 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B29" s="26"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C30" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="E30" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -5791,7 +5788,7 @@
         <v>2</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J31" s="17">
         <v>302.94028916180002</v>
@@ -5799,7 +5796,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -5816,7 +5813,7 @@
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
       <c r="I32" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J32" s="21">
         <v>17.23574117758357</v>
@@ -5824,7 +5821,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -5839,7 +5836,7 @@
         <v>0.5625</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H33" s="33"/>
       <c r="I33" s="33"/>
@@ -5849,7 +5846,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -5864,7 +5861,7 @@
         <v>0.89513888888888893</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -5874,7 +5871,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5895,7 +5892,7 @@
         <v>4</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J35" s="17">
         <v>305.19036102299998</v>
@@ -5903,7 +5900,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -5921,7 +5918,7 @@
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
       <c r="I36" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J36" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5929,7 +5926,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -5945,7 +5942,7 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H37" s="33"/>
       <c r="I37" s="33"/>
@@ -5955,7 +5952,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -5971,7 +5968,7 @@
         <v>0.57916666666666672</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H38" s="33"/>
       <c r="I38" s="33"/>
@@ -5981,7 +5978,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -6003,7 +6000,7 @@
         <v>8</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="J39" s="17">
         <v>384.05235557549997</v>
@@ -6011,7 +6008,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -6029,7 +6026,7 @@
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
       <c r="I40" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J40" s="21">
         <v>32.66972061151673</v>
@@ -6037,7 +6034,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -6053,7 +6050,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="33"/>
@@ -6063,7 +6060,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -6078,7 +6075,7 @@
         <v>0.70972222222222225</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H42" s="33"/>
       <c r="I42" s="33"/>
@@ -6088,7 +6085,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -6103,7 +6100,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
@@ -6113,7 +6110,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -6128,7 +6125,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -6138,7 +6135,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -6155,7 +6152,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -6172,7 +6169,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -6187,19 +6184,19 @@
     </row>
     <row r="48" spans="1:10">
       <c r="C48" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D48" s="2">
         <f>AVERAGE(D30:D47)</f>
         <v>356.83130192700003</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="C49" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D49" s="2">
         <f>STDEV(D31:D47)</f>
@@ -6216,40 +6213,40 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="26" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B52" s="26"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="26" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C53" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E53" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="D53" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>121</v>
-      </c>
       <c r="G53" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -6267,7 +6264,7 @@
         <v>4</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I54" s="17">
         <v>14.1872649193</v>
@@ -6275,7 +6272,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -6291,7 +6288,7 @@
       </c>
       <c r="G55" s="32"/>
       <c r="H55" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I55" s="21" t="e">
         <v>#DIV/0!</v>
@@ -6299,7 +6296,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -6317,7 +6314,7 @@
         <v>8</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I56" s="17">
         <v>44.782275199920001</v>
@@ -6325,7 +6322,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -6341,7 +6338,7 @@
       </c>
       <c r="G57" s="32"/>
       <c r="H57" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I57" s="21">
         <v>15.843792242505828</v>
@@ -6349,7 +6346,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -6367,7 +6364,7 @@
         <v>16</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I58" s="17">
         <v>56.964924156674996</v>
@@ -6375,7 +6372,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -6391,7 +6388,7 @@
       </c>
       <c r="G59" s="32"/>
       <c r="H59" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I59" s="21">
         <v>9.4994883808250847</v>
@@ -6399,7 +6396,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -6417,7 +6414,7 @@
         <v>32</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I60" s="17">
         <v>187.55037531850999</v>
@@ -6425,7 +6422,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -6441,7 +6438,7 @@
       </c>
       <c r="G61" s="32"/>
       <c r="H61" s="18" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I61" s="21">
         <v>179.97433590633514</v>
@@ -6449,7 +6446,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -6464,7 +6461,7 @@
         <v>0.59236111111111112</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H62" s="33"/>
       <c r="I62" s="17">
@@ -6473,7 +6470,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -6488,7 +6485,7 @@
         <v>0.61875000000000002</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H63" s="34"/>
       <c r="I63" s="25">
@@ -6497,7 +6494,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B64">
         <v>8</v>
@@ -6514,7 +6511,7 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -6531,7 +6528,7 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -6548,7 +6545,7 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B67">
         <v>8</v>
@@ -6565,7 +6562,7 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B68">
         <v>8</v>
@@ -6582,7 +6579,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -6599,7 +6596,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B70">
         <v>8</v>
@@ -6616,7 +6613,7 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -6633,7 +6630,7 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -6650,7 +6647,7 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -6665,36 +6662,36 @@
     </row>
     <row r="74" spans="1:10">
       <c r="C74" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D74" s="2">
         <f>AVERAGE(D54:D73)</f>
         <v>117.073104536535</v>
       </c>
       <c r="E74" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="H74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I74" s="55">
         <f>AVERAGE(D54:D63,D65:D66,D68:D70,D73)</f>
         <v>53.003791779293749</v>
       </c>
       <c r="J74" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="C75" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D75" s="2">
         <f>STDEV(D54:D73)</f>
         <v>143.93518726021225</v>
       </c>
       <c r="H75" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I75" s="55">
         <f>STDEV(D54:D63,D65:D66,D68:D70,D73)</f>
@@ -6710,26 +6707,26 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="26" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C80" s="26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -6743,7 +6740,7 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B82">
         <v>4</v>
@@ -6757,7 +6754,7 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B83">
         <v>8</v>
@@ -6771,7 +6768,7 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B84">
         <v>16</v>
@@ -6785,7 +6782,7 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -6799,7 +6796,7 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B86">
         <v>2</v>
@@ -6813,7 +6810,7 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B87">
         <v>2</v>
@@ -6827,7 +6824,7 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B88">
         <v>2</v>
@@ -6841,7 +6838,7 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -6855,7 +6852,7 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -6869,7 +6866,7 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -6883,7 +6880,7 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -6897,7 +6894,7 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B93">
         <v>2</v>
@@ -6911,7 +6908,7 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -6929,7 +6926,7 @@
         <v>331.21428571428572</v>
       </c>
       <c r="E95" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -6977,69 +6974,69 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" ht="39" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B5" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>128</v>
-      </c>
       <c r="G5" s="29" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H5" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="29" t="s">
-        <v>63</v>
-      </c>
       <c r="J5" s="29" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K5" s="28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M5" s="28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -7074,13 +7071,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -7115,13 +7112,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" s="31">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -7156,7 +7153,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -7194,7 +7191,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -7229,7 +7226,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>32</v>
@@ -7270,7 +7267,7 @@
     </row>
     <row r="12" spans="1:14" s="49" customFormat="1" ht="14" thickBot="1">
       <c r="A12" s="49" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="49">
         <v>32</v>
@@ -7311,7 +7308,7 @@
     </row>
     <row r="13" spans="1:14" ht="40" thickTop="1">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -7342,12 +7339,12 @@
         <v>2</v>
       </c>
       <c r="N13" s="52" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="39">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -7378,12 +7375,12 @@
         <v>2</v>
       </c>
       <c r="N14" s="52" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="39">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" s="41">
         <v>16</v>
@@ -7414,12 +7411,12 @@
         <v>1</v>
       </c>
       <c r="N15" s="52" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="39">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -7450,12 +7447,12 @@
         <v>0</v>
       </c>
       <c r="N16" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>32</v>
@@ -7488,7 +7485,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>32</v>
@@ -7521,7 +7518,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>32</v>
@@ -7560,13 +7557,13 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -7586,10 +7583,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -7599,17 +7596,17 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="56" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -7617,7 +7614,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -7625,39 +7622,39 @@
     </row>
     <row r="8" spans="1:10" s="58" customFormat="1" ht="39">
       <c r="A8" s="29" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B8" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="57" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" s="57" t="s">
-        <v>81</v>
-      </c>
-      <c r="I8" s="57" t="s">
-        <v>82</v>
-      </c>
       <c r="J8" s="58" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="58" customFormat="1">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -7669,7 +7666,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -7689,7 +7686,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -7702,7 +7699,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F10">
         <v>8</v>
@@ -7722,7 +7719,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -7735,7 +7732,7 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F11">
         <v>8</v>
@@ -7752,7 +7749,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>8</v>
@@ -7761,7 +7758,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:D26" si="0">C12*2</f>
+        <f t="shared" ref="D12:D33" si="0">C12*2</f>
         <v>0</v>
       </c>
       <c r="E12" s="59" t="s">
@@ -7785,172 +7782,164 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>8</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
+        <v>0</v>
+      </c>
+      <c r="E13" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J13" s="55">
-        <v>985.09084010100003</v>
+        <v>1047.54509687</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>8</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E14" t="s">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="E14" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>3</v>
-      </c>
-      <c r="J14" s="55">
-        <v>692.35480594600006</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J14" s="55"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>8</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E15" t="s">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="E15" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>3</v>
-      </c>
-      <c r="J15" s="55">
-        <v>677.63002896299997</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J15" s="55"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>8</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="E16" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>3</v>
-      </c>
-      <c r="J16" s="55">
-        <v>736.197400808</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J16" s="55"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>8</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E17" t="s">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="E17" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>3</v>
-      </c>
-      <c r="J17" s="55">
-        <v>691.674695015</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J17" s="55"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -7963,27 +7952,27 @@
         <v>8</v>
       </c>
       <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18">
         <v>16</v>
       </c>
-      <c r="F18">
-        <v>8</v>
-      </c>
       <c r="G18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J18" s="55">
-        <v>691.32184195499997</v>
+        <v>985.09084010100003</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>8</v>
@@ -7996,7 +7985,7 @@
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F19">
         <v>8</v>
@@ -8011,12 +8000,12 @@
         <v>3</v>
       </c>
       <c r="J19" s="55">
-        <v>662.85133695599995</v>
+        <v>692.35480594600006</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -8029,7 +8018,7 @@
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F20">
         <v>8</v>
@@ -8044,12 +8033,12 @@
         <v>3</v>
       </c>
       <c r="J20" s="55">
-        <v>677.42435908300001</v>
+        <v>677.63002896299997</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <v>8</v>
@@ -8062,7 +8051,7 @@
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F21">
         <v>8</v>
@@ -8077,12 +8066,12 @@
         <v>3</v>
       </c>
       <c r="J21" s="55">
-        <v>676.69090104099996</v>
+        <v>736.197400808</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -8095,7 +8084,7 @@
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F22">
         <v>8</v>
@@ -8110,12 +8099,12 @@
         <v>3</v>
       </c>
       <c r="J22" s="55">
-        <v>691.62961697599997</v>
+        <v>691.674695015</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -8128,7 +8117,7 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F23">
         <v>8</v>
@@ -8137,18 +8126,18 @@
         <v>4</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J23" s="55">
-        <v>543.97266197199997</v>
+        <v>691.32184195499997</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B24">
         <v>8</v>
@@ -8161,7 +8150,7 @@
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F24">
         <v>8</v>
@@ -8170,18 +8159,18 @@
         <v>4</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J24" s="55">
-        <v>866.94245719900005</v>
+        <v>662.85133695599995</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B25">
         <v>8</v>
@@ -8194,7 +8183,7 @@
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F25">
         <v>8</v>
@@ -8203,18 +8192,18 @@
         <v>4</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J25" s="55">
-        <v>529.44632291799996</v>
+        <v>677.42435908300001</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B26">
         <v>8</v>
@@ -8227,7 +8216,7 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F26">
         <v>8</v>
@@ -8236,73 +8225,304 @@
         <v>4</v>
       </c>
       <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26" s="55">
+        <v>676.69090104099996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27">
+        <v>8</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>3</v>
+      </c>
+      <c r="J27" s="55">
+        <v>691.62961697599997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28">
+        <v>8</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+      <c r="H28">
         <v>0</v>
       </c>
-      <c r="I26">
-        <v>4</v>
-      </c>
-      <c r="J26" s="55">
+      <c r="I28">
+        <v>4</v>
+      </c>
+      <c r="J28" s="55">
+        <v>543.97266197199997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29">
+        <v>8</v>
+      </c>
+      <c r="G29">
+        <v>4</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>4</v>
+      </c>
+      <c r="J29" s="55">
+        <v>866.94245719900005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30">
+        <v>8</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>4</v>
+      </c>
+      <c r="J30" s="55">
+        <v>529.44632291799996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31">
+        <v>8</v>
+      </c>
+      <c r="G31">
+        <v>4</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>4</v>
+      </c>
+      <c r="J31" s="55">
         <v>543.98205781000001</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="B53" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="58" t="s">
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32">
+        <v>8</v>
+      </c>
+      <c r="G32">
+        <v>4</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>4</v>
+      </c>
+      <c r="J32" s="55">
+        <v>676.056340933</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33">
+        <v>8</v>
+      </c>
+      <c r="G33">
+        <v>4</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>4</v>
+      </c>
+      <c r="J33" s="55">
+        <v>735.39046001400004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="B58" t="s">
         <v>1</v>
       </c>
-      <c r="B54" s="55">
+      <c r="C58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="55">
         <f>J12</f>
         <v>1027.9399099300001</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>2</v>
-      </c>
-      <c r="B55" s="55">
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" s="55">
         <f>J10</f>
         <v>1050.4892129899999</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="26">
-      <c r="A56" s="52" t="s">
-        <v>3</v>
-      </c>
-      <c r="B56" s="55">
+    <row r="61" spans="1:3" ht="26">
+      <c r="A61" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="55">
         <f>J9</f>
         <v>1051.7398700700001</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="26">
-      <c r="A57" s="52" t="s">
-        <v>4</v>
-      </c>
-      <c r="B57" s="55">
-        <f>AVERAGE(J23:J26)</f>
+    <row r="62" spans="1:3" ht="26">
+      <c r="A62" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" s="55">
+        <f>AVERAGE(J28:J31)</f>
         <v>621.08587497474991</v>
       </c>
-      <c r="C57">
-        <f>STDEV(J23:J26)</f>
+      <c r="C62">
+        <f>STDEV(J28:J31)</f>
         <v>164.04746545348206</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="39">
-      <c r="A58" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58" s="55">
-        <f>AVERAGE(J14:J22)</f>
+    <row r="63" spans="1:3" ht="39">
+      <c r="A63" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="55">
+        <f>AVERAGE(J19:J27)</f>
         <v>688.64166519366654</v>
       </c>
-      <c r="C58" s="55">
-        <f>STDEV(J14:J22)</f>
+      <c r="C63" s="55">
+        <f>STDEV(J19:J27)</f>
         <v>20.480758532664797</v>
       </c>
     </row>
@@ -8311,7 +8531,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="B58" formulaRange="1"/>
+    <ignoredError sqref="B63" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
   <extLst>
@@ -8328,7 +8548,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="A6:H16"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -8338,50 +8558,50 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="53" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="54" customFormat="1" ht="39">
       <c r="A5" s="54" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F5" s="54" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G5" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="54" t="s">
-        <v>56</v>
-      </c>
       <c r="I5" s="54" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J5" s="54" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K5" s="54" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L5" s="54" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -8420,7 +8640,7 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -8531,7 +8751,7 @@
         <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -8570,7 +8790,7 @@
         <v>3</v>
       </c>
       <c r="L10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -8808,6 +9028,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -8848,10 +9069,10 @@
   <sheetData>
     <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -8863,7 +9084,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
@@ -8887,12 +9108,12 @@
         <v>32</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
@@ -8909,7 +9130,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="18" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="20">
@@ -8926,7 +9147,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
@@ -8947,7 +9168,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B8" s="19">
         <v>2070.8984270000001</v>
@@ -8964,7 +9185,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B9" s="19">
         <v>1095.4940549999999</v>
@@ -8991,7 +9212,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="18" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
@@ -9012,7 +9233,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="18" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -9033,7 +9254,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B12" s="23">
         <v>1583.1962410000001</v>
@@ -9061,6 +9282,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
referenced costs of running science in the cloud updated figure to new BigJob writing small stuff here and there
git-svn-id: file://localhost/tmp/svn2git/svn@1932 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="-200" windowWidth="35980" windowHeight="21780" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="-200" windowWidth="35980" windowHeight="21780" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NAMD Runtimes" sheetId="1" r:id="rId1"/>
@@ -52,35 +52,35 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>Grid 8/6
+    <t>Condor Pool 8/8</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Science Cloud</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Condor Pool</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI 8/6
 Science Cloud 8/2</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>Grid 8/4
+    <t>LONI 8/4 
+Condor Pool 8/4</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI 8/4
 Condor Pool 8/3
 Science Cloud 8/1</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Condor Pool 8/8</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Grid 8/4 
-Condor Pool 8/4</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Science Cloud</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>Condor Pool</t>
-    <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <t>LONI</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
@@ -1332,8 +1332,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.124673396389476"/>
-          <c:y val="0.0327626436670966"/>
+          <c:x val="0.132295347608988"/>
+          <c:y val="0.0303176558920355"/>
           <c:w val="0.858558310927597"/>
           <c:h val="0.78585410931213"/>
         </c:manualLayout>
@@ -1344,6 +1344,58 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Fixed!$C$59:$C$63</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>38.1596507066595</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>164.0474654534821</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>20.4807585326648</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Fixed!$C$59:$C$63</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>38.1596507066595</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>164.0474654534821</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>20.4807585326648</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Fixed!$A$59:$A$63</c:f>
@@ -1356,13 +1408,13 @@
                   <c:v>Condor Pool 8/8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Grid 8/6_x000d_Science Cloud 8/2</c:v>
+                  <c:v>LONI 8/6_x000d_Science Cloud 8/2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Grid 8/4 _x000d_Condor Pool 8/4</c:v>
+                  <c:v>LONI 8/4 _x000d_Condor Pool 8/4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Grid 8/4_x000d_Condor Pool 8/3_x000d_Science Cloud 8/1</c:v>
+                  <c:v>LONI 8/4_x000d_Condor Pool 8/3_x000d_Science Cloud 8/1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5194,6 +5246,7 @@
       <c r="A98" s="1"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -5209,8 +5262,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="P60" sqref="P60"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -6191,7 +6244,7 @@
         <v>356.83130192700003</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -6669,7 +6722,7 @@
         <v>117.073104536535</v>
       </c>
       <c r="E74" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H74" t="s">
         <v>85</v>
@@ -6926,7 +6979,7 @@
         <v>331.21428571428572</v>
       </c>
       <c r="E95" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -7585,8 +7638,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -7842,7 +7895,9 @@
       <c r="I14">
         <v>0</v>
       </c>
-      <c r="J14" s="55"/>
+      <c r="J14" s="55">
+        <v>1120.1365640199999</v>
+      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
@@ -7873,7 +7928,9 @@
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15" s="55"/>
+      <c r="J15" s="55">
+        <v>1028.1918029799999</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
@@ -7904,7 +7961,9 @@
       <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16" s="55"/>
+      <c r="J16" s="55">
+        <v>1046.0163061600001</v>
+      </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
@@ -8481,28 +8540,38 @@
         <f>J12</f>
         <v>1027.9399099300001</v>
       </c>
+      <c r="C59">
+        <f>STDEV(J12:J17)</f>
+        <v>38.159650706659498</v>
+      </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B60" s="55">
         <f>J10</f>
         <v>1050.4892129899999</v>
       </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:3" ht="26">
       <c r="A61" s="52" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B61" s="55">
         <f>J9</f>
         <v>1051.7398700700001</v>
       </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:3" ht="26">
       <c r="A62" s="52" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B62" s="55">
         <f>AVERAGE(J28:J31)</f>
@@ -8515,7 +8584,7 @@
     </row>
     <row r="63" spans="1:3" ht="39">
       <c r="A63" s="52" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B63" s="55">
         <f>AVERAGE(J19:J27)</f>
@@ -8527,6 +8596,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
try to get somehow a consistent spelling of Grid, Cloud, VM, etc.
git-svn-id: file://localhost/tmp/svn2git/svn@1933 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="157">
   <si>
     <t>-</t>
     <phoneticPr fontId="11" type="noConversion"/>
@@ -1349,15 +1349,15 @@
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>Fixed!$C$59:$C$63</c:f>
+                <c:f>Fixed!$C$64:$C$68</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>38.1596507066595</c:v>
+                    <c:v>66.50024881633016</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>291.3167352451899</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0.0</c:v>
@@ -1373,15 +1373,15 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Fixed!$C$59:$C$63</c:f>
+                <c:f>Fixed!$C$64:$C$68</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>38.1596507066595</c:v>
+                    <c:v>66.50024881633016</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>291.3167352451899</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0.0</c:v>
@@ -1398,7 +1398,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Fixed!$A$59:$A$63</c:f>
+              <c:f>Fixed!$A$64:$A$68</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1421,7 +1421,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Fixed!$B$59:$B$63</c:f>
+              <c:f>Fixed!$B$64:$B$68</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1429,7 +1429,7 @@
                   <c:v>1027.93990993</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1050.48921299</c:v>
+                  <c:v>1256.481251955</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1051.73987007</c:v>
@@ -1621,13 +1621,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>939800</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7636,10 +7636,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="O70" sqref="O70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -7778,11 +7778,11 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <f>C11*2</f>
-        <v>8</v>
+        <f t="shared" ref="D11:D15" si="0">C11*2</f>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
         <v>121</v>
@@ -7790,55 +7790,56 @@
       <c r="F11">
         <v>8</v>
       </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
       <c r="H11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J11" s="55">
-        <v>990.53072500200005</v>
+        <v>1462.47329092</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:D33" si="0">C12*2</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="59" t="s">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>121</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G12">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12" s="55">
-        <v>1027.9399099300001</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J12" s="55"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -7847,31 +7848,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E13" s="59" t="s">
-        <v>0</v>
+      <c r="E13" t="s">
+        <v>121</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G13">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13" s="55">
-        <v>1047.54509687</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J13" s="55"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -7880,31 +7879,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E14" s="59" t="s">
-        <v>0</v>
+      <c r="E14" t="s">
+        <v>121</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G14">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14" s="55">
-        <v>1120.1365640199999</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J14" s="55"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -7913,56 +7910,51 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E15" s="59" t="s">
-        <v>0</v>
+      <c r="E15" t="s">
+        <v>121</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G15">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15" s="55">
-        <v>1028.1918029799999</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J15" s="55"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B16">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="59" t="s">
-        <v>0</v>
+        <f>C16*2</f>
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>121</v>
       </c>
       <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
         <v>8</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J16" s="55">
-        <v>1046.0163061600001</v>
+        <v>990.53072500200005</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -7976,7 +7968,7 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D17:D38" si="1">C17*2</f>
         <v>0</v>
       </c>
       <c r="E17" s="59" t="s">
@@ -7994,7 +7986,9 @@
       <c r="I17">
         <v>0</v>
       </c>
-      <c r="J17" s="55"/>
+      <c r="J17" s="55">
+        <v>1027.9399099300001</v>
+      </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
@@ -8004,29 +7998,29 @@
         <v>8</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E18" t="s">
-        <v>19</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J18" s="55">
-        <v>985.09084010100003</v>
+        <v>1047.54509687</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -8037,29 +8031,29 @@
         <v>8</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E19" t="s">
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J19" s="55">
-        <v>692.35480594600006</v>
+        <v>1120.1365640199999</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -8070,29 +8064,29 @@
         <v>8</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E20" t="s">
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J20" s="55">
-        <v>677.63002896299997</v>
+        <v>1028.1918029799999</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -8103,29 +8097,29 @@
         <v>8</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E21" t="s">
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J21" s="55">
-        <v>736.197400808</v>
+        <v>1046.0163061600001</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -8136,29 +8130,29 @@
         <v>8</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E22" t="s">
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J22" s="55">
-        <v>691.674695015</v>
+        <v>1193.76627803</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -8172,26 +8166,26 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F23">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J23" s="55">
-        <v>691.32184195499997</v>
+        <v>985.09084010100003</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -8205,7 +8199,7 @@
         <v>4</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="E24" t="s">
@@ -8224,7 +8218,7 @@
         <v>3</v>
       </c>
       <c r="J24" s="55">
-        <v>662.85133695599995</v>
+        <v>692.35480594600006</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -8238,7 +8232,7 @@
         <v>4</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="E25" t="s">
@@ -8257,7 +8251,7 @@
         <v>3</v>
       </c>
       <c r="J25" s="55">
-        <v>677.42435908300001</v>
+        <v>677.63002896299997</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -8271,7 +8265,7 @@
         <v>4</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="E26" t="s">
@@ -8290,7 +8284,7 @@
         <v>3</v>
       </c>
       <c r="J26" s="55">
-        <v>676.69090104099996</v>
+        <v>736.197400808</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -8304,7 +8298,7 @@
         <v>4</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="E27" t="s">
@@ -8323,7 +8317,7 @@
         <v>3</v>
       </c>
       <c r="J27" s="55">
-        <v>691.62961697599997</v>
+        <v>691.674695015</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -8337,7 +8331,7 @@
         <v>4</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="E28" t="s">
@@ -8350,13 +8344,13 @@
         <v>4</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J28" s="55">
-        <v>543.97266197199997</v>
+        <v>691.32184195499997</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -8370,7 +8364,7 @@
         <v>4</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="E29" t="s">
@@ -8383,13 +8377,13 @@
         <v>4</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J29" s="55">
-        <v>866.94245719900005</v>
+        <v>662.85133695599995</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -8403,7 +8397,7 @@
         <v>4</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="E30" t="s">
@@ -8416,13 +8410,13 @@
         <v>4</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J30" s="55">
-        <v>529.44632291799996</v>
+        <v>677.42435908300001</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -8436,7 +8430,7 @@
         <v>4</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="E31" t="s">
@@ -8449,13 +8443,13 @@
         <v>4</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J31" s="55">
-        <v>543.98205781000001</v>
+        <v>676.69090104099996</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -8469,7 +8463,7 @@
         <v>4</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="E32" t="s">
@@ -8482,13 +8476,13 @@
         <v>4</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J32" s="55">
-        <v>676.056340933</v>
+        <v>691.62961697599997</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -8502,7 +8496,7 @@
         <v>4</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="E33" t="s">
@@ -8521,77 +8515,243 @@
         <v>4</v>
       </c>
       <c r="J33" s="55">
+        <v>543.97266197199997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34">
+        <v>8</v>
+      </c>
+      <c r="G34">
+        <v>4</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>4</v>
+      </c>
+      <c r="J34" s="55">
+        <v>866.94245719900005</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35">
+        <v>8</v>
+      </c>
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>4</v>
+      </c>
+      <c r="J35" s="55">
+        <v>529.44632291799996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36">
+        <v>8</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36">
+        <v>8</v>
+      </c>
+      <c r="G36">
+        <v>4</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>4</v>
+      </c>
+      <c r="J36" s="55">
+        <v>543.98205781000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37">
+        <v>8</v>
+      </c>
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>4</v>
+      </c>
+      <c r="J37" s="55">
+        <v>676.056340933</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38">
+        <v>8</v>
+      </c>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>4</v>
+      </c>
+      <c r="J38" s="55">
         <v>735.39046001400004</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
-      <c r="B58" t="s">
+    <row r="63" spans="1:3">
+      <c r="B63" t="s">
         <v>1</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C63" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" s="55">
-        <f>J12</f>
+    <row r="64" spans="1:3">
+      <c r="A64" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64" s="55">
+        <f>J17</f>
         <v>1027.9399099300001</v>
       </c>
-      <c r="C59">
-        <f>STDEV(J12:J17)</f>
-        <v>38.159650706659498</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
+      <c r="C64">
+        <f>STDEV(J17:J22)</f>
+        <v>66.500248816330156</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="55">
-        <f>J10</f>
-        <v>1050.4892129899999</v>
-      </c>
-      <c r="C60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="26">
-      <c r="A61" s="52" t="s">
+      <c r="B65" s="55">
+        <f>AVERAGE(J10:J15)</f>
+        <v>1256.4812519550001</v>
+      </c>
+      <c r="C65">
+        <f>STDEV(J10:J15)</f>
+        <v>291.31673524518988</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="26">
+      <c r="A66" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B61" s="55">
+      <c r="B66" s="55">
         <f>J9</f>
         <v>1051.7398700700001</v>
       </c>
-      <c r="C61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="26">
-      <c r="A62" s="52" t="s">
+      <c r="C66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="26">
+      <c r="A67" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B62" s="55">
-        <f>AVERAGE(J28:J31)</f>
+      <c r="B67" s="55">
+        <f>AVERAGE(J33:J36)</f>
         <v>621.08587497474991</v>
       </c>
-      <c r="C62">
-        <f>STDEV(J28:J31)</f>
+      <c r="C67">
+        <f>STDEV(J33:J36)</f>
         <v>164.04746545348206</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="39">
-      <c r="A63" s="52" t="s">
+    <row r="68" spans="1:3" ht="39">
+      <c r="A68" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="B63" s="55">
-        <f>AVERAGE(J19:J27)</f>
+      <c r="B68" s="55">
+        <f>AVERAGE(J24:J32)</f>
         <v>688.64166519366654</v>
       </c>
-      <c r="C63" s="55">
-        <f>STDEV(J19:J27)</f>
+      <c r="C68" s="55">
+        <f>STDEV(J24:J32)</f>
         <v>20.480758532664797</v>
       </c>
     </row>
@@ -8601,7 +8761,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="B63" formulaRange="1"/>
+    <ignoredError sqref="B68" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
   <extLst>

</xml_diff>

<commit_message>
Updated performance figures Updated Bib file Updated BigJob Cloud section
git-svn-id: file://localhost/tmp/svn2git/svn@1934 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="159">
   <si>
     <t>-</t>
     <phoneticPr fontId="11" type="noConversion"/>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>-</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
@@ -363,6 +366,9 @@
   <si>
     <t>Number Cores</t>
     <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Poseidon</t>
   </si>
   <si>
     <t>Average (drop maxima)</t>
@@ -1349,7 +1355,7 @@
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>Fixed!$C$64:$C$68</c:f>
+                <c:f>Fixed!$C$69:$C$73</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1357,10 +1363,10 @@
                     <c:v>66.50024881633016</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>291.3167352451899</c:v>
+                    <c:v>164.6223850037502</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0</c:v>
+                    <c:v>31.79494325424413</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>164.0474654534821</c:v>
@@ -1373,7 +1379,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Fixed!$C$64:$C$68</c:f>
+                <c:f>Fixed!$C$69:$C$73</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
@@ -1381,10 +1387,10 @@
                     <c:v>66.50024881633016</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>291.3167352451899</c:v>
+                    <c:v>164.6223850037502</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0</c:v>
+                    <c:v>31.79494325424413</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>164.0474654534821</c:v>
@@ -1398,7 +1404,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Fixed!$A$64:$A$68</c:f>
+              <c:f>Fixed!$A$69:$A$73</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1421,7 +1427,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Fixed!$B$64:$B$68</c:f>
+              <c:f>Fixed!$B$69:$B$73</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1429,10 +1435,10 @@
                   <c:v>1027.93990993</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1256.481251955</c:v>
+                  <c:v>1127.429073335</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1051.73987007</c:v>
+                  <c:v>1015.026539325333</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>621.08587497475</c:v>
@@ -1460,10 +1466,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600"/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1600"/>
+                  <a:rPr lang="de-DE" sz="2000"/>
                   <a:t>Resource #cores/#replicas</a:t>
                 </a:r>
               </a:p>
@@ -1502,10 +1508,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600"/>
+                  <a:defRPr sz="2000"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1600"/>
+                  <a:rPr lang="de-DE" sz="2000"/>
                   <a:t>Runtime (in sec)</a:t>
                 </a:r>
               </a:p>
@@ -1620,15 +1626,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>939800</xdr:colOff>
-      <xdr:row>89</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3232,12 +3238,12 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -3245,36 +3251,36 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="39">
       <c r="A4" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3294,7 +3300,7 @@
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -3314,7 +3320,7 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -3334,7 +3340,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3354,7 +3360,7 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -3374,7 +3380,7 @@
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -3394,7 +3400,7 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3414,7 +3420,7 @@
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -3434,7 +3440,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -3454,7 +3460,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3474,7 +3480,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3494,7 +3500,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -3514,7 +3520,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3534,7 +3540,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -3554,7 +3560,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -3574,7 +3580,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -3594,7 +3600,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3625,7 +3631,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3656,7 +3662,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -3687,7 +3693,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -3710,7 +3716,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -3733,7 +3739,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -3754,7 +3760,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -3775,7 +3781,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -3796,7 +3802,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -3817,7 +3823,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -3838,7 +3844,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -3859,7 +3865,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -3880,7 +3886,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -3901,7 +3907,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B34">
         <v>8</v>
@@ -3922,7 +3928,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B35">
         <v>8</v>
@@ -3943,7 +3949,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -3964,7 +3970,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -3985,7 +3991,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="44" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B38" s="44">
         <v>2</v>
@@ -4006,7 +4012,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -4027,7 +4033,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -4048,7 +4054,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -4069,7 +4075,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -4090,7 +4096,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -4111,7 +4117,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -4132,7 +4138,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -4153,7 +4159,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -4184,7 +4190,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -4215,7 +4221,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -4236,7 +4242,7 @@
     </row>
     <row r="49" spans="1:8" s="41" customFormat="1">
       <c r="A49" s="41" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B49" s="41">
         <v>2</v>
@@ -4257,7 +4263,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="39" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B50" s="39">
         <v>4</v>
@@ -4278,7 +4284,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -4299,7 +4305,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -4320,7 +4326,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -4341,7 +4347,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -4362,7 +4368,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -4383,7 +4389,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -4404,7 +4410,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -4425,7 +4431,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -4446,7 +4452,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B59">
         <v>15</v>
@@ -4467,7 +4473,7 @@
     </row>
     <row r="60" spans="1:8" hidden="1">
       <c r="A60" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -4488,7 +4494,7 @@
     </row>
     <row r="61" spans="1:8" hidden="1">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -4500,7 +4506,7 @@
     </row>
     <row r="62" spans="1:8" hidden="1">
       <c r="A62" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -4512,7 +4518,7 @@
     </row>
     <row r="63" spans="1:8" hidden="1">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -4524,7 +4530,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -4545,7 +4551,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -4566,7 +4572,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -4597,7 +4603,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -4628,7 +4634,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -4659,7 +4665,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -4682,7 +4688,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -4705,7 +4711,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -4728,7 +4734,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -4751,7 +4757,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -4774,7 +4780,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -4797,7 +4803,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B75">
         <v>8</v>
@@ -4820,7 +4826,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B76">
         <v>8</v>
@@ -4843,7 +4849,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B77">
         <v>16</v>
@@ -4866,7 +4872,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B78">
         <v>16</v>
@@ -4889,7 +4895,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B79">
         <v>16</v>
@@ -4912,7 +4918,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B80">
         <v>16</v>
@@ -4935,7 +4941,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B81">
         <v>16</v>
@@ -4958,7 +4964,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B82">
         <v>16</v>
@@ -4981,7 +4987,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B83">
         <v>16</v>
@@ -5004,7 +5010,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -5024,7 +5030,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -5044,7 +5050,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -5064,7 +5070,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -5084,7 +5090,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -5104,7 +5110,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -5124,7 +5130,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -5144,7 +5150,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -5164,7 +5170,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -5184,7 +5190,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B93">
         <v>4</v>
@@ -5204,7 +5210,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B94">
         <v>4</v>
@@ -5224,7 +5230,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -5278,45 +5284,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="H5" s="11" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5331,7 +5337,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I6" s="17">
         <v>221.43898490266665</v>
@@ -5339,7 +5345,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5355,7 +5361,7 @@
       </c>
       <c r="G7" s="32"/>
       <c r="H7" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I7" s="21">
         <v>27.888301147358074</v>
@@ -5363,7 +5369,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5379,7 +5385,7 @@
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I8" s="21">
         <v>6</v>
@@ -5387,7 +5393,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5405,7 +5411,7 @@
         <v>4</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I9" s="17">
         <v>230.1513251065</v>
@@ -5413,7 +5419,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5429,7 +5435,7 @@
       </c>
       <c r="G10" s="32"/>
       <c r="H10" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I10" s="21">
         <v>21.442701960879447</v>
@@ -5437,7 +5443,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5453,7 +5459,7 @@
       </c>
       <c r="G11" s="32"/>
       <c r="H11" s="18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I11" s="21">
         <v>4</v>
@@ -5461,7 +5467,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -5479,7 +5485,7 @@
         <v>8</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I12" s="17">
         <v>524.47522211100011</v>
@@ -5487,7 +5493,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -5503,7 +5509,7 @@
       </c>
       <c r="G13" s="32"/>
       <c r="H13" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I13" s="21">
         <v>249.37176975472715</v>
@@ -5511,7 +5517,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -5527,7 +5533,7 @@
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I14" s="21">
         <v>32</v>
@@ -5535,7 +5541,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -5553,7 +5559,7 @@
         <v>16</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I15" s="17">
         <v>338.08045351500004</v>
@@ -5561,7 +5567,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -5577,7 +5583,7 @@
       </c>
       <c r="G16" s="32"/>
       <c r="H16" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I16" s="21">
         <v>46.784586737362908</v>
@@ -5585,7 +5591,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -5601,7 +5607,7 @@
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I17" s="21">
         <v>16</v>
@@ -5609,7 +5615,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -5624,7 +5630,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H18" s="33"/>
       <c r="I18" s="17">
@@ -5633,7 +5639,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -5648,7 +5654,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H19" s="33"/>
       <c r="I19" s="17">
@@ -5657,7 +5663,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -5672,7 +5678,7 @@
         <v>0.75</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H20" s="34"/>
       <c r="I20" s="25">
@@ -5681,7 +5687,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -5698,7 +5704,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -5715,7 +5721,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -5732,7 +5738,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -5749,7 +5755,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B25">
         <v>16</v>
@@ -5766,19 +5772,19 @@
     </row>
     <row r="26" spans="1:10">
       <c r="C26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D26" s="2">
         <f>AVERAGE(D6:D25)</f>
         <v>373.44653231864999</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="C27" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D27" s="2">
         <f>STDEV(D6:D25)</f>
@@ -5788,42 +5794,42 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B29" s="26"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="J30" s="14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -5841,7 +5847,7 @@
         <v>2</v>
       </c>
       <c r="I31" s="10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J31" s="17">
         <v>302.94028916180002</v>
@@ -5849,7 +5855,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -5866,7 +5872,7 @@
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
       <c r="I32" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J32" s="21">
         <v>17.23574117758357</v>
@@ -5874,7 +5880,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -5889,7 +5895,7 @@
         <v>0.5625</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H33" s="33"/>
       <c r="I33" s="33"/>
@@ -5899,7 +5905,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -5914,7 +5920,7 @@
         <v>0.89513888888888893</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -5924,7 +5930,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5945,7 +5951,7 @@
         <v>4</v>
       </c>
       <c r="I35" s="10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J35" s="17">
         <v>305.19036102299998</v>
@@ -5953,7 +5959,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -5971,7 +5977,7 @@
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
       <c r="I36" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J36" s="21" t="e">
         <v>#DIV/0!</v>
@@ -5979,7 +5985,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -5995,7 +6001,7 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H37" s="33"/>
       <c r="I37" s="33"/>
@@ -6005,7 +6011,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -6021,7 +6027,7 @@
         <v>0.57916666666666672</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H38" s="33"/>
       <c r="I38" s="33"/>
@@ -6031,7 +6037,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -6053,7 +6059,7 @@
         <v>8</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J39" s="17">
         <v>384.05235557549997</v>
@@ -6061,7 +6067,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -6079,7 +6085,7 @@
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
       <c r="I40" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J40" s="21">
         <v>32.66972061151673</v>
@@ -6087,7 +6093,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -6103,7 +6109,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="33"/>
@@ -6113,7 +6119,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -6128,7 +6134,7 @@
         <v>0.70972222222222225</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H42" s="33"/>
       <c r="I42" s="33"/>
@@ -6138,7 +6144,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -6153,7 +6159,7 @@
         <v>0.71388888888888891</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H43" s="33"/>
       <c r="I43" s="33"/>
@@ -6163,7 +6169,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -6178,7 +6184,7 @@
         <v>0.73749999999999993</v>
       </c>
       <c r="G44" s="22" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H44" s="34"/>
       <c r="I44" s="34"/>
@@ -6188,7 +6194,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -6205,7 +6211,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -6222,7 +6228,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -6237,7 +6243,7 @@
     </row>
     <row r="48" spans="1:10">
       <c r="C48" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D48" s="2">
         <f>AVERAGE(D30:D47)</f>
@@ -6249,7 +6255,7 @@
     </row>
     <row r="49" spans="1:9">
       <c r="C49" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D49" s="2">
         <f>STDEV(D31:D47)</f>
@@ -6266,40 +6272,40 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="26" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B52" s="26"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="H53" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="B53" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C53" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="G53" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="H53" s="11" t="s">
-        <v>145</v>
-      </c>
       <c r="I53" s="14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -6317,7 +6323,7 @@
         <v>4</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I54" s="17">
         <v>14.1872649193</v>
@@ -6325,7 +6331,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -6341,7 +6347,7 @@
       </c>
       <c r="G55" s="32"/>
       <c r="H55" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I55" s="21" t="e">
         <v>#DIV/0!</v>
@@ -6349,7 +6355,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -6367,7 +6373,7 @@
         <v>8</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I56" s="17">
         <v>44.782275199920001</v>
@@ -6375,7 +6381,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -6391,7 +6397,7 @@
       </c>
       <c r="G57" s="32"/>
       <c r="H57" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I57" s="21">
         <v>15.843792242505828</v>
@@ -6399,7 +6405,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -6417,7 +6423,7 @@
         <v>16</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I58" s="17">
         <v>56.964924156674996</v>
@@ -6425,7 +6431,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -6441,7 +6447,7 @@
       </c>
       <c r="G59" s="32"/>
       <c r="H59" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I59" s="21">
         <v>9.4994883808250847</v>
@@ -6449,7 +6455,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -6467,7 +6473,7 @@
         <v>32</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="I60" s="17">
         <v>187.55037531850999</v>
@@ -6475,7 +6481,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -6491,7 +6497,7 @@
       </c>
       <c r="G61" s="32"/>
       <c r="H61" s="18" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="I61" s="21">
         <v>179.97433590633514</v>
@@ -6499,7 +6505,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -6514,7 +6520,7 @@
         <v>0.59236111111111112</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H62" s="33"/>
       <c r="I62" s="17">
@@ -6523,7 +6529,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -6538,7 +6544,7 @@
         <v>0.61875000000000002</v>
       </c>
       <c r="G63" s="22" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H63" s="34"/>
       <c r="I63" s="25">
@@ -6547,7 +6553,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B64">
         <v>8</v>
@@ -6564,7 +6570,7 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -6581,7 +6587,7 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -6598,7 +6604,7 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B67">
         <v>8</v>
@@ -6615,7 +6621,7 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B68">
         <v>8</v>
@@ -6632,7 +6638,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -6649,7 +6655,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B70">
         <v>8</v>
@@ -6666,7 +6672,7 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -6683,7 +6689,7 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -6700,7 +6706,7 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -6715,7 +6721,7 @@
     </row>
     <row r="74" spans="1:10">
       <c r="C74" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D74" s="2">
         <f>AVERAGE(D54:D73)</f>
@@ -6725,7 +6731,7 @@
         <v>8</v>
       </c>
       <c r="H74" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I74" s="55">
         <f>AVERAGE(D54:D63,D65:D66,D68:D70,D73)</f>
@@ -6737,14 +6743,14 @@
     </row>
     <row r="75" spans="1:10">
       <c r="C75" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D75" s="2">
         <f>STDEV(D54:D73)</f>
         <v>143.93518726021225</v>
       </c>
       <c r="H75" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I75" s="55">
         <f>STDEV(D54:D63,D65:D66,D68:D70,D73)</f>
@@ -6760,26 +6766,26 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="26" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C80" s="26" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -6793,7 +6799,7 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B82">
         <v>4</v>
@@ -6807,7 +6813,7 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B83">
         <v>8</v>
@@ -6821,7 +6827,7 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B84">
         <v>16</v>
@@ -6835,7 +6841,7 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -6849,7 +6855,7 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B86">
         <v>2</v>
@@ -6863,7 +6869,7 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B87">
         <v>2</v>
@@ -6877,7 +6883,7 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B88">
         <v>2</v>
@@ -6891,7 +6897,7 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -6905,7 +6911,7 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -6919,7 +6925,7 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -6933,7 +6939,7 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -6947,7 +6953,7 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B93">
         <v>2</v>
@@ -6961,7 +6967,7 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -7027,69 +7033,69 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" ht="39" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C5" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>129</v>
-      </c>
       <c r="G5" s="29" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H5" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="29" t="s">
-        <v>64</v>
-      </c>
       <c r="J5" s="29" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K5" s="28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M5" s="28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -7124,13 +7130,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -7165,13 +7171,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" s="31">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -7206,7 +7212,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -7244,7 +7250,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -7279,7 +7285,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>32</v>
@@ -7320,7 +7326,7 @@
     </row>
     <row r="12" spans="1:14" s="49" customFormat="1" ht="14" thickBot="1">
       <c r="A12" s="49" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12" s="49">
         <v>32</v>
@@ -7361,7 +7367,7 @@
     </row>
     <row r="13" spans="1:14" ht="40" thickTop="1">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -7392,12 +7398,12 @@
         <v>2</v>
       </c>
       <c r="N13" s="52" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="39">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -7428,12 +7434,12 @@
         <v>2</v>
       </c>
       <c r="N14" s="52" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="39">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" s="41">
         <v>16</v>
@@ -7464,12 +7470,12 @@
         <v>1</v>
       </c>
       <c r="N15" s="52" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="39">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -7500,12 +7506,12 @@
         <v>0</v>
       </c>
       <c r="N16" s="52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>32</v>
@@ -7538,7 +7544,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>32</v>
@@ -7571,7 +7577,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>32</v>
@@ -7610,13 +7616,13 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -7636,15 +7642,16 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="O70" sqref="O70"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="O77" sqref="O77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -7654,12 +7661,12 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -7675,16 +7682,16 @@
     </row>
     <row r="8" spans="1:10" s="58" customFormat="1" ht="39">
       <c r="A8" s="29" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>13</v>
@@ -7693,13 +7700,13 @@
         <v>14</v>
       </c>
       <c r="G8" s="57" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H8" s="57" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I8" s="57" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J8" s="58" t="s">
         <v>17</v>
@@ -7707,7 +7714,7 @@
     </row>
     <row r="9" spans="1:10" s="58" customFormat="1">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -7719,7 +7726,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -7737,164 +7744,159 @@
         <v>1051.7398700700001</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" s="58" customFormat="1">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>123</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <f>C10*2</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="F10">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>8</v>
-      </c>
-      <c r="J10" s="55">
-        <v>1050.4892129899999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>2</v>
+      </c>
+      <c r="I10" s="60">
+        <v>0</v>
+      </c>
+      <c r="J10" s="51">
+        <v>996.53977489500005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="58" customFormat="1">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>123</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11:D15" si="0">C11*2</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="F11">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>8</v>
-      </c>
-      <c r="J11" s="55">
-        <v>1462.47329092</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>2</v>
+      </c>
+      <c r="I11" s="60">
+        <v>0</v>
+      </c>
+      <c r="J11" s="51">
+        <v>996.79997301100002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="58" customFormat="1">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>121</v>
+        <v>21</v>
       </c>
       <c r="F12">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>8</v>
-      </c>
-      <c r="J12" s="55"/>
-    </row>
-    <row r="13" spans="1:10">
+        <v>2</v>
+      </c>
+      <c r="I12" s="58">
+        <v>0</v>
+      </c>
+      <c r="J12" s="51"/>
+    </row>
+    <row r="13" spans="1:10" s="58" customFormat="1">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>123</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="F13">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>8</v>
-      </c>
-      <c r="J13" s="55"/>
-    </row>
-    <row r="14" spans="1:10">
+        <v>2</v>
+      </c>
+      <c r="I13" s="60">
+        <v>0</v>
+      </c>
+      <c r="J13" s="51"/>
+    </row>
+    <row r="14" spans="1:10" s="58" customFormat="1">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>123</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="F14">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>8</v>
-      </c>
-      <c r="J14" s="55"/>
+        <v>2</v>
+      </c>
+      <c r="I14" s="60">
+        <v>0</v>
+      </c>
+      <c r="J14" s="51"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
@@ -7907,11 +7909,11 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f>C15*2</f>
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F15">
         <v>8</v>
@@ -7925,7 +7927,9 @@
       <c r="I15">
         <v>8</v>
       </c>
-      <c r="J15" s="55"/>
+      <c r="J15" s="55">
+        <v>1050.4892129899999</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
@@ -7935,191 +7939,194 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <f>C16*2</f>
-        <v>8</v>
+        <f t="shared" ref="D16:D20" si="0">C16*2</f>
+        <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F16">
         <v>8</v>
       </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
       <c r="H16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J16" s="55">
-        <v>990.53072500200005</v>
+        <v>1040.42276812</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <f t="shared" ref="D17:D38" si="1">C17*2</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="59" t="s">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>123</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G17">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J17" s="55">
-        <v>1027.9399099300001</v>
+        <v>1462.47329092</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B18">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="59" t="s">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>123</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G18">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J18" s="55">
-        <v>1047.54509687</v>
+        <v>1070.3956189200001</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B19">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="59" t="s">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>123</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G19">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J19" s="55">
-        <v>1120.1365640199999</v>
+        <v>1070.4035170100001</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="59" t="s">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>123</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G20">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J20" s="55">
-        <v>1028.1918029799999</v>
+        <v>1070.3900320499999</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="59" t="s">
-        <v>0</v>
+        <f>C21*2</f>
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>123</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G21">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J21" s="55">
-        <v>1046.0163061600001</v>
+        <v>990.53072500200005</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -8133,7 +8140,7 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D22:D43" si="1">C22*2</f>
         <v>0</v>
       </c>
       <c r="E22" s="59" t="s">
@@ -8152,7 +8159,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="55">
-        <v>1193.76627803</v>
+        <v>1027.9399099300001</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -8163,29 +8170,29 @@
         <v>8</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>19</v>
+        <v>0</v>
+      </c>
+      <c r="E23" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J23" s="55">
-        <v>985.09084010100003</v>
+        <v>1047.54509687</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -8196,29 +8203,29 @@
         <v>8</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="E24" t="s">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="E24" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J24" s="55">
-        <v>692.35480594600006</v>
+        <v>1120.1365640199999</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -8229,29 +8236,29 @@
         <v>8</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="E25" t="s">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="E25" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J25" s="55">
-        <v>677.63002896299997</v>
+        <v>1028.1918029799999</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -8262,29 +8269,29 @@
         <v>8</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="E26" t="s">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="E26" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G26">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J26" s="55">
-        <v>736.197400808</v>
+        <v>1046.0163061600001</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -8295,29 +8302,29 @@
         <v>8</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D27">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="E27" t="s">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="E27" s="59" t="s">
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G27">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J27" s="55">
-        <v>691.674695015</v>
+        <v>1193.76627803</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -8335,22 +8342,22 @@
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F28">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G28">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J28" s="55">
-        <v>691.32184195499997</v>
+        <v>985.09084010100003</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -8383,7 +8390,7 @@
         <v>3</v>
       </c>
       <c r="J29" s="55">
-        <v>662.85133695599995</v>
+        <v>692.35480594600006</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -8416,7 +8423,7 @@
         <v>3</v>
       </c>
       <c r="J30" s="55">
-        <v>677.42435908300001</v>
+        <v>677.63002896299997</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -8449,7 +8456,7 @@
         <v>3</v>
       </c>
       <c r="J31" s="55">
-        <v>676.69090104099996</v>
+        <v>736.197400808</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -8482,7 +8489,7 @@
         <v>3</v>
       </c>
       <c r="J32" s="55">
-        <v>691.62961697599997</v>
+        <v>691.674695015</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -8509,13 +8516,13 @@
         <v>4</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J33" s="55">
-        <v>543.97266197199997</v>
+        <v>691.32184195499997</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -8542,13 +8549,13 @@
         <v>4</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J34" s="55">
-        <v>866.94245719900005</v>
+        <v>662.85133695599995</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -8575,13 +8582,13 @@
         <v>4</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J35" s="55">
-        <v>529.44632291799996</v>
+        <v>677.42435908300001</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -8608,13 +8615,13 @@
         <v>4</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J36" s="55">
-        <v>543.98205781000001</v>
+        <v>676.69090104099996</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -8641,13 +8648,13 @@
         <v>4</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J37" s="55">
-        <v>676.056340933</v>
+        <v>691.62961697599997</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -8680,78 +8687,244 @@
         <v>4</v>
       </c>
       <c r="J38" s="55">
+        <v>543.97266197199997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39">
+        <v>8</v>
+      </c>
+      <c r="G39">
+        <v>4</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>4</v>
+      </c>
+      <c r="J39" s="55">
+        <v>866.94245719900005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40">
+        <v>8</v>
+      </c>
+      <c r="G40">
+        <v>4</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>4</v>
+      </c>
+      <c r="J40" s="55">
+        <v>529.44632291799996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41">
+        <v>8</v>
+      </c>
+      <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>4</v>
+      </c>
+      <c r="J41" s="55">
+        <v>543.98205781000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42">
+        <v>8</v>
+      </c>
+      <c r="G42">
+        <v>4</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>4</v>
+      </c>
+      <c r="J42" s="55">
+        <v>676.056340933</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43">
+        <v>8</v>
+      </c>
+      <c r="G43">
+        <v>4</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>4</v>
+      </c>
+      <c r="J43" s="55">
         <v>735.39046001400004</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="B63" t="s">
+    <row r="68" spans="1:3">
+      <c r="B68" t="s">
         <v>1</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C68" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="B64" s="55">
-        <f>J17</f>
+    <row r="69" spans="1:3">
+      <c r="A69" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" s="55">
+        <f>J22</f>
         <v>1027.9399099300001</v>
       </c>
-      <c r="C64">
-        <f>STDEV(J17:J22)</f>
+      <c r="C69">
+        <f>STDEV(J22:J27)</f>
         <v>66.500248816330156</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
         <v>5</v>
       </c>
-      <c r="B65" s="55">
-        <f>AVERAGE(J10:J15)</f>
-        <v>1256.4812519550001</v>
-      </c>
-      <c r="C65">
-        <f>STDEV(J10:J15)</f>
-        <v>291.31673524518988</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="26">
-      <c r="A66" s="52" t="s">
+      <c r="B70" s="55">
+        <f>AVERAGE(J15:J20)</f>
+        <v>1127.4290733349999</v>
+      </c>
+      <c r="C70">
+        <f>STDEV(J15:J20)</f>
+        <v>164.62238500375017</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="26">
+      <c r="A71" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B66" s="55">
-        <f>J9</f>
-        <v>1051.7398700700001</v>
-      </c>
-      <c r="C66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="26">
-      <c r="A67" s="52" t="s">
+      <c r="B71" s="55">
+        <f>AVERAGE(J9:J14)</f>
+        <v>1015.0265393253334</v>
+      </c>
+      <c r="C71">
+        <f>STDEV(J9:J14)</f>
+        <v>31.794943254244128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="26">
+      <c r="A72" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B67" s="55">
-        <f>AVERAGE(J33:J36)</f>
+      <c r="B72" s="55">
+        <f>AVERAGE(J38:J41)</f>
         <v>621.08587497474991</v>
       </c>
-      <c r="C67">
-        <f>STDEV(J33:J36)</f>
+      <c r="C72">
+        <f>STDEV(J38:J41)</f>
         <v>164.04746545348206</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="39">
-      <c r="A68" s="52" t="s">
+    <row r="73" spans="1:3" ht="39">
+      <c r="A73" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="B68" s="55">
-        <f>AVERAGE(J24:J32)</f>
+      <c r="B73" s="55">
+        <f>AVERAGE(J29:J37)</f>
         <v>688.64166519366654</v>
       </c>
-      <c r="C68" s="55">
-        <f>STDEV(J24:J32)</f>
+      <c r="C73" s="55">
+        <f>STDEV(J29:J37)</f>
         <v>20.480758532664797</v>
       </c>
     </row>
@@ -8761,7 +8934,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="B68" formulaRange="1"/>
+    <ignoredError sqref="B73" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
   <extLst>
@@ -8788,50 +8961,50 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="53" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="54" customFormat="1" ht="39">
       <c r="A5" s="54" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F5" s="54" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G5" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="54" t="s">
-        <v>57</v>
-      </c>
       <c r="I5" s="54" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J5" s="54" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K5" s="54" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L5" s="54" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -8870,7 +9043,7 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -8981,7 +9154,7 @@
         <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -9020,7 +9193,7 @@
         <v>3</v>
       </c>
       <c r="L10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -9299,10 +9472,10 @@
   <sheetData>
     <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -9314,7 +9487,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="11" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
@@ -9338,12 +9511,12 @@
         <v>32</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
@@ -9360,7 +9533,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="18" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="20">
@@ -9377,7 +9550,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="18" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
@@ -9398,7 +9571,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="18" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B8" s="19">
         <v>2070.8984270000001</v>
@@ -9415,7 +9588,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B9" s="19">
         <v>1095.4940549999999</v>
@@ -9442,7 +9615,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="18" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
@@ -9463,7 +9636,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="18" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -9484,7 +9657,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="22" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B12" s="23">
         <v>1583.1962410000001</v>

</xml_diff>

<commit_message>
Added Condor runtimes figure Small changes here and there
git-svn-id: file://localhost/tmp/svn2git/svn@1941 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="161">
   <si>
     <t>Memory (in MB)</t>
     <phoneticPr fontId="12" type="noConversion"/>
@@ -80,6 +80,10 @@
   </si>
   <si>
     <t>-</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Science Cloud 8/8</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
@@ -1376,23 +1380,26 @@
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>Fixed!$C$74:$C$78</c:f>
+                <c:f>Fixed!$C$74:$C$79</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
+                  <c:ptCount val="6"/>
                   <c:pt idx="0">
+                    <c:v>4.808027173907892</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
                     <c:v>66.50024881633016</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="2">
                     <c:v>164.6223850037502</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>22.30811914346319</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>164.0474654534821</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>20.4807585326648</c:v>
                   </c:pt>
                 </c:numCache>
@@ -1400,23 +1407,26 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Fixed!$C$74:$C$78</c:f>
+                <c:f>Fixed!$C$74:$C$79</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
+                  <c:ptCount val="6"/>
                   <c:pt idx="0">
+                    <c:v>4.808027173907892</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
                     <c:v>66.50024881633016</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="2">
                     <c:v>164.6223850037502</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
                     <c:v>22.30811914346319</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>164.0474654534821</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>20.4807585326648</c:v>
                   </c:pt>
                 </c:numCache>
@@ -1425,22 +1435,25 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Fixed!$A$74:$A$78</c:f>
+              <c:f>Fixed!$A$74:$A$79</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>Science Cloud 8/8</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>LONI 8/8</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Condor Pool 8/8</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>LONI 8/6_x000d_Science Cloud 8/2</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>LONI 8/4 _x000d_Condor Pool 8/4</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>LONI 8/4_x000d_Condor Pool 8/3_x000d_Science Cloud 8/1</c:v>
                 </c:pt>
               </c:strCache>
@@ -1448,23 +1461,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Fixed!$B$74:$B$78</c:f>
+              <c:f>Fixed!$B$74:$B$79</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>2853.1651462325</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1027.93990993</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1127.429073335</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1008.339432994167</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>621.08587497475</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>688.6416651936665</c:v>
                 </c:pt>
               </c:numCache>
@@ -1504,7 +1520,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400"/>
+              <a:defRPr sz="1200"/>
             </a:pPr>
             <a:endParaRPr lang="de-DE"/>
           </a:p>
@@ -1654,7 +1670,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>825500</xdr:colOff>
-      <xdr:row>100</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3259,12 +3275,12 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -3272,36 +3288,36 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="39">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3321,7 +3337,7 @@
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -3341,7 +3357,7 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -3361,7 +3377,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3381,7 +3397,7 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -3401,7 +3417,7 @@
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -3421,7 +3437,7 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3441,7 +3457,7 @@
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -3461,7 +3477,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -3481,7 +3497,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3501,7 +3517,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3521,7 +3537,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -3541,7 +3557,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3561,7 +3577,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -3581,7 +3597,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -3601,7 +3617,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -3621,7 +3637,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3652,7 +3668,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3683,7 +3699,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -3714,7 +3730,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -3737,7 +3753,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -3760,7 +3776,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -3781,7 +3797,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -3802,7 +3818,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -3823,7 +3839,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -3844,7 +3860,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -3865,7 +3881,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -3886,7 +3902,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -3907,7 +3923,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -3928,7 +3944,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B34">
         <v>8</v>
@@ -3949,7 +3965,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B35">
         <v>8</v>
@@ -3970,7 +3986,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -3991,7 +4007,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -4012,7 +4028,7 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="44" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B38" s="44">
         <v>2</v>
@@ -4033,7 +4049,7 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -4054,7 +4070,7 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -4075,7 +4091,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -4096,7 +4112,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -4117,7 +4133,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -4138,7 +4154,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -4159,7 +4175,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -4180,7 +4196,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -4211,7 +4227,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -4242,7 +4258,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -4263,7 +4279,7 @@
     </row>
     <row r="49" spans="1:8" s="41" customFormat="1">
       <c r="A49" s="41" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B49" s="41">
         <v>2</v>
@@ -4284,7 +4300,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="39" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B50" s="39">
         <v>4</v>
@@ -4305,7 +4321,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -4326,7 +4342,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -4347,7 +4363,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -4368,7 +4384,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -4389,7 +4405,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -4410,7 +4426,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -4431,7 +4447,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -4452,7 +4468,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -4473,7 +4489,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B59">
         <v>15</v>
@@ -4494,7 +4510,7 @@
     </row>
     <row r="60" spans="1:8" hidden="1">
       <c r="A60" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -4515,7 +4531,7 @@
     </row>
     <row r="61" spans="1:8" hidden="1">
       <c r="A61" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -4527,7 +4543,7 @@
     </row>
     <row r="62" spans="1:8" hidden="1">
       <c r="A62" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -4539,7 +4555,7 @@
     </row>
     <row r="63" spans="1:8" hidden="1">
       <c r="A63" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -4551,7 +4567,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -4572,7 +4588,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -4593,7 +4609,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -4624,7 +4640,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -4655,7 +4671,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -4686,7 +4702,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -4709,7 +4725,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -4732,7 +4748,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -4755,7 +4771,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -4778,7 +4794,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -4801,7 +4817,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -4824,7 +4840,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B75">
         <v>8</v>
@@ -4847,7 +4863,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B76">
         <v>8</v>
@@ -4870,7 +4886,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B77">
         <v>16</v>
@@ -4893,7 +4909,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B78">
         <v>16</v>
@@ -4916,7 +4932,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B79">
         <v>16</v>
@@ -4939,7 +4955,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B80">
         <v>16</v>
@@ -4962,7 +4978,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B81">
         <v>16</v>
@@ -4985,7 +5001,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B82">
         <v>16</v>
@@ -5008,7 +5024,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B83">
         <v>16</v>
@@ -5031,7 +5047,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -5051,7 +5067,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -5071,7 +5087,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -5091,7 +5107,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -5111,7 +5127,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -5131,7 +5147,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -5151,7 +5167,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -5171,7 +5187,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -5191,7 +5207,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -5211,7 +5227,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B93">
         <v>4</v>
@@ -5231,7 +5247,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B94">
         <v>4</v>
@@ -5251,7 +5267,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -5304,33 +5320,33 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="E5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>119</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>118</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>2</v>
@@ -5342,7 +5358,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5365,7 +5381,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5389,7 +5405,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5405,7 +5421,7 @@
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I8" s="21">
         <v>6</v>
@@ -5413,7 +5429,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5439,7 +5455,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5463,7 +5479,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5479,7 +5495,7 @@
       </c>
       <c r="G11" s="32"/>
       <c r="H11" s="18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I11" s="21">
         <v>4</v>
@@ -5487,7 +5503,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -5513,7 +5529,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -5537,7 +5553,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -5553,7 +5569,7 @@
       </c>
       <c r="G14" s="32"/>
       <c r="H14" s="18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I14" s="21">
         <v>32</v>
@@ -5561,7 +5577,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -5587,7 +5603,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -5611,7 +5627,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -5627,7 +5643,7 @@
       </c>
       <c r="G17" s="32"/>
       <c r="H17" s="18" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I17" s="21">
         <v>16</v>
@@ -5635,7 +5651,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -5659,7 +5675,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -5683,7 +5699,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -5698,7 +5714,7 @@
         <v>0.75</v>
       </c>
       <c r="G20" s="22" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H20" s="34"/>
       <c r="I20" s="25">
@@ -5707,7 +5723,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -5724,7 +5740,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -5741,7 +5757,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -5758,7 +5774,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B24">
         <v>16</v>
@@ -5775,7 +5791,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B25">
         <v>16</v>
@@ -5792,19 +5808,19 @@
     </row>
     <row r="26" spans="1:10">
       <c r="C26" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D26" s="2">
         <f>AVERAGE(D6:D25)</f>
         <v>373.44653231864999</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="C27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D27" s="2">
         <f>STDEV(D6:D25)</f>
@@ -5814,31 +5830,31 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B29" s="26"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>51</v>
-      </c>
       <c r="E30" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G30" s="11" t="s">
         <v>1</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I30" s="11" t="s">
         <v>2</v>
@@ -5849,7 +5865,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -5875,7 +5891,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -5900,7 +5916,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -5915,7 +5931,7 @@
         <v>0.5625</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H33" s="33"/>
       <c r="I33" s="33"/>
@@ -5925,7 +5941,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -5940,7 +5956,7 @@
         <v>0.89513888888888893</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -5950,7 +5966,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5979,7 +5995,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -6005,7 +6021,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -6021,7 +6037,7 @@
         <v>0.96527777777777779</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H37" s="33"/>
       <c r="I37" s="33"/>
@@ -6031,7 +6047,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -6047,7 +6063,7 @@
         <v>0.57916666666666672</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H38" s="33"/>
       <c r="I38" s="33"/>
@@ -6057,7 +6073,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -6087,7 +6103,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -6113,7 +6129,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -6129,7 +6145,7 @@
         <v>0.67013888888888884</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H41" s="33"/>
       <c r="I41" s="33"/>
@@ -6139,7 +6155,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -6154,7 +6170,7 @@
         <v>0.70972222222222225</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H42" s="33"/>
       <c r="I42" s="33"/>
@@ -6164,7 +6180,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -6189,7 +6205,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -6214,7 +6230,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B45">
         <v>4</v>
@@ -6231,7 +6247,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B46">
         <v>4</v>
@@ -6248,7 +6264,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B47">
         <v>4</v>
@@ -6263,19 +6279,19 @@
     </row>
     <row r="48" spans="1:10">
       <c r="C48" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D48" s="2">
         <f>AVERAGE(D30:D47)</f>
         <v>356.83130192700003</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="C49" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D49" s="2">
         <f>STDEV(D31:D47)</f>
@@ -6292,7 +6308,7 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B52" s="26"/>
       <c r="D52" s="2"/>
@@ -6302,19 +6318,19 @@
         <v>4</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C53" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E53" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="D53" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>71</v>
-      </c>
       <c r="G53" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H53" s="11" t="s">
         <v>2</v>
@@ -6325,7 +6341,7 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -6351,7 +6367,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -6375,7 +6391,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -6401,7 +6417,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -6425,7 +6441,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -6451,7 +6467,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -6475,7 +6491,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -6501,7 +6517,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -6525,7 +6541,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -6549,7 +6565,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -6573,7 +6589,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B64">
         <v>8</v>
@@ -6590,7 +6606,7 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B65">
         <v>8</v>
@@ -6607,7 +6623,7 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B66">
         <v>8</v>
@@ -6624,7 +6640,7 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B67">
         <v>8</v>
@@ -6641,7 +6657,7 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B68">
         <v>8</v>
@@ -6658,7 +6674,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B69">
         <v>8</v>
@@ -6675,7 +6691,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B70">
         <v>8</v>
@@ -6692,7 +6708,7 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -6709,7 +6725,7 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -6726,7 +6742,7 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -6741,29 +6757,29 @@
     </row>
     <row r="74" spans="1:10">
       <c r="C74" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D74" s="2">
         <f>AVERAGE(D54:D73)</f>
         <v>117.073104536535</v>
       </c>
       <c r="E74" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H74" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I74" s="55">
         <f>AVERAGE(D54:D63,D65:D66,D68:D70,D73)</f>
         <v>53.003791779293749</v>
       </c>
       <c r="J74" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="C75" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D75" s="2">
         <f>STDEV(D54:D73)</f>
@@ -6794,18 +6810,18 @@
         <v>4</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C80" s="26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -6833,7 +6849,7 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B83">
         <v>8</v>
@@ -6847,7 +6863,7 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B84">
         <v>16</v>
@@ -6861,7 +6877,7 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -6875,7 +6891,7 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B86">
         <v>2</v>
@@ -6889,7 +6905,7 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B87">
         <v>2</v>
@@ -6903,7 +6919,7 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B88">
         <v>2</v>
@@ -6917,7 +6933,7 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -6931,7 +6947,7 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -6945,7 +6961,7 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -6959,7 +6975,7 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -6973,7 +6989,7 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B93">
         <v>2</v>
@@ -6987,7 +7003,7 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -7005,7 +7021,7 @@
         <v>331.21428571428572</v>
       </c>
       <c r="E95" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -7018,7 +7034,6 @@
       <c r="H109" s="2"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId4"/>
@@ -7052,69 +7067,69 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="28" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" ht="39" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B5" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>78</v>
-      </c>
       <c r="G5" s="29" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H5" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="I5" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="I5" s="29" t="s">
-        <v>157</v>
-      </c>
       <c r="J5" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K5" s="28" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L5" s="28" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M5" s="28" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -7149,13 +7164,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -7190,13 +7205,13 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B8" s="31">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -7231,7 +7246,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B9">
         <v>16</v>
@@ -7269,7 +7284,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -7304,7 +7319,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B11">
         <v>32</v>
@@ -7345,7 +7360,7 @@
     </row>
     <row r="12" spans="1:14" s="49" customFormat="1" ht="14" thickBot="1">
       <c r="A12" s="49" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B12" s="49">
         <v>32</v>
@@ -7386,7 +7401,7 @@
     </row>
     <row r="13" spans="1:14" ht="40" thickTop="1">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B13">
         <v>8</v>
@@ -7417,12 +7432,12 @@
         <v>2</v>
       </c>
       <c r="N13" s="52" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="39">
       <c r="A14" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -7453,12 +7468,12 @@
         <v>2</v>
       </c>
       <c r="N14" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="39">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B15" s="41">
         <v>16</v>
@@ -7489,12 +7504,12 @@
         <v>1</v>
       </c>
       <c r="N15" s="52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="39">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B16">
         <v>16</v>
@@ -7525,12 +7540,12 @@
         <v>0</v>
       </c>
       <c r="N16" s="52" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B17">
         <v>32</v>
@@ -7563,7 +7578,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B18">
         <v>32</v>
@@ -7596,7 +7611,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B19">
         <v>32</v>
@@ -7635,13 +7650,13 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="28" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -7660,10 +7675,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -7674,17 +7689,17 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="56" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -7692,7 +7707,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -7700,34 +7715,34 @@
     </row>
     <row r="8" spans="1:10" s="58" customFormat="1" ht="39">
       <c r="A8" s="29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B8" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="G8" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="57" t="s">
-        <v>31</v>
-      </c>
       <c r="J8" s="57" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="61" customFormat="1">
@@ -7822,7 +7837,9 @@
       <c r="I11" s="61">
         <v>0</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="51">
+        <v>2852.47939301</v>
+      </c>
     </row>
     <row r="12" spans="1:10" s="61" customFormat="1">
       <c r="A12" s="62" t="s">
@@ -7852,11 +7869,13 @@
       <c r="I12" s="61">
         <v>0</v>
       </c>
-      <c r="J12" s="51"/>
+      <c r="J12" s="51">
+        <v>2860.1625001399998</v>
+      </c>
     </row>
     <row r="13" spans="1:10" s="61" customFormat="1">
       <c r="A13" s="64" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B13" s="65">
         <v>0</v>
@@ -7868,7 +7887,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="64" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F13" s="65">
         <v>0</v>
@@ -7886,7 +7905,7 @@
     </row>
     <row r="14" spans="1:10" s="58" customFormat="1">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -7898,7 +7917,7 @@
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -7918,7 +7937,7 @@
     </row>
     <row r="15" spans="1:10" s="58" customFormat="1">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B15">
         <v>8</v>
@@ -7930,7 +7949,7 @@
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -7950,7 +7969,7 @@
     </row>
     <row r="16" spans="1:10" s="58" customFormat="1">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B16">
         <v>8</v>
@@ -7962,7 +7981,7 @@
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -7982,7 +8001,7 @@
     </row>
     <row r="17" spans="1:10" s="58" customFormat="1">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>8</v>
@@ -7994,7 +8013,7 @@
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -8014,7 +8033,7 @@
     </row>
     <row r="18" spans="1:10" s="58" customFormat="1">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -8026,7 +8045,7 @@
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -8046,7 +8065,7 @@
     </row>
     <row r="19" spans="1:10" s="58" customFormat="1">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B19">
         <v>8</v>
@@ -8058,7 +8077,7 @@
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -8078,7 +8097,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -8091,7 +8110,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F20">
         <v>8</v>
@@ -8111,7 +8130,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -8124,7 +8143,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F21">
         <v>8</v>
@@ -8144,7 +8163,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -8157,7 +8176,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F22">
         <v>8</v>
@@ -8177,7 +8196,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -8190,7 +8209,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F23">
         <v>8</v>
@@ -8210,7 +8229,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -8223,7 +8242,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F24">
         <v>8</v>
@@ -8243,7 +8262,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -8256,7 +8275,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F25">
         <v>8</v>
@@ -8276,7 +8295,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -8289,7 +8308,7 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F26">
         <v>8</v>
@@ -8309,7 +8328,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -8322,7 +8341,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="59" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -8342,7 +8361,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -8355,7 +8374,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="59" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -8375,7 +8394,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -8388,7 +8407,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="59" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -8408,7 +8427,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -8421,7 +8440,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="59" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -8441,7 +8460,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -8454,7 +8473,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="59" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -8474,7 +8493,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -8487,7 +8506,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="59" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -8507,7 +8526,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -8520,7 +8539,7 @@
         <v>8</v>
       </c>
       <c r="E33" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F33">
         <v>16</v>
@@ -8540,7 +8559,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B34">
         <v>8</v>
@@ -8553,7 +8572,7 @@
         <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F34">
         <v>8</v>
@@ -8573,7 +8592,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B35">
         <v>8</v>
@@ -8586,7 +8605,7 @@
         <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F35">
         <v>8</v>
@@ -8606,7 +8625,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -8619,7 +8638,7 @@
         <v>8</v>
       </c>
       <c r="E36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F36">
         <v>8</v>
@@ -8639,7 +8658,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -8652,7 +8671,7 @@
         <v>8</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F37">
         <v>8</v>
@@ -8672,7 +8691,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B38">
         <v>8</v>
@@ -8685,7 +8704,7 @@
         <v>8</v>
       </c>
       <c r="E38" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F38">
         <v>8</v>
@@ -8705,7 +8724,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B39">
         <v>8</v>
@@ -8718,7 +8737,7 @@
         <v>8</v>
       </c>
       <c r="E39" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F39">
         <v>8</v>
@@ -8738,7 +8757,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B40">
         <v>8</v>
@@ -8751,7 +8770,7 @@
         <v>8</v>
       </c>
       <c r="E40" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F40">
         <v>8</v>
@@ -8771,7 +8790,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B41">
         <v>8</v>
@@ -8784,7 +8803,7 @@
         <v>8</v>
       </c>
       <c r="E41" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F41">
         <v>8</v>
@@ -8804,7 +8823,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B42">
         <v>8</v>
@@ -8817,7 +8836,7 @@
         <v>8</v>
       </c>
       <c r="E42" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F42">
         <v>8</v>
@@ -8837,7 +8856,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B43">
         <v>8</v>
@@ -8850,7 +8869,7 @@
         <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F43">
         <v>8</v>
@@ -8870,7 +8889,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B44">
         <v>8</v>
@@ -8883,7 +8902,7 @@
         <v>8</v>
       </c>
       <c r="E44" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F44">
         <v>8</v>
@@ -8903,7 +8922,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B45">
         <v>8</v>
@@ -8916,7 +8935,7 @@
         <v>8</v>
       </c>
       <c r="E45" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F45">
         <v>8</v>
@@ -8936,7 +8955,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B46">
         <v>8</v>
@@ -8949,7 +8968,7 @@
         <v>8</v>
       </c>
       <c r="E46" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F46">
         <v>8</v>
@@ -8969,7 +8988,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B47">
         <v>8</v>
@@ -8982,7 +9001,7 @@
         <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F47">
         <v>8</v>
@@ -9002,7 +9021,7 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B48">
         <v>8</v>
@@ -9015,7 +9034,7 @@
         <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F48">
         <v>8</v>
@@ -9035,49 +9054,49 @@
     </row>
     <row r="73" spans="1:3">
       <c r="B73" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C73" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="58" t="s">
-        <v>96</v>
+      <c r="A74" t="s">
+        <v>15</v>
       </c>
       <c r="B74" s="55">
+        <f>AVERAGE(J9:J13)</f>
+        <v>2853.1651462324999</v>
+      </c>
+      <c r="C74">
+        <f>STDEV(J9:J13)</f>
+        <v>4.8080271739078917</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B75" s="55">
         <f>J27</f>
         <v>1027.9399099300001</v>
       </c>
-      <c r="C74">
+      <c r="C75">
         <f>STDEV(J27:J32)</f>
         <v>66.500248816330156</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>97</v>
-      </c>
-      <c r="B75" s="55">
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>98</v>
+      </c>
+      <c r="B76" s="55">
         <f>AVERAGE(J20:J25)</f>
         <v>1127.4290733349999</v>
       </c>
-      <c r="C75">
+      <c r="C76">
         <f>STDEV(J20:J25)</f>
         <v>164.62238500375017</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="26">
-      <c r="A76" s="52" t="s">
-        <v>101</v>
-      </c>
-      <c r="B76" s="55">
-        <f>AVERAGE(J14:J19)</f>
-        <v>1008.3394329941667</v>
-      </c>
-      <c r="C76">
-        <f>STDEV(J14:J19)</f>
-        <v>22.308119143463191</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="26">
@@ -9085,23 +9104,36 @@
         <v>102</v>
       </c>
       <c r="B77" s="55">
+        <f>AVERAGE(J14:J19)</f>
+        <v>1008.3394329941667</v>
+      </c>
+      <c r="C77">
+        <f>STDEV(J14:J19)</f>
+        <v>22.308119143463191</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="26">
+      <c r="A78" s="52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B78" s="55">
         <f>AVERAGE(J43:J46)</f>
         <v>621.08587497474991</v>
       </c>
-      <c r="C77">
+      <c r="C78">
         <f>STDEV(J43:J46)</f>
         <v>164.04746545348206</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="39">
-      <c r="A78" s="52" t="s">
-        <v>103</v>
-      </c>
-      <c r="B78" s="55">
+    <row r="79" spans="1:3" ht="39">
+      <c r="A79" s="52" t="s">
+        <v>104</v>
+      </c>
+      <c r="B79" s="55">
         <f>AVERAGE(J34:J42)</f>
         <v>688.64166519366654</v>
       </c>
-      <c r="C78" s="55">
+      <c r="C79" s="55">
         <f>STDEV(J34:J42)</f>
         <v>20.480758532664797</v>
       </c>
@@ -9112,7 +9144,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="B78" formulaRange="1"/>
+    <ignoredError sqref="B79" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId1"/>
   <extLst>
@@ -9139,50 +9171,50 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="53" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="54" customFormat="1" ht="39">
       <c r="A5" s="54" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F5" s="54" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G5" s="54" t="s">
+        <v>152</v>
+      </c>
+      <c r="H5" s="54" t="s">
         <v>151</v>
       </c>
-      <c r="H5" s="54" t="s">
-        <v>150</v>
-      </c>
       <c r="I5" s="54" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J5" s="54" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K5" s="54" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L5" s="54" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -9221,7 +9253,7 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -9332,7 +9364,7 @@
         <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -9371,7 +9403,7 @@
         <v>3</v>
       </c>
       <c r="L10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -9609,7 +9641,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -9650,10 +9681,10 @@
   <sheetData>
     <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -9665,7 +9696,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
@@ -9689,12 +9720,12 @@
         <v>32</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
@@ -9711,7 +9742,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="20">
@@ -9728,7 +9759,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
@@ -9749,7 +9780,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" s="19">
         <v>2070.8984270000001</v>
@@ -9766,7 +9797,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B9" s="19">
         <v>1095.4940549999999</v>
@@ -9793,7 +9824,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
@@ -9814,7 +9845,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -9835,7 +9866,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B12" s="23">
         <v>1583.1962410000001</v>

</xml_diff>

<commit_message>
larger fontsize of figure 8
git-svn-id: file://localhost/tmp/svn2git/svn@1955 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -87,6 +87,23 @@
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
+    <t>LONI 8/6
+Sci. Cloud 8/2</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI 8/4
+Condor Pool 8/3
+Sci. Cloud 8/1</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>LONI 8/4 
+Condor
+Pool 8/4</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
     <t>SAGA Pilot Sub-Job Runtime</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
@@ -418,22 +435,6 @@
   </si>
   <si>
     <t>LONI</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>LONI 8/6
-Science Cloud 8/2</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>LONI 8/4 
-Condor Pool 8/4</t>
-    <phoneticPr fontId="12" type="noConversion"/>
-  </si>
-  <si>
-    <t>LONI 8/4
-Condor Pool 8/3
-Science Cloud 8/1</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
   <si>
@@ -1448,13 +1449,13 @@
                   <c:v>Condor Pool 8/8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>LONI 8/6_x000d_Science Cloud 8/2</c:v>
+                  <c:v>LONI 8/6_x000d_Sci. Cloud 8/2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>LONI 8/4 _x000d_Condor Pool 8/4</c:v>
+                  <c:v>LONI 8/4 _x000d_Condor_x000d_Pool 8/4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>LONI 8/4_x000d_Condor Pool 8/3_x000d_Science Cloud 8/1</c:v>
+                  <c:v>LONI 8/4_x000d_Condor Pool 8/3_x000d_Sci. Cloud 8/1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1503,16 +1504,23 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000"/>
+                  <a:defRPr sz="2400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:rPr lang="de-DE" sz="2400"/>
                   <a:t>Resource #cores/#replicas</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.225245912411157"/>
+              <c:y val="0.932196162046908"/>
+            </c:manualLayout>
+          </c:layout>
         </c:title>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
@@ -1520,7 +1528,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1800"/>
             </a:pPr>
             <a:endParaRPr lang="de-DE"/>
           </a:p>
@@ -1545,10 +1553,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="2000"/>
+                  <a:defRPr sz="2400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="2000"/>
+                  <a:rPr lang="de-DE" sz="2400"/>
                   <a:t>Runtime (in sec)</a:t>
                 </a:r>
               </a:p>
@@ -1668,10 +1676,10 @@
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>825500</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3275,12 +3283,12 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>500</v>
@@ -3288,36 +3296,36 @@
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="39">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3337,7 +3345,7 @@
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -3357,7 +3365,7 @@
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -3377,7 +3385,7 @@
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3397,7 +3405,7 @@
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -3417,7 +3425,7 @@
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -3437,7 +3445,7 @@
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3457,7 +3465,7 @@
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -3477,7 +3485,7 @@
     </row>
     <row r="13" spans="1:9" s="4" customFormat="1">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -3497,7 +3505,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3517,7 +3525,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -3537,7 +3545,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -3557,7 +3565,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3577,7 +3585,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -3597,7 +3605,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -3617,7 +3625,7 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -3637,7 +3645,7 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3668,7 +3676,7 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3699,7 +3707,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -3730,7 +3738,7 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -3753,7 +3761,7 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -3776,7 +3784,7 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -3797,7 +3805,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B27">
         <v>8</v>
@@ -3818,7 +3826,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B28">
         <v>8</v>
@@ -3839,7 +3847,7 @@
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B29">
         <v>8</v>
@@ -3860,7 +3868,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -3881,7 +3889,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B31">
         <v>8</v>
@@ -3902,7 +3910,7 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -3923,7 +3931,7 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -3944,7 +3952,7 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B34">
         <v>8</v>
@@ -3965,7 +3973,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B35">
         <v>8</v>
@@ -3986,7 +3994,7 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B36">
         <v>8</v>
@@ -4007,7 +4015,7 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B37">
         <v>8</v>
@@ -4154,7 +4162,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -4175,7 +4183,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -4196,7 +4204,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -4227,7 +4235,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B47">
         <v>2</v>
@@ -4258,7 +4266,7 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B48">
         <v>2</v>
@@ -4279,7 +4287,7 @@
     </row>
     <row r="49" spans="1:8" s="41" customFormat="1">
       <c r="A49" s="41" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B49" s="41">
         <v>2</v>
@@ -4300,7 +4308,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="39" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B50" s="39">
         <v>4</v>
@@ -4321,7 +4329,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B51">
         <v>4</v>
@@ -4342,7 +4350,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B52">
         <v>4</v>
@@ -4363,7 +4371,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B53">
         <v>4</v>
@@ -4384,7 +4392,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B54">
         <v>4</v>
@@ -4405,7 +4413,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B55">
         <v>4</v>
@@ -4426,7 +4434,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B56">
         <v>4</v>
@@ -4447,7 +4455,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B57">
         <v>8</v>
@@ -4468,7 +4476,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B58">
         <v>8</v>
@@ -4489,7 +4497,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B59">
         <v>15</v>
@@ -4510,7 +4518,7 @@
     </row>
     <row r="60" spans="1:8" hidden="1">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -4531,7 +4539,7 @@
     </row>
     <row r="61" spans="1:8" hidden="1">
       <c r="A61" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -4543,7 +4551,7 @@
     </row>
     <row r="62" spans="1:8" hidden="1">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -4555,7 +4563,7 @@
     </row>
     <row r="63" spans="1:8" hidden="1">
       <c r="A63" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -4567,7 +4575,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -4588,7 +4596,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -4609,7 +4617,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -4640,7 +4648,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -4671,7 +4679,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B68">
         <v>2</v>
@@ -4702,7 +4710,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -4725,7 +4733,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B70">
         <v>4</v>
@@ -4748,7 +4756,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B71">
         <v>8</v>
@@ -4771,7 +4779,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B72">
         <v>8</v>
@@ -4794,7 +4802,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B73">
         <v>8</v>
@@ -4817,7 +4825,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B74">
         <v>8</v>
@@ -4840,7 +4848,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B75">
         <v>8</v>
@@ -4863,7 +4871,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B76">
         <v>8</v>
@@ -4886,7 +4894,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B77">
         <v>16</v>
@@ -4909,7 +4917,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B78">
         <v>16</v>
@@ -4932,7 +4940,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B79">
         <v>16</v>
@@ -4955,7 +4963,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B80">
         <v>16</v>
@@ -4978,7 +4986,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B81">
         <v>16</v>
@@ -5001,7 +5009,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B82">
         <v>16</v>
@@ -5024,7 +5032,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B83">
         <v>16</v>
@@ -5047,7 +5055,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -5067,7 +5075,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -5087,7 +5095,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -5107,7 +5115,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -5127,7 +5135,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -5147,7 +5155,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -5167,7 +5175,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -5187,7 +5195,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -5207,7 +5215,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -5227,7 +5235,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B93">
         <v>4</v>
@@ -5247,7 +5255,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B94">
         <v>4</v>
@@ -5267,7 +5275,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B95">
         <v>4</v>
@@ -5289,6 +5297,7 @@
       <c r="A98" s="1"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -5320,30 +5329,30 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="26" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:10" s="6" customFormat="1">
       <c r="A5" s="6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>120</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G5" s="11" t="s">
         <v>119</v>
@@ -5358,7 +5367,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5381,7 +5390,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5405,7 +5414,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5429,7 +5438,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -5455,7 +5464,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -5479,7 +5488,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -5503,7 +5512,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -5529,7 +5538,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -5553,7 +5562,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -5577,7 +5586,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -5757,7 +5766,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B23">
         <v>8</v>
@@ -5820,7 +5829,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="C27" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D27" s="2">
         <f>STDEV(D6:D25)</f>
@@ -5830,25 +5839,25 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="26" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B29" s="26"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C30" s="37" t="s">
         <v>122</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G30" s="11" t="s">
         <v>1</v>
@@ -5865,7 +5874,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -5891,7 +5900,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -5916,7 +5925,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -5941,7 +5950,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -5966,7 +5975,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -5995,7 +6004,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B36">
         <v>2</v>
@@ -6021,7 +6030,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -6047,7 +6056,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -6073,7 +6082,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -6103,7 +6112,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -6279,19 +6288,19 @@
     </row>
     <row r="48" spans="1:10">
       <c r="C48" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D48" s="2">
         <f>AVERAGE(D30:D47)</f>
         <v>356.83130192700003</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="C49" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D49" s="2">
         <f>STDEV(D31:D47)</f>
@@ -6308,7 +6317,7 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="26" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B52" s="26"/>
       <c r="D52" s="2"/>
@@ -6321,13 +6330,13 @@
         <v>121</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G53" s="11" t="s">
         <v>132</v>
@@ -6341,7 +6350,7 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -6367,7 +6376,7 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B55">
         <v>2</v>
@@ -6391,7 +6400,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -6417,7 +6426,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -6441,7 +6450,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B58">
         <v>2</v>
@@ -6467,7 +6476,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -6491,7 +6500,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B60">
         <v>8</v>
@@ -6517,7 +6526,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B61">
         <v>8</v>
@@ -6541,7 +6550,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B62">
         <v>8</v>
@@ -6565,7 +6574,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B63">
         <v>8</v>
@@ -6757,29 +6766,29 @@
     </row>
     <row r="74" spans="1:10">
       <c r="C74" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D74" s="2">
         <f>AVERAGE(D54:D73)</f>
         <v>117.073104536535</v>
       </c>
       <c r="E74" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H74" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I74" s="55">
         <f>AVERAGE(D54:D63,D65:D66,D68:D70,D73)</f>
         <v>53.003791779293749</v>
       </c>
       <c r="J74" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:10">
       <c r="C75" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D75" s="2">
         <f>STDEV(D54:D73)</f>
@@ -6813,15 +6822,15 @@
         <v>121</v>
       </c>
       <c r="C80" s="26" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -6849,7 +6858,7 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B83">
         <v>8</v>
@@ -6863,7 +6872,7 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B84">
         <v>16</v>
@@ -6877,7 +6886,7 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -6891,7 +6900,7 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B86">
         <v>2</v>
@@ -6905,7 +6914,7 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B87">
         <v>2</v>
@@ -6919,7 +6928,7 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B88">
         <v>2</v>
@@ -6933,7 +6942,7 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -6947,7 +6956,7 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -6961,7 +6970,7 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -6975,7 +6984,7 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -6989,7 +6998,7 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B93">
         <v>2</v>
@@ -7003,7 +7012,7 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -7021,7 +7030,7 @@
         <v>331.21428571428572</v>
       </c>
       <c r="E95" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -7034,6 +7043,7 @@
       <c r="H109" s="2"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId4"/>
@@ -7082,25 +7092,25 @@
     </row>
     <row r="5" spans="1:14" s="28" customFormat="1" ht="39" customHeight="1">
       <c r="A5" s="29" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D5" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>79</v>
-      </c>
       <c r="G5" s="29" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H5" s="29" t="s">
         <v>159</v>
@@ -7109,7 +7119,7 @@
         <v>158</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="K5" s="28" t="s">
         <v>138</v>
@@ -7129,7 +7139,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -7211,7 +7221,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -7432,7 +7442,7 @@
         <v>2</v>
       </c>
       <c r="N13" s="52" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="39">
@@ -7468,7 +7478,7 @@
         <v>2</v>
       </c>
       <c r="N14" s="52" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="39">
@@ -7504,7 +7514,7 @@
         <v>1</v>
       </c>
       <c r="N15" s="52" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="39">
@@ -7677,8 +7687,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="J106" sqref="J106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -7694,12 +7704,12 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -7715,16 +7725,16 @@
     </row>
     <row r="8" spans="1:10" s="58" customFormat="1" ht="39">
       <c r="A8" s="29" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C8" s="29" t="s">
         <v>143</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>106</v>
@@ -7733,13 +7743,13 @@
         <v>107</v>
       </c>
       <c r="G8" s="57" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H8" s="57" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I8" s="57" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J8" s="57" t="s">
         <v>110</v>
@@ -7907,7 +7917,7 @@
     </row>
     <row r="14" spans="1:10" s="58" customFormat="1">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B14">
         <v>8</v>
@@ -7939,7 +7949,7 @@
     </row>
     <row r="15" spans="1:10" s="58" customFormat="1">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B15">
         <v>8</v>
@@ -7971,7 +7981,7 @@
     </row>
     <row r="16" spans="1:10" s="58" customFormat="1">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B16">
         <v>8</v>
@@ -8003,7 +8013,7 @@
     </row>
     <row r="17" spans="1:10" s="58" customFormat="1">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B17">
         <v>8</v>
@@ -8035,7 +8045,7 @@
     </row>
     <row r="18" spans="1:10" s="58" customFormat="1">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -8067,7 +8077,7 @@
     </row>
     <row r="19" spans="1:10" s="58" customFormat="1">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B19">
         <v>8</v>
@@ -8112,7 +8122,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F20">
         <v>8</v>
@@ -8145,7 +8155,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F21">
         <v>8</v>
@@ -8178,7 +8188,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F22">
         <v>8</v>
@@ -8211,7 +8221,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F23">
         <v>8</v>
@@ -8244,7 +8254,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F24">
         <v>8</v>
@@ -8277,7 +8287,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F25">
         <v>8</v>
@@ -8310,7 +8320,7 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F26">
         <v>8</v>
@@ -8343,7 +8353,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="59" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -8376,7 +8386,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="59" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -8409,7 +8419,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="59" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -8442,7 +8452,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="59" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -8475,7 +8485,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="59" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -8508,7 +8518,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="59" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -9056,10 +9066,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="B73" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C73" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -9077,7 +9087,7 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="58" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B75" s="55">
         <f>J27</f>
@@ -9090,7 +9100,7 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B76" s="55">
         <f>AVERAGE(J20:J25)</f>
@@ -9103,7 +9113,7 @@
     </row>
     <row r="77" spans="1:3" ht="26">
       <c r="A77" s="52" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
       <c r="B77" s="55">
         <f>AVERAGE(J14:J19)</f>
@@ -9114,9 +9124,9 @@
         <v>22.308119143463191</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="26">
+    <row r="78" spans="1:3" ht="39">
       <c r="A78" s="52" t="s">
-        <v>103</v>
+        <v>18</v>
       </c>
       <c r="B78" s="55">
         <f>AVERAGE(J43:J46)</f>
@@ -9129,7 +9139,7 @@
     </row>
     <row r="79" spans="1:3" ht="39">
       <c r="A79" s="52" t="s">
-        <v>104</v>
+        <v>17</v>
       </c>
       <c r="B79" s="55">
         <f>AVERAGE(J34:J42)</f>
@@ -9141,7 +9151,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -9216,7 +9225,7 @@
         <v>155</v>
       </c>
       <c r="L5" s="54" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -9255,7 +9264,7 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -9366,7 +9375,7 @@
         <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -9405,7 +9414,7 @@
         <v>3</v>
       </c>
       <c r="L10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -9643,7 +9652,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -9684,10 +9692,10 @@
   <sheetData>
     <row r="3" spans="1:9">
       <c r="A3" s="10" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -9699,7 +9707,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
@@ -9723,12 +9731,12 @@
         <v>32</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
@@ -9745,7 +9753,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="18" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="20">
@@ -9762,7 +9770,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="18" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
@@ -9783,7 +9791,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="18" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B8" s="19">
         <v>2070.8984270000001</v>
@@ -9800,7 +9808,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="18" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B9" s="19">
         <v>1095.4940549999999</v>
@@ -9827,7 +9835,7 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="18" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="20"/>
@@ -9848,7 +9856,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="18" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
@@ -9869,7 +9877,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="22" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B12" s="23">
         <v>1583.1962410000001</v>
@@ -9897,7 +9905,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
first reviewer remarks incorporated (quick wins)
git-svn-id: file://localhost/tmp/svn2git/svn@2273 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/ccgrid10/performance/namd_runs.xlsx
+++ b/papers/ccgrid10/performance/namd_runs.xlsx
@@ -5297,7 +5297,6 @@
       <c r="A98" s="1"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -7670,7 +7669,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -7687,8 +7685,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="J106" sqref="J106"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -9151,6 +9149,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -9652,6 +9651,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -9905,6 +9905,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>